<commit_message>
update from LEBS (data prep 2016)
</commit_message>
<xml_diff>
--- a/data_prep/WB_Effort.xlsx
+++ b/data_prep/WB_Effort.xlsx
@@ -247,8 +247,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -279,27 +280,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="22"/>
-      </left>
-      <right style="thin">
-        <color indexed="22"/>
-      </right>
-      <top style="thin">
-        <color indexed="22"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="22"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -328,15 +314,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -344,6 +321,13 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -619,7 +603,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -630,8 +614,8 @@
   <dimension ref="A1:N288"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1:G1048576"/>
+      <pane ySplit="1" topLeftCell="A237" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M1" sqref="M1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,8 +632,8 @@
     <col min="10" max="10" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.85546875" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -689,10 +673,10 @@
       <c r="L1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="13" t="s">
         <v>47</v>
       </c>
     </row>
@@ -735,10 +719,10 @@
       <c r="L2" s="5">
         <v>0.42759283700655587</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="13">
         <v>41.780549999999998</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="13">
         <v>-83.347767000000005</v>
       </c>
     </row>
@@ -781,10 +765,10 @@
       <c r="L3" s="5">
         <v>0.47835417632651644</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="13">
         <v>41.780067000000003</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="13">
         <v>-83.249449999999996</v>
       </c>
     </row>
@@ -827,10 +811,10 @@
       <c r="L4" s="5">
         <v>0.49159381055880208</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="13">
         <v>41.881067000000002</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="13">
         <v>-83.249549999999999</v>
       </c>
     </row>
@@ -873,10 +857,10 @@
       <c r="L5" s="5">
         <v>0.47192437474536075</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="13">
         <v>41.679349999999999</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="13">
         <v>-83.149950000000004</v>
       </c>
     </row>
@@ -919,10 +903,10 @@
       <c r="L6" s="5">
         <v>0.47733659924079486</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="13">
         <v>41.780166999999999</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="13">
         <v>-83.14855</v>
       </c>
     </row>
@@ -965,10 +949,10 @@
       <c r="L7" s="5">
         <v>0.52149482168840922</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="13">
         <v>41.863430000000001</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="13">
         <v>-83.149050000000003</v>
       </c>
     </row>
@@ -1011,10 +995,10 @@
       <c r="L8" s="5">
         <v>0.50861287457363658</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="13">
         <v>41.980617000000002</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="13">
         <v>-83.116600000000005</v>
       </c>
     </row>
@@ -1057,10 +1041,10 @@
       <c r="L9" s="5">
         <v>0.46192957311971261</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="13">
         <v>41.679482999999998</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="13">
         <v>-83.049666999999999</v>
       </c>
     </row>
@@ -1103,10 +1087,10 @@
       <c r="L10" s="5">
         <v>0.44878118019790902</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="13">
         <v>41.781083000000002</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="13">
         <v>-83.047882999999999</v>
       </c>
     </row>
@@ -1149,10 +1133,10 @@
       <c r="L11" s="5">
         <v>0.52027109485797818</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="13">
         <v>41.867182999999997</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="13">
         <v>-83.051000000000002</v>
       </c>
     </row>
@@ -1195,10 +1179,10 @@
       <c r="L12" s="5">
         <v>0.52916993917831412</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="13">
         <v>41.980767</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="13">
         <v>-83.050066999999999</v>
       </c>
     </row>
@@ -1241,10 +1225,10 @@
       <c r="L13" s="5">
         <v>0.45607177990416026</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="13">
         <v>41.579932999999997</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="13">
         <v>-82.943217000000004</v>
       </c>
     </row>
@@ -1287,10 +1271,10 @@
       <c r="L14" s="5">
         <v>0.50345817522221004</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="13">
         <v>41.6798</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="13">
         <v>-82.950666999999996</v>
       </c>
     </row>
@@ -1333,10 +1317,10 @@
       <c r="L15" s="5">
         <v>0.47385765534552238</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="13">
         <v>41.779916999999998</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="13">
         <v>-82.949349999999995</v>
       </c>
     </row>
@@ -1379,10 +1363,10 @@
       <c r="L16" s="5">
         <v>0.51658520144320685</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="13">
         <v>41.867400000000004</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="13">
         <v>-82.951283000000004</v>
       </c>
     </row>
@@ -1425,10 +1409,10 @@
       <c r="L17" s="5">
         <v>0.48436377071722309</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="13">
         <v>41.672882999999999</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="13">
         <v>-82.851866999999999</v>
       </c>
     </row>
@@ -1471,10 +1455,10 @@
       <c r="L18" s="5">
         <v>0.49333218203870766</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="13">
         <v>41.780433000000002</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="13">
         <v>-82.849783000000002</v>
       </c>
     </row>
@@ -1517,10 +1501,10 @@
       <c r="L19" s="5">
         <v>0.48009421882876735</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="13">
         <v>41.868217000000001</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="13">
         <v>-82.848766999999995</v>
       </c>
     </row>
@@ -1563,10 +1547,10 @@
       <c r="L20" s="5">
         <v>0.46651251062203869</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="13">
         <v>41.980367000000001</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="13">
         <v>-82.849582999999996</v>
       </c>
     </row>
@@ -1609,10 +1593,10 @@
       <c r="L21" s="5">
         <v>0.46423252856658587</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="13">
         <v>41.580117000000001</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="13">
         <v>-82.747950000000003</v>
       </c>
     </row>
@@ -1655,10 +1639,10 @@
       <c r="L22" s="5">
         <v>0.51607444019366855</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="13">
         <v>41.680300000000003</v>
       </c>
-      <c r="N22">
+      <c r="N22" s="13">
         <v>-82.750467</v>
       </c>
     </row>
@@ -1701,10 +1685,10 @@
       <c r="L23" s="5">
         <v>0.61275189373731198</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="13">
         <v>41.779383000000003</v>
       </c>
-      <c r="N23">
+      <c r="N23" s="13">
         <v>-82.750183000000007</v>
       </c>
     </row>
@@ -1747,10 +1731,10 @@
       <c r="L24" s="5">
         <v>0.53221236617854006</v>
       </c>
-      <c r="M24">
+      <c r="M24" s="13">
         <v>41.866833</v>
       </c>
-      <c r="N24">
+      <c r="N24" s="13">
         <v>-82.749899999999997</v>
       </c>
     </row>
@@ -1793,10 +1777,10 @@
       <c r="L25" s="5">
         <v>0.47583025969117326</v>
       </c>
-      <c r="M25">
+      <c r="M25" s="13">
         <v>41.980083</v>
       </c>
-      <c r="N25">
+      <c r="N25" s="13">
         <v>-82.750200000000007</v>
       </c>
     </row>
@@ -1839,10 +1823,10 @@
       <c r="L26" s="5">
         <v>0.54718649221698989</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="13">
         <v>41.579500000000003</v>
       </c>
-      <c r="N26">
+      <c r="N26" s="13">
         <v>-82.64255</v>
       </c>
     </row>
@@ -1885,10 +1869,10 @@
       <c r="L27" s="5">
         <v>0.52095892106817565</v>
       </c>
-      <c r="M27">
+      <c r="M27" s="13">
         <v>41.679467000000002</v>
       </c>
-      <c r="N27">
+      <c r="N27" s="13">
         <v>-82.649167000000006</v>
       </c>
     </row>
@@ -1931,10 +1915,10 @@
       <c r="L28" s="5">
         <v>0.53953835825958141</v>
       </c>
-      <c r="M28">
+      <c r="M28" s="13">
         <v>41.881082999999997</v>
       </c>
-      <c r="N28">
+      <c r="N28" s="13">
         <v>-82.649732999999998</v>
       </c>
     </row>
@@ -1977,10 +1961,10 @@
       <c r="L29" s="5">
         <v>0.47007719437297657</v>
       </c>
-      <c r="M29">
+      <c r="M29" s="13">
         <v>41.9801</v>
       </c>
-      <c r="N29">
+      <c r="N29" s="13">
         <v>-82.649782999999999</v>
       </c>
     </row>
@@ -2023,10 +2007,10 @@
       <c r="L30" s="5">
         <v>0.47262451730256438</v>
       </c>
-      <c r="M30">
+      <c r="M30" s="13">
         <v>41.479416999999998</v>
       </c>
-      <c r="N30">
+      <c r="N30" s="13">
         <v>-82.550749999999994</v>
       </c>
     </row>
@@ -2069,10 +2053,10 @@
       <c r="L31" s="5">
         <v>0.50564126750361971</v>
       </c>
-      <c r="M31">
+      <c r="M31" s="13">
         <v>41.577367000000002</v>
       </c>
-      <c r="N31">
+      <c r="N31" s="13">
         <v>-82.551550000000006</v>
       </c>
     </row>
@@ -2115,10 +2099,10 @@
       <c r="L32" s="5">
         <v>0.49725799060280707</v>
       </c>
-      <c r="M32">
+      <c r="M32" s="13">
         <v>41.680382999999999</v>
       </c>
-      <c r="N32">
+      <c r="N32" s="13">
         <v>-82.549250000000001</v>
       </c>
     </row>
@@ -2161,10 +2145,10 @@
       <c r="L33" s="5">
         <v>0.50058737014612098</v>
       </c>
-      <c r="M33">
+      <c r="M33" s="13">
         <v>41.780633000000002</v>
       </c>
-      <c r="N33">
+      <c r="N33" s="13">
         <v>-82.550233000000006</v>
       </c>
     </row>
@@ -2207,10 +2191,10 @@
       <c r="L34" s="5">
         <v>0.51547105527438164</v>
       </c>
-      <c r="M34">
+      <c r="M34" s="13">
         <v>41.866399999999999</v>
       </c>
-      <c r="N34">
+      <c r="N34" s="13">
         <v>-82.532550000000001</v>
       </c>
     </row>
@@ -2253,10 +2237,10 @@
       <c r="L35" s="5">
         <v>0.52322508537456136</v>
       </c>
-      <c r="M35">
+      <c r="M35" s="13">
         <v>41.480016999999997</v>
       </c>
-      <c r="N35">
+      <c r="N35" s="13">
         <v>-82.449832999999998</v>
       </c>
     </row>
@@ -2299,10 +2283,10 @@
       <c r="L36" s="5">
         <v>0.65183531091519187</v>
       </c>
-      <c r="M36">
+      <c r="M36" s="13">
         <v>41.579282999999997</v>
       </c>
-      <c r="N36">
+      <c r="N36" s="13">
         <v>-82.450567000000007</v>
       </c>
     </row>
@@ -2345,10 +2329,10 @@
       <c r="L37" s="5">
         <v>0.53399952187267319</v>
       </c>
-      <c r="M37">
+      <c r="M37" s="13">
         <v>41.680100000000003</v>
       </c>
-      <c r="N37">
+      <c r="N37" s="13">
         <v>-82.450017000000003</v>
       </c>
     </row>
@@ -2391,10 +2375,10 @@
       <c r="L38" s="5">
         <v>0.520548168103939</v>
       </c>
-      <c r="M38">
+      <c r="M38" s="13">
         <v>41.779499999999999</v>
       </c>
-      <c r="N38">
+      <c r="N38" s="13">
         <v>-82.448817000000005</v>
       </c>
     </row>
@@ -2437,10 +2421,10 @@
       <c r="L39" s="5">
         <v>0.59313110668180724</v>
       </c>
-      <c r="M39">
+      <c r="M39" s="13">
         <v>41.480849999999997</v>
       </c>
-      <c r="N39">
+      <c r="N39" s="13">
         <v>-82.351016999999999</v>
       </c>
     </row>
@@ -2483,10 +2467,10 @@
       <c r="L40" s="5">
         <v>0.6330254505607793</v>
       </c>
-      <c r="M40">
+      <c r="M40" s="13">
         <v>41.579799999999999</v>
       </c>
-      <c r="N40">
+      <c r="N40" s="13">
         <v>-82.349867000000003</v>
       </c>
     </row>
@@ -2529,10 +2513,10 @@
       <c r="L41" s="5">
         <v>0.51374334097202901</v>
       </c>
-      <c r="M41">
+      <c r="M41" s="13">
         <v>41.679482999999998</v>
       </c>
-      <c r="N41">
+      <c r="N41" s="13">
         <v>-82.347733000000005</v>
       </c>
     </row>
@@ -2575,10 +2559,10 @@
       <c r="L42" s="5">
         <v>0.53159573953215633</v>
       </c>
-      <c r="M42">
+      <c r="M42" s="13">
         <v>41.480867000000003</v>
       </c>
-      <c r="N42">
+      <c r="N42" s="13">
         <v>-82.250900000000001</v>
       </c>
     </row>
@@ -2621,10 +2605,10 @@
       <c r="L43" s="5">
         <v>0.40665155167155803</v>
       </c>
-      <c r="M43">
+      <c r="M43" s="13">
         <v>41.763750000000002</v>
       </c>
-      <c r="N43">
+      <c r="N43" s="13">
         <v>-83.346149999999994</v>
       </c>
     </row>
@@ -2667,10 +2651,10 @@
       <c r="L44" s="5">
         <v>0.49402235268560929</v>
       </c>
-      <c r="M44">
+      <c r="M44" s="13">
         <v>41.763383330000003</v>
       </c>
-      <c r="N44">
+      <c r="N44" s="13">
         <v>-83.249866670000003</v>
       </c>
     </row>
@@ -2713,10 +2697,10 @@
       <c r="L45" s="5">
         <v>0.43527902044196753</v>
       </c>
-      <c r="M45">
+      <c r="M45" s="13">
         <v>41.863399999999999</v>
       </c>
-      <c r="N45">
+      <c r="N45" s="13">
         <v>-83.249933330000005</v>
       </c>
     </row>
@@ -2759,10 +2743,10 @@
       <c r="L46" s="5">
         <v>0.34419639358242476</v>
       </c>
-      <c r="M46">
+      <c r="M46" s="13">
         <v>41.663383330000002</v>
       </c>
-      <c r="N46">
+      <c r="N46" s="13">
         <v>-83.149799999999999</v>
       </c>
     </row>
@@ -2805,10 +2789,10 @@
       <c r="L47" s="5">
         <v>0.47790615118739344</v>
       </c>
-      <c r="M47">
+      <c r="M47" s="13">
         <v>41.763433329999998</v>
       </c>
-      <c r="N47">
+      <c r="N47" s="13">
         <v>-83.149866669999994</v>
       </c>
     </row>
@@ -2851,10 +2835,10 @@
       <c r="L48" s="5">
         <v>0.46303494928896383</v>
       </c>
-      <c r="M48">
+      <c r="M48" s="13">
         <v>41.863433329999999</v>
       </c>
-      <c r="N48">
+      <c r="N48" s="13">
         <v>-83.149950000000004</v>
       </c>
     </row>
@@ -2897,10 +2881,10 @@
       <c r="L49" s="5">
         <v>0.42892417393730176</v>
       </c>
-      <c r="M49">
+      <c r="M49" s="13">
         <v>41.963466670000003</v>
       </c>
-      <c r="N49">
+      <c r="N49" s="13">
         <v>-83.149883329999994</v>
       </c>
     </row>
@@ -2943,10 +2927,10 @@
       <c r="L50" s="5">
         <v>0.4157291360279437</v>
       </c>
-      <c r="M50">
+      <c r="M50" s="13">
         <v>41.663266669999999</v>
       </c>
-      <c r="N50">
+      <c r="N50" s="13">
         <v>-83.049666669999993</v>
       </c>
     </row>
@@ -2989,10 +2973,10 @@
       <c r="L51" s="5">
         <v>0.47307057038846262</v>
       </c>
-      <c r="M51">
+      <c r="M51" s="13">
         <v>41.761316669999999</v>
       </c>
-      <c r="N51">
+      <c r="N51" s="13">
         <v>-83.060016669999996</v>
       </c>
     </row>
@@ -3035,10 +3019,10 @@
       <c r="L52" s="5">
         <v>0.44952612450128365</v>
       </c>
-      <c r="M52">
+      <c r="M52" s="13">
         <v>41.868499999999997</v>
       </c>
-      <c r="N52">
+      <c r="N52" s="13">
         <v>-83.050933330000007</v>
       </c>
     </row>
@@ -3081,10 +3065,10 @@
       <c r="L53" s="5">
         <v>0.46862574996049355</v>
       </c>
-      <c r="M53">
+      <c r="M53" s="13">
         <v>41.963149999999999</v>
       </c>
-      <c r="N53">
+      <c r="N53" s="13">
         <v>-83.050666669999998</v>
       </c>
     </row>
@@ -3127,10 +3111,10 @@
       <c r="L54" s="5">
         <v>0.4236538982954815</v>
       </c>
-      <c r="M54">
+      <c r="M54" s="13">
         <v>41.563466669999997</v>
       </c>
-      <c r="N54">
+      <c r="N54" s="13">
         <v>-82.950916669999998</v>
       </c>
     </row>
@@ -3173,10 +3157,10 @@
       <c r="L55" s="5">
         <v>0.46909056277250505</v>
       </c>
-      <c r="M55">
+      <c r="M55" s="13">
         <v>41.66438333</v>
       </c>
-      <c r="N55">
+      <c r="N55" s="13">
         <v>-82.950699999999998</v>
       </c>
     </row>
@@ -3219,10 +3203,10 @@
       <c r="L56" s="5">
         <v>0.50821438315528666</v>
       </c>
-      <c r="M56">
+      <c r="M56" s="13">
         <v>41.762749999999997</v>
       </c>
-      <c r="N56">
+      <c r="N56" s="13">
         <v>-82.950383329999994</v>
       </c>
     </row>
@@ -3265,10 +3249,10 @@
       <c r="L57" s="5">
         <v>0.48947766224820166</v>
       </c>
-      <c r="M57">
+      <c r="M57" s="13">
         <v>41.863566669999997</v>
       </c>
-      <c r="N57">
+      <c r="N57" s="13">
         <v>-82.950183330000002</v>
       </c>
     </row>
@@ -3311,10 +3295,10 @@
       <c r="L58" s="5">
         <v>0.47197367777899274</v>
       </c>
-      <c r="M58">
+      <c r="M58" s="13">
         <v>41.6633</v>
       </c>
-      <c r="N58">
+      <c r="N58" s="13">
         <v>-82.850116670000006</v>
       </c>
     </row>
@@ -3357,10 +3341,10 @@
       <c r="L59" s="5">
         <v>0.47399564858406407</v>
       </c>
-      <c r="M59">
+      <c r="M59" s="13">
         <v>41.762916670000003</v>
       </c>
-      <c r="N59">
+      <c r="N59" s="13">
         <v>-82.849500000000006</v>
       </c>
     </row>
@@ -3403,10 +3387,10 @@
       <c r="L60" s="5">
         <v>0.24061843385443007</v>
       </c>
-      <c r="M60">
+      <c r="M60" s="13">
         <v>41.863250000000001</v>
       </c>
-      <c r="N60">
+      <c r="N60" s="13">
         <v>-82.850099999999998</v>
       </c>
     </row>
@@ -3449,10 +3433,10 @@
       <c r="L61" s="5">
         <v>0.486711701981626</v>
       </c>
-      <c r="M61">
+      <c r="M61" s="13">
         <v>41.963666670000002</v>
       </c>
-      <c r="N61">
+      <c r="N61" s="13">
         <v>-82.850300000000004</v>
       </c>
     </row>
@@ -3495,10 +3479,10 @@
       <c r="L62" s="5">
         <v>0.44882276004406152</v>
       </c>
-      <c r="M62">
+      <c r="M62" s="13">
         <v>41.563416670000002</v>
       </c>
-      <c r="N62">
+      <c r="N62" s="13">
         <v>-82.750516669999996</v>
       </c>
     </row>
@@ -3541,10 +3525,10 @@
       <c r="L63" s="5">
         <v>0.47974214019783751</v>
       </c>
-      <c r="M63">
+      <c r="M63" s="13">
         <v>41.663183330000003</v>
       </c>
-      <c r="N63">
+      <c r="N63" s="13">
         <v>-82.749966670000006</v>
       </c>
     </row>
@@ -3587,10 +3571,10 @@
       <c r="L64" s="5">
         <v>0.44821995830570832</v>
       </c>
-      <c r="M64">
+      <c r="M64" s="13">
         <v>41.763233329999998</v>
       </c>
-      <c r="N64">
+      <c r="N64" s="13">
         <v>-82.74978333</v>
       </c>
     </row>
@@ -3633,10 +3617,10 @@
       <c r="L65" s="5">
         <v>0.49067864879780804</v>
       </c>
-      <c r="M65">
+      <c r="M65" s="13">
         <v>41.863199999999999</v>
       </c>
-      <c r="N65">
+      <c r="N65" s="13">
         <v>-82.749849999999995</v>
       </c>
     </row>
@@ -3679,10 +3663,10 @@
       <c r="L66" s="5">
         <v>0.4929769198694936</v>
       </c>
-      <c r="M66">
+      <c r="M66" s="13">
         <v>41.963299999999997</v>
       </c>
-      <c r="N66">
+      <c r="N66" s="13">
         <v>-82.753100000000003</v>
       </c>
     </row>
@@ -3725,10 +3709,10 @@
       <c r="L67" s="5">
         <v>0.55021120978700544</v>
       </c>
-      <c r="M67">
+      <c r="M67" s="13">
         <v>41.563433330000002</v>
       </c>
-      <c r="N67">
+      <c r="N67" s="13">
         <v>-82.650716669999994</v>
       </c>
     </row>
@@ -3771,10 +3755,10 @@
       <c r="L68" s="5">
         <v>0.5404072358379306</v>
       </c>
-      <c r="M68">
+      <c r="M68" s="13">
         <v>41.663416669999997</v>
       </c>
-      <c r="N68">
+      <c r="N68" s="13">
         <v>-82.654666669999997</v>
       </c>
     </row>
@@ -3817,10 +3801,10 @@
       <c r="L69" s="5">
         <v>0.42574650101494876</v>
       </c>
-      <c r="M69">
+      <c r="M69" s="13">
         <v>41.863333330000003</v>
       </c>
-      <c r="N69">
+      <c r="N69" s="13">
         <v>-82.650066670000001</v>
       </c>
     </row>
@@ -3863,10 +3847,10 @@
       <c r="L70" s="5">
         <v>0.51114265991505414</v>
       </c>
-      <c r="M70">
+      <c r="M70" s="13">
         <v>41.963416670000001</v>
       </c>
-      <c r="N70">
+      <c r="N70" s="13">
         <v>-82.650016669999999</v>
       </c>
     </row>
@@ -3909,10 +3893,10 @@
       <c r="L71" s="5">
         <v>0.52142916217189106</v>
       </c>
-      <c r="M71">
+      <c r="M71" s="13">
         <v>41.463466670000003</v>
       </c>
-      <c r="N71">
+      <c r="N71" s="13">
         <v>-82.550250000000005</v>
       </c>
     </row>
@@ -3955,10 +3939,10 @@
       <c r="L72" s="5">
         <v>0.49444878704563</v>
       </c>
-      <c r="M72">
+      <c r="M72" s="13">
         <v>41.563316669999999</v>
       </c>
-      <c r="N72">
+      <c r="N72" s="13">
         <v>-82.550349999999995</v>
       </c>
     </row>
@@ -4001,10 +3985,10 @@
       <c r="L73" s="5">
         <v>0.51834394257342953</v>
       </c>
-      <c r="M73">
+      <c r="M73" s="13">
         <v>41.659816669999998</v>
       </c>
-      <c r="N73">
+      <c r="N73" s="13">
         <v>-82.54988333</v>
       </c>
     </row>
@@ -4047,10 +4031,10 @@
       <c r="L74" s="5">
         <v>0.50892440076665679</v>
       </c>
-      <c r="M74">
+      <c r="M74" s="13">
         <v>41.766316670000002</v>
       </c>
-      <c r="N74">
+      <c r="N74" s="13">
         <v>-82.550449999999998</v>
       </c>
     </row>
@@ -4093,10 +4077,10 @@
       <c r="L75" s="5">
         <v>0.50748540229622074</v>
       </c>
-      <c r="M75">
+      <c r="M75" s="13">
         <v>41.863500000000002</v>
       </c>
-      <c r="N75">
+      <c r="N75" s="13">
         <v>-82.550016670000005</v>
       </c>
     </row>
@@ -4139,10 +4123,10 @@
       <c r="L76" s="5">
         <v>0.53891142599048181</v>
       </c>
-      <c r="M76">
+      <c r="M76" s="13">
         <v>41.463333329999998</v>
       </c>
-      <c r="N76">
+      <c r="N76" s="13">
         <v>-82.447066669999998</v>
       </c>
     </row>
@@ -4185,10 +4169,10 @@
       <c r="L77" s="5">
         <v>0.56150591991466814</v>
       </c>
-      <c r="M77">
+      <c r="M77" s="13">
         <v>41.563916669999998</v>
       </c>
-      <c r="N77">
+      <c r="N77" s="13">
         <v>-82.452699999999993</v>
       </c>
     </row>
@@ -4231,10 +4215,10 @@
       <c r="L78" s="5">
         <v>0.51919553396762341</v>
       </c>
-      <c r="M78">
+      <c r="M78" s="13">
         <v>41.663350000000001</v>
       </c>
-      <c r="N78">
+      <c r="N78" s="13">
         <v>-82.453916669999998</v>
       </c>
     </row>
@@ -4277,10 +4261,10 @@
       <c r="L79" s="5">
         <v>0.5150067371827064</v>
       </c>
-      <c r="M79">
+      <c r="M79" s="13">
         <v>41.764749999999999</v>
       </c>
-      <c r="N79">
+      <c r="N79" s="13">
         <v>-82.449516669999994</v>
       </c>
     </row>
@@ -4323,10 +4307,10 @@
       <c r="L80" s="5">
         <v>0.48726630996837877</v>
       </c>
-      <c r="M80">
+      <c r="M80" s="13">
         <v>41.463333329999998</v>
       </c>
-      <c r="N80">
+      <c r="N80" s="13">
         <v>-82.346933329999999</v>
       </c>
     </row>
@@ -4369,10 +4353,10 @@
       <c r="L81" s="5">
         <v>0.53449326175326084</v>
       </c>
-      <c r="M81">
+      <c r="M81" s="13">
         <v>41.564483330000002</v>
       </c>
-      <c r="N81">
+      <c r="N81" s="13">
         <v>-82.351749999999996</v>
       </c>
     </row>
@@ -4415,10 +4399,10 @@
       <c r="L82" s="5">
         <v>0.54176197665435111</v>
       </c>
-      <c r="M82">
+      <c r="M82" s="13">
         <v>41.66545</v>
       </c>
-      <c r="N82">
+      <c r="N82" s="13">
         <v>-82.348699999999994</v>
       </c>
     </row>
@@ -4461,10 +4445,10 @@
       <c r="L83" s="5">
         <v>0.51212808978322744</v>
       </c>
-      <c r="M83">
+      <c r="M83" s="13">
         <v>41.462916669999998</v>
       </c>
-      <c r="N83">
+      <c r="N83" s="13">
         <v>-82.249116670000006</v>
       </c>
     </row>
@@ -4507,10 +4491,10 @@
       <c r="L84" s="5">
         <v>0.49734958876183893</v>
       </c>
-      <c r="M84">
+      <c r="M84" s="13">
         <v>41.763449999999999</v>
       </c>
-      <c r="N84">
+      <c r="N84" s="13">
         <v>-83.349233330000004</v>
       </c>
     </row>
@@ -4553,10 +4537,10 @@
       <c r="L85" s="5">
         <v>0.62102705061372798</v>
       </c>
-      <c r="M85">
+      <c r="M85" s="13">
         <v>41.763379999999998</v>
       </c>
-      <c r="N85">
+      <c r="N85" s="13">
         <v>-83.249870000000001</v>
       </c>
     </row>
@@ -4599,10 +4583,10 @@
       <c r="L86" s="5">
         <v>0.59905196381220294</v>
       </c>
-      <c r="M86">
+      <c r="M86" s="13">
         <v>41.863399999999999</v>
       </c>
-      <c r="N86">
+      <c r="N86" s="13">
         <v>-83.249930000000006</v>
       </c>
     </row>
@@ -4645,10 +4629,10 @@
       <c r="L87" s="5">
         <v>0.60453120730032273</v>
       </c>
-      <c r="M87">
+      <c r="M87" s="13">
         <v>41.663379999999997</v>
       </c>
-      <c r="N87">
+      <c r="N87" s="13">
         <v>-83.149799999999999</v>
       </c>
     </row>
@@ -4691,10 +4675,10 @@
       <c r="L88" s="5">
         <v>0.64507928528400849</v>
       </c>
-      <c r="M88">
+      <c r="M88" s="13">
         <v>41.76343</v>
       </c>
-      <c r="N88">
+      <c r="N88" s="13">
         <v>-83.149870000000007</v>
       </c>
     </row>
@@ -4737,10 +4721,10 @@
       <c r="L89" s="5">
         <v>0.59277530802606526</v>
       </c>
-      <c r="M89">
+      <c r="M89" s="13">
         <v>41.863430000000001</v>
       </c>
-      <c r="N89">
+      <c r="N89" s="13">
         <v>-83.149950000000004</v>
       </c>
     </row>
@@ -4783,10 +4767,10 @@
       <c r="L90" s="5">
         <v>0.55991000000000002</v>
       </c>
-      <c r="M90">
+      <c r="M90" s="13">
         <v>41.963470000000001</v>
       </c>
-      <c r="N90">
+      <c r="N90" s="13">
         <v>-83.149879999999996</v>
       </c>
     </row>
@@ -4829,10 +4813,10 @@
       <c r="L91" s="5">
         <v>0.61053461028887013</v>
       </c>
-      <c r="M91">
+      <c r="M91" s="13">
         <v>41.663269999999997</v>
       </c>
-      <c r="N91">
+      <c r="N91" s="13">
         <v>-83.049670000000006</v>
       </c>
     </row>
@@ -4875,10 +4859,10 @@
       <c r="L92" s="5">
         <v>0.64385116909712126</v>
       </c>
-      <c r="M92">
+      <c r="M92" s="13">
         <v>41.76343</v>
       </c>
-      <c r="N92">
+      <c r="N92" s="13">
         <v>-83.049899999999994</v>
       </c>
     </row>
@@ -4921,10 +4905,10 @@
       <c r="L93" s="5">
         <v>0.70759110716377471</v>
       </c>
-      <c r="M93">
+      <c r="M93" s="13">
         <v>41.868499999999997</v>
       </c>
-      <c r="N93">
+      <c r="N93" s="13">
         <v>-83.050929999999994</v>
       </c>
     </row>
@@ -4967,10 +4951,10 @@
       <c r="L94" s="5">
         <v>0.67228357592390164</v>
       </c>
-      <c r="M94">
+      <c r="M94" s="13">
         <v>41.963149999999999</v>
       </c>
-      <c r="N94">
+      <c r="N94" s="13">
         <v>-83.050669999999997</v>
       </c>
     </row>
@@ -5013,10 +4997,10 @@
       <c r="L95" s="5">
         <v>0.38047079775127157</v>
       </c>
-      <c r="M95">
+      <c r="M95" s="13">
         <v>41.563470000000002</v>
       </c>
-      <c r="N95">
+      <c r="N95" s="13">
         <v>-82.950919999999996</v>
       </c>
     </row>
@@ -5059,10 +5043,10 @@
       <c r="L96" s="5">
         <v>0.60073952020023225</v>
       </c>
-      <c r="M96">
+      <c r="M96" s="13">
         <v>41.664380000000001</v>
       </c>
-      <c r="N96">
+      <c r="N96" s="13">
         <v>-82.950699999999998</v>
       </c>
     </row>
@@ -5105,10 +5089,10 @@
       <c r="L97" s="5">
         <v>0.67567447496250277</v>
       </c>
-      <c r="M97">
+      <c r="M97" s="13">
         <v>41.762749999999997</v>
       </c>
-      <c r="N97">
+      <c r="N97" s="13">
         <v>-82.950379999999996</v>
       </c>
     </row>
@@ -5151,10 +5135,10 @@
       <c r="L98" s="5">
         <v>0.67134655564087153</v>
       </c>
-      <c r="M98">
+      <c r="M98" s="13">
         <v>41.863570000000003</v>
       </c>
-      <c r="N98">
+      <c r="N98" s="13">
         <v>-82.950180000000003</v>
       </c>
     </row>
@@ -5197,10 +5181,10 @@
       <c r="L99" s="5">
         <v>0.61460628095419212</v>
       </c>
-      <c r="M99">
+      <c r="M99" s="13">
         <v>41.6633</v>
       </c>
-      <c r="N99">
+      <c r="N99" s="13">
         <v>-82.850120000000004</v>
       </c>
     </row>
@@ -5243,10 +5227,10 @@
       <c r="L100" s="5">
         <v>0.66436328319957572</v>
       </c>
-      <c r="M100">
+      <c r="M100" s="13">
         <v>41.762920000000001</v>
       </c>
-      <c r="N100">
+      <c r="N100" s="13">
         <v>-82.849500000000006</v>
       </c>
     </row>
@@ -5289,10 +5273,10 @@
       <c r="L101" s="5">
         <v>0.64565541979786512</v>
       </c>
-      <c r="M101">
+      <c r="M101" s="13">
         <v>41.863250000000001</v>
       </c>
-      <c r="N101">
+      <c r="N101" s="13">
         <v>-82.850099999999998</v>
       </c>
     </row>
@@ -5335,10 +5319,10 @@
       <c r="L102" s="5">
         <v>0.68555597300154947</v>
       </c>
-      <c r="M102">
+      <c r="M102" s="13">
         <v>41.96367</v>
       </c>
-      <c r="N102">
+      <c r="N102" s="13">
         <v>-82.850300000000004</v>
       </c>
     </row>
@@ -5381,10 +5365,10 @@
       <c r="L103" s="5">
         <v>0.68096625847776315</v>
       </c>
-      <c r="M103">
+      <c r="M103" s="13">
         <v>41.563420000000001</v>
       </c>
-      <c r="N103">
+      <c r="N103" s="13">
         <v>-82.750519999999995</v>
       </c>
     </row>
@@ -5427,10 +5411,10 @@
       <c r="L104" s="5">
         <v>0.59837443423748571</v>
       </c>
-      <c r="M104">
+      <c r="M104" s="13">
         <v>41.663179999999997</v>
       </c>
-      <c r="N104">
+      <c r="N104" s="13">
         <v>-82.749970000000005</v>
       </c>
     </row>
@@ -5473,10 +5457,10 @@
       <c r="L105" s="5">
         <v>0.60717363173724803</v>
       </c>
-      <c r="M105">
+      <c r="M105" s="13">
         <v>41.76323</v>
       </c>
-      <c r="N105">
+      <c r="N105" s="13">
         <v>-82.749780000000001</v>
       </c>
     </row>
@@ -5519,10 +5503,10 @@
       <c r="L106" s="5">
         <v>0.60651754063087582</v>
       </c>
-      <c r="M106">
+      <c r="M106" s="13">
         <v>41.863199999999999</v>
       </c>
-      <c r="N106">
+      <c r="N106" s="13">
         <v>-82.749849999999995</v>
       </c>
     </row>
@@ -5565,10 +5549,10 @@
       <c r="L107" s="5">
         <v>0.67145904055057148</v>
       </c>
-      <c r="M107">
+      <c r="M107" s="13">
         <v>41.963299999999997</v>
       </c>
-      <c r="N107">
+      <c r="N107" s="13">
         <v>-82.753100000000003</v>
       </c>
     </row>
@@ -5611,10 +5595,10 @@
       <c r="L108" s="5">
         <v>0.68603801479023585</v>
       </c>
-      <c r="M108">
+      <c r="M108" s="13">
         <v>41.563429999999997</v>
       </c>
-      <c r="N108">
+      <c r="N108" s="13">
         <v>-82.650720000000007</v>
       </c>
     </row>
@@ -5657,10 +5641,10 @@
       <c r="L109" s="5">
         <v>0.70349680598767572</v>
       </c>
-      <c r="M109">
+      <c r="M109" s="13">
         <v>41.662316670000003</v>
       </c>
-      <c r="N109">
+      <c r="N109" s="13">
         <v>-82.64748333</v>
       </c>
     </row>
@@ -5703,10 +5687,10 @@
       <c r="L110" s="5">
         <v>0.64421766234339428</v>
       </c>
-      <c r="M110">
+      <c r="M110" s="13">
         <v>41.863683330000001</v>
       </c>
-      <c r="N110">
+      <c r="N110" s="13">
         <v>-82.647900000000007</v>
       </c>
     </row>
@@ -5749,10 +5733,10 @@
       <c r="L111" s="5">
         <v>0.68607002906065773</v>
       </c>
-      <c r="M111">
+      <c r="M111" s="13">
         <v>41.964066670000001</v>
       </c>
-      <c r="N111">
+      <c r="N111" s="13">
         <v>-82.650700000000001</v>
       </c>
     </row>
@@ -5795,10 +5779,10 @@
       <c r="L112" s="5">
         <v>0.61451206654001589</v>
       </c>
-      <c r="M112">
+      <c r="M112" s="13">
         <v>41.465449999999997</v>
       </c>
-      <c r="N112">
+      <c r="N112" s="13">
         <v>-82.549133330000004</v>
       </c>
     </row>
@@ -5841,10 +5825,10 @@
       <c r="L113" s="5">
         <v>0.70226000000000011</v>
       </c>
-      <c r="M113">
+      <c r="M113" s="13">
         <v>41.563749999999999</v>
       </c>
-      <c r="N113">
+      <c r="N113" s="13">
         <v>-82.548966669999999</v>
       </c>
     </row>
@@ -5887,10 +5871,10 @@
       <c r="L114" s="5">
         <v>0.69297210432653999</v>
       </c>
-      <c r="M114">
+      <c r="M114" s="13">
         <v>41.663366670000002</v>
       </c>
-      <c r="N114">
+      <c r="N114" s="13">
         <v>-82.548900000000003</v>
       </c>
     </row>
@@ -5933,10 +5917,10 @@
       <c r="L115" s="5">
         <v>0.62075000000000002</v>
       </c>
-      <c r="M115">
+      <c r="M115" s="13">
         <v>41.761816670000002</v>
       </c>
-      <c r="N115">
+      <c r="N115" s="13">
         <v>-82.552233330000007</v>
       </c>
     </row>
@@ -5979,10 +5963,10 @@
       <c r="L116" s="5">
         <v>0.69209020073061822</v>
       </c>
-      <c r="M116">
+      <c r="M116" s="13">
         <v>41.867350000000002</v>
       </c>
-      <c r="N116">
+      <c r="N116" s="13">
         <v>-82.518366670000006</v>
       </c>
     </row>
@@ -6025,10 +6009,10 @@
       <c r="L117" s="5">
         <v>0.71384789355768807</v>
       </c>
-      <c r="M117">
+      <c r="M117" s="13">
         <v>41.463549999999998</v>
       </c>
-      <c r="N117">
+      <c r="N117" s="13">
         <v>-82.451816669999999</v>
       </c>
     </row>
@@ -6071,10 +6055,10 @@
       <c r="L118" s="5">
         <v>0.71356334142941813</v>
       </c>
-      <c r="M118">
+      <c r="M118" s="13">
         <v>41.563049999999997</v>
       </c>
-      <c r="N118">
+      <c r="N118" s="13">
         <v>-82.450566670000001</v>
       </c>
     </row>
@@ -6117,10 +6101,10 @@
       <c r="L119" s="5">
         <v>0.74936845112265682</v>
       </c>
-      <c r="M119">
+      <c r="M119" s="13">
         <v>41.66481667</v>
       </c>
-      <c r="N119">
+      <c r="N119" s="13">
         <v>-82.449466670000007</v>
       </c>
     </row>
@@ -6163,10 +6147,10 @@
       <c r="L120" s="5">
         <v>0.72870432689766185</v>
       </c>
-      <c r="M120">
+      <c r="M120" s="13">
         <v>41.7637</v>
       </c>
-      <c r="N120">
+      <c r="N120" s="13">
         <v>-82.449383330000003</v>
       </c>
     </row>
@@ -6209,10 +6193,10 @@
       <c r="L121" s="5">
         <v>0.65890583043048512</v>
       </c>
-      <c r="M121">
+      <c r="M121" s="13">
         <v>41.463799999999999</v>
       </c>
-      <c r="N121">
+      <c r="N121" s="13">
         <v>-82.352249999999998</v>
       </c>
     </row>
@@ -6255,10 +6239,10 @@
       <c r="L122" s="5">
         <v>0.69099119719119972</v>
       </c>
-      <c r="M122">
+      <c r="M122" s="13">
         <v>41.564133329999997</v>
       </c>
-      <c r="N122">
+      <c r="N122" s="13">
         <v>-82.348283330000001</v>
       </c>
     </row>
@@ -6301,10 +6285,10 @@
       <c r="L123" s="5">
         <v>0.78898938108287486</v>
       </c>
-      <c r="M123">
+      <c r="M123" s="13">
         <v>41.66545</v>
       </c>
-      <c r="N123">
+      <c r="N123" s="13">
         <v>-82.348699999999994</v>
       </c>
     </row>
@@ -6347,10 +6331,10 @@
       <c r="L124" s="5">
         <v>0.57023002360326391</v>
       </c>
-      <c r="M124">
+      <c r="M124" s="13">
         <v>41.46553333</v>
       </c>
-      <c r="N124">
+      <c r="N124" s="13">
         <v>-82.249683329999996</v>
       </c>
     </row>
@@ -6393,10 +6377,10 @@
       <c r="L125" s="6">
         <v>0.53627232941579606</v>
       </c>
-      <c r="M125">
+      <c r="M125" s="13">
         <v>41.765283333299998</v>
       </c>
-      <c r="N125">
+      <c r="N125" s="13">
         <v>-83.3481833333</v>
       </c>
     </row>
@@ -6439,10 +6423,10 @@
       <c r="L126" s="6">
         <v>0.58282386190937518</v>
       </c>
-      <c r="M126">
+      <c r="M126" s="13">
         <v>41.763300000000001</v>
       </c>
-      <c r="N126">
+      <c r="N126" s="13">
         <v>-83.150933333300003</v>
       </c>
     </row>
@@ -6485,10 +6469,10 @@
       <c r="L127" s="6">
         <v>0.58027686699030445</v>
       </c>
-      <c r="M127">
+      <c r="M127" s="13">
         <v>41.863566666700002</v>
       </c>
-      <c r="N127">
+      <c r="N127" s="13">
         <v>-83.248999999999995</v>
       </c>
     </row>
@@ -6531,10 +6515,10 @@
       <c r="L128" s="6">
         <v>0.63302039835325752</v>
       </c>
-      <c r="M128">
+      <c r="M128" s="13">
         <v>41.680100000000003</v>
       </c>
-      <c r="N128">
+      <c r="N128" s="13">
         <v>-83.149516666699995</v>
       </c>
     </row>
@@ -6577,10 +6561,10 @@
       <c r="L129" s="6">
         <v>0.52778523101958319</v>
       </c>
-      <c r="M129">
+      <c r="M129" s="13">
         <v>41.763300000000001</v>
       </c>
-      <c r="N129">
+      <c r="N129" s="13">
         <v>-83.150933333300003</v>
       </c>
     </row>
@@ -6623,10 +6607,10 @@
       <c r="L130" s="6">
         <v>0.57682738019156576</v>
       </c>
-      <c r="M130">
+      <c r="M130" s="13">
         <v>41.864199999999997</v>
       </c>
-      <c r="N130">
+      <c r="N130" s="13">
         <v>-83.149950000000004</v>
       </c>
     </row>
@@ -6669,10 +6653,10 @@
       <c r="L131" s="6">
         <v>0.51609582731140768</v>
       </c>
-      <c r="M131">
+      <c r="M131" s="13">
         <v>41.971466666700003</v>
       </c>
-      <c r="N131">
+      <c r="N131" s="13">
         <v>-83.145750000000007</v>
       </c>
     </row>
@@ -6715,10 +6699,10 @@
       <c r="L132" s="6">
         <v>0.63302039835325752</v>
       </c>
-      <c r="M132">
+      <c r="M132" s="13">
         <v>41.680433333300002</v>
       </c>
-      <c r="N132">
+      <c r="N132" s="13">
         <v>-83.050749999999994</v>
       </c>
     </row>
@@ -6761,10 +6745,10 @@
       <c r="L133" s="6">
         <v>0.70908208531803041</v>
       </c>
-      <c r="M133">
+      <c r="M133" s="13">
         <v>41.7634333333</v>
       </c>
-      <c r="N133">
+      <c r="N133" s="13">
         <v>-83.049899999999994</v>
       </c>
     </row>
@@ -6807,10 +6791,10 @@
       <c r="L134" s="6">
         <v>0.58629250220060147</v>
       </c>
-      <c r="M134">
+      <c r="M134" s="13">
         <v>41.864166666700001</v>
       </c>
-      <c r="N134">
+      <c r="N134" s="13">
         <v>-83.049549999999996</v>
       </c>
     </row>
@@ -6853,10 +6837,10 @@
       <c r="L135" s="6">
         <v>0.60667641614375978</v>
       </c>
-      <c r="M135">
+      <c r="M135" s="13">
         <v>41.964016666699997</v>
       </c>
-      <c r="N135">
+      <c r="N135" s="13">
         <v>-83.048850000000002</v>
       </c>
     </row>
@@ -6899,10 +6883,10 @@
       <c r="L136" s="6">
         <v>0.50365366734909101</v>
       </c>
-      <c r="M136">
+      <c r="M136" s="13">
         <v>41.564149999999998</v>
       </c>
-      <c r="N136">
+      <c r="N136" s="13">
         <v>-82.950249999999997</v>
       </c>
     </row>
@@ -6945,10 +6929,10 @@
       <c r="L137" s="6">
         <v>0.61736469324083998</v>
       </c>
-      <c r="M137">
+      <c r="M137" s="13">
         <v>41.66395</v>
       </c>
-      <c r="N137">
+      <c r="N137" s="13">
         <v>-82.950483333333295</v>
       </c>
     </row>
@@ -6991,10 +6975,10 @@
       <c r="L138" s="6">
         <v>0.61106636681466042</v>
       </c>
-      <c r="M138">
+      <c r="M138" s="13">
         <v>41.763249999999999</v>
       </c>
-      <c r="N138">
+      <c r="N138" s="13">
         <v>-82.949516666700006</v>
       </c>
     </row>
@@ -7037,10 +7021,10 @@
       <c r="L139" s="6">
         <v>0.63693193573927154</v>
       </c>
-      <c r="M139">
+      <c r="M139" s="13">
         <v>41.867066666699998</v>
       </c>
-      <c r="N139">
+      <c r="N139" s="13">
         <v>-82.949783333300005</v>
       </c>
     </row>
@@ -7083,10 +7067,10 @@
       <c r="L140" s="6">
         <v>0.58865064290849622</v>
       </c>
-      <c r="M140">
+      <c r="M140" s="13">
         <v>41.668500000000002</v>
       </c>
-      <c r="N140">
+      <c r="N140" s="13">
         <v>-82.854483333299996</v>
       </c>
     </row>
@@ -7129,10 +7113,10 @@
       <c r="L141" s="6">
         <v>0.54910551529349239</v>
       </c>
-      <c r="M141">
+      <c r="M141" s="13">
         <v>41.763133333299997</v>
       </c>
-      <c r="N141">
+      <c r="N141" s="13">
         <v>-82.851699999999994</v>
       </c>
     </row>
@@ -7175,10 +7159,10 @@
       <c r="L142" s="6">
         <v>0.57002979593922998</v>
       </c>
-      <c r="M142">
+      <c r="M142" s="13">
         <v>41.864649999999997</v>
       </c>
-      <c r="N142">
+      <c r="N142" s="13">
         <v>-82.850250000000003</v>
       </c>
     </row>
@@ -7221,10 +7205,10 @@
       <c r="L143" s="6">
         <v>0.58234820095409079</v>
       </c>
-      <c r="M143">
+      <c r="M143" s="13">
         <v>41.964816666700003</v>
       </c>
-      <c r="N143">
+      <c r="N143" s="13">
         <v>-82.851633333300001</v>
       </c>
     </row>
@@ -7267,10 +7251,10 @@
       <c r="L144" s="6">
         <v>0.50322351915279739</v>
       </c>
-      <c r="M144">
+      <c r="M144" s="13">
         <v>41.56335</v>
       </c>
-      <c r="N144">
+      <c r="N144" s="13">
         <v>-82.749833333300003</v>
       </c>
     </row>
@@ -7313,10 +7297,10 @@
       <c r="L145" s="6">
         <v>0.62123104710157206</v>
       </c>
-      <c r="M145">
+      <c r="M145" s="13">
         <v>41.6636833333</v>
       </c>
-      <c r="N145">
+      <c r="N145" s="13">
         <v>-82.749616666700007</v>
       </c>
     </row>
@@ -7359,10 +7343,10 @@
       <c r="L146" s="6">
         <v>0.57575789487948059</v>
       </c>
-      <c r="M146">
+      <c r="M146" s="13">
         <v>41.763849999999998</v>
       </c>
-      <c r="N146">
+      <c r="N146" s="13">
         <v>-82.749966666700004</v>
       </c>
     </row>
@@ -7405,10 +7389,10 @@
       <c r="L147" s="6">
         <v>0.77355074910964505</v>
       </c>
-      <c r="M147">
+      <c r="M147" s="13">
         <v>41.865166666699999</v>
       </c>
-      <c r="N147">
+      <c r="N147" s="13">
         <v>-82.750666666699999</v>
       </c>
     </row>
@@ -7451,10 +7435,10 @@
       <c r="L148" s="6">
         <v>0.60165415033207326</v>
       </c>
-      <c r="M148">
+      <c r="M148" s="13">
         <v>41.9638666667</v>
       </c>
-      <c r="N148">
+      <c r="N148" s="13">
         <v>-82.748666666700004</v>
       </c>
     </row>
@@ -7497,10 +7481,10 @@
       <c r="L149" s="6">
         <v>0.65911138893688814</v>
       </c>
-      <c r="M149">
+      <c r="M149" s="13">
         <v>41.564100000000003</v>
       </c>
-      <c r="N149">
+      <c r="N149" s="13">
         <v>-82.650149999999996</v>
       </c>
     </row>
@@ -7543,10 +7527,10 @@
       <c r="L150" s="6">
         <v>0.7179910368492457</v>
       </c>
-      <c r="M150">
+      <c r="M150" s="13">
         <v>41.664149999999999</v>
       </c>
-      <c r="N150">
+      <c r="N150" s="13">
         <v>-82.650433333300001</v>
       </c>
     </row>
@@ -7589,10 +7573,10 @@
       <c r="L151" s="6">
         <v>0.67903223234635024</v>
       </c>
-      <c r="M151">
+      <c r="M151" s="13">
         <v>41.862716666700003</v>
       </c>
-      <c r="N151">
+      <c r="N151" s="13">
         <v>-82.648083333299994</v>
       </c>
     </row>
@@ -7635,10 +7619,10 @@
       <c r="L152" s="6">
         <v>0.59221839255200026</v>
       </c>
-      <c r="M152">
+      <c r="M152" s="13">
         <v>41.964266666699999</v>
       </c>
-      <c r="N152">
+      <c r="N152" s="13">
         <v>-82.649533333299999</v>
       </c>
     </row>
@@ -7681,10 +7665,10 @@
       <c r="L153" s="6">
         <v>0.62958488178832617</v>
       </c>
-      <c r="M153">
+      <c r="M153" s="13">
         <v>41.458416666700003</v>
       </c>
-      <c r="N153">
+      <c r="N153" s="13">
         <v>-82.546000000000006</v>
       </c>
     </row>
@@ -7727,10 +7711,10 @@
       <c r="L154" s="6">
         <v>0.64155119791544846</v>
       </c>
-      <c r="M154">
+      <c r="M154" s="13">
         <v>41.564483333333335</v>
       </c>
-      <c r="N154">
+      <c r="N154" s="13">
         <v>-82.550216666666699</v>
       </c>
     </row>
@@ -7773,10 +7757,10 @@
       <c r="L155" s="6">
         <v>0.71590313350532775</v>
       </c>
-      <c r="M155">
+      <c r="M155" s="13">
         <v>41.663666666700003</v>
       </c>
-      <c r="N155">
+      <c r="N155" s="13">
         <v>-82.549666666700006</v>
       </c>
     </row>
@@ -7819,10 +7803,10 @@
       <c r="L156" s="6">
         <v>0.65629507896807771</v>
       </c>
-      <c r="M156">
+      <c r="M156" s="13">
         <v>41.761949999999999</v>
       </c>
-      <c r="N156">
+      <c r="N156" s="13">
         <v>-82.550299999999993</v>
       </c>
     </row>
@@ -7865,10 +7849,10 @@
       <c r="L157" s="6">
         <v>0.63634038103536561</v>
       </c>
-      <c r="M157">
+      <c r="M157" s="13">
         <v>41.862883333299997</v>
       </c>
-      <c r="N157">
+      <c r="N157" s="13">
         <v>-82.548833333299996</v>
       </c>
     </row>
@@ -7911,10 +7895,10 @@
       <c r="L158" s="6">
         <v>0.62556373067306748</v>
       </c>
-      <c r="M158">
+      <c r="M158" s="13">
         <v>41.4636</v>
       </c>
-      <c r="N158">
+      <c r="N158" s="13">
         <v>-82.449700000000007</v>
       </c>
     </row>
@@ -7957,10 +7941,10 @@
       <c r="L159" s="6">
         <v>0.65326482594047519</v>
       </c>
-      <c r="M159">
+      <c r="M159" s="13">
         <v>41.563633333299997</v>
       </c>
-      <c r="N159">
+      <c r="N159" s="13">
         <v>-82.450066666699996</v>
       </c>
     </row>
@@ -8003,10 +7987,10 @@
       <c r="L160" s="6">
         <v>0.62371911656983692</v>
       </c>
-      <c r="M160">
+      <c r="M160" s="13">
         <v>41.663699999999999</v>
       </c>
-      <c r="N160">
+      <c r="N160" s="13">
         <v>-82.45</v>
       </c>
     </row>
@@ -8049,10 +8033,10 @@
       <c r="L161" s="6">
         <v>0.61194040465231814</v>
       </c>
-      <c r="M161">
+      <c r="M161" s="13">
         <v>41.763350000000003</v>
       </c>
-      <c r="N161">
+      <c r="N161" s="13">
         <v>-82.447433333299998</v>
       </c>
     </row>
@@ -8095,10 +8079,10 @@
       <c r="L162" s="6">
         <v>0.65897205424039818</v>
       </c>
-      <c r="M162">
+      <c r="M162" s="13">
         <v>41.463833333300002</v>
       </c>
-      <c r="N162">
+      <c r="N162" s="13">
         <v>-82.349666666700003</v>
       </c>
     </row>
@@ -8141,10 +8125,10 @@
       <c r="L163" s="6">
         <v>0.73248020476843945</v>
       </c>
-      <c r="M163">
+      <c r="M163" s="13">
         <v>41.563299999999998</v>
       </c>
-      <c r="N163">
+      <c r="N163" s="13">
         <v>-82.352099999999993</v>
       </c>
     </row>
@@ -8187,10 +8171,10 @@
       <c r="L164" s="6">
         <v>0.69245375035463375</v>
       </c>
-      <c r="M164">
+      <c r="M164" s="13">
         <v>41.66375</v>
       </c>
-      <c r="N164">
+      <c r="N164" s="13">
         <v>-82.350700000000003</v>
       </c>
     </row>
@@ -8233,10 +8217,10 @@
       <c r="L165" s="6">
         <v>0.60882440121479198</v>
       </c>
-      <c r="M165">
+      <c r="M165" s="13">
         <v>41.464100000000002</v>
       </c>
-      <c r="N165">
+      <c r="N165" s="13">
         <v>-82.2511166667</v>
       </c>
     </row>
@@ -8279,10 +8263,10 @@
       <c r="L166" s="5">
         <v>0.76791993741240283</v>
       </c>
-      <c r="M166">
+      <c r="M166" s="13">
         <v>41.782096666666668</v>
       </c>
-      <c r="N166">
+      <c r="N166" s="13">
         <v>-83.346805000000003</v>
       </c>
     </row>
@@ -8325,10 +8309,10 @@
       <c r="L167" s="5">
         <v>0.73108296493094804</v>
       </c>
-      <c r="M167">
+      <c r="M167" s="13">
         <v>41.780005000000003</v>
       </c>
-      <c r="N167">
+      <c r="N167" s="13">
         <v>-83.250766666666664</v>
       </c>
     </row>
@@ -8371,10 +8355,10 @@
       <c r="L168" s="5">
         <v>0.76822074255089645</v>
       </c>
-      <c r="M168">
+      <c r="M168" s="13">
         <v>41.880015</v>
       </c>
-      <c r="N168">
+      <c r="N168" s="13">
         <v>-83.251293333333336</v>
       </c>
     </row>
@@ -8417,10 +8401,10 @@
       <c r="L169" s="5">
         <v>0.86660510111128952</v>
       </c>
-      <c r="M169">
+      <c r="M169" s="13">
         <v>41.699516666666668</v>
       </c>
-      <c r="N169">
+      <c r="N169" s="13">
         <v>-83.056703333333331</v>
       </c>
     </row>
@@ -8463,10 +8447,10 @@
       <c r="L170" s="5">
         <v>0.71298551240683172</v>
       </c>
-      <c r="M170">
+      <c r="M170" s="13">
         <v>41.779969999999999</v>
       </c>
-      <c r="N170">
+      <c r="N170" s="13">
         <v>-83.151103333333339</v>
       </c>
     </row>
@@ -8509,10 +8493,10 @@
       <c r="L171" s="5">
         <v>0.79824072083378672</v>
       </c>
-      <c r="M171">
+      <c r="M171" s="13">
         <v>41.879006666666669</v>
       </c>
-      <c r="N171">
+      <c r="N171" s="13">
         <v>-83.150631666666669</v>
       </c>
     </row>
@@ -8555,10 +8539,10 @@
       <c r="L172" s="5">
         <v>0.7343301057130468</v>
       </c>
-      <c r="M172">
+      <c r="M172" s="13">
         <v>41.979826666666668</v>
       </c>
-      <c r="N172">
+      <c r="N172" s="13">
         <v>-83.115136666666672</v>
       </c>
     </row>
@@ -8601,10 +8585,10 @@
       <c r="L173" s="5">
         <v>0.73005997679352053</v>
       </c>
-      <c r="M173">
+      <c r="M173" s="13">
         <v>41.680973333333334</v>
       </c>
-      <c r="N173">
+      <c r="N173" s="13">
         <v>-83.052424999999999</v>
       </c>
     </row>
@@ -8647,10 +8631,10 @@
       <c r="L174" s="5">
         <v>0.73556769199915761</v>
       </c>
-      <c r="M174">
+      <c r="M174" s="13">
         <v>41.77124666666667</v>
       </c>
-      <c r="N174">
+      <c r="N174" s="13">
         <v>-83.025885000000002</v>
       </c>
     </row>
@@ -8693,10 +8677,10 @@
       <c r="L175" s="5">
         <v>0.75836376302411246</v>
       </c>
-      <c r="M175">
+      <c r="M175" s="13">
         <v>41.880495000000003</v>
       </c>
-      <c r="N175">
+      <c r="N175" s="13">
         <v>-83.049525000000003</v>
       </c>
     </row>
@@ -8739,10 +8723,10 @@
       <c r="L176" s="5">
         <v>0.75113389812588005</v>
       </c>
-      <c r="M176">
+      <c r="M176" s="13">
         <v>41.979711666666667</v>
       </c>
-      <c r="N176">
+      <c r="N176" s="13">
         <v>-83.049806666666669</v>
       </c>
     </row>
@@ -8785,10 +8769,10 @@
       <c r="L177" s="5">
         <v>0.84774038697019138</v>
       </c>
-      <c r="M177">
+      <c r="M177" s="13">
         <v>41.581563333333335</v>
       </c>
-      <c r="N177">
+      <c r="N177" s="13">
         <v>-82.947753333333338</v>
       </c>
     </row>
@@ -8831,10 +8815,10 @@
       <c r="L178" s="5">
         <v>0.80254183202277563</v>
       </c>
-      <c r="M178">
+      <c r="M178" s="13">
         <v>41.684338333333336</v>
       </c>
-      <c r="N178">
+      <c r="N178" s="13">
         <v>-82.952056666666664</v>
       </c>
     </row>
@@ -8877,10 +8861,10 @@
       <c r="L179" s="5">
         <v>0.80166015902387822</v>
       </c>
-      <c r="M179">
+      <c r="M179" s="13">
         <v>41.762965000000001</v>
       </c>
-      <c r="N179">
+      <c r="N179" s="13">
         <v>-82.949583333333337</v>
       </c>
     </row>
@@ -8923,10 +8907,10 @@
       <c r="L180" s="5">
         <v>0.75539828195566883</v>
       </c>
-      <c r="M180">
+      <c r="M180" s="13">
         <v>41.879559999999998</v>
       </c>
-      <c r="N180">
+      <c r="N180" s="13">
         <v>-82.949924999999993</v>
       </c>
     </row>
@@ -8969,10 +8953,10 @@
       <c r="L181" s="5">
         <v>0.76352035364471771</v>
       </c>
-      <c r="M181">
+      <c r="M181" s="13">
         <v>41.673313333333333</v>
       </c>
-      <c r="N181">
+      <c r="N181" s="13">
         <v>-82.849699999999999</v>
       </c>
     </row>
@@ -9015,10 +8999,10 @@
       <c r="L182" s="5">
         <v>0.74695260861996238</v>
       </c>
-      <c r="M182">
+      <c r="M182" s="13">
         <v>41.763330000000003</v>
       </c>
-      <c r="N182">
+      <c r="N182" s="13">
         <v>-82.850219999999993</v>
       </c>
     </row>
@@ -9061,10 +9045,10 @@
       <c r="L183" s="5">
         <v>0.71360770331318424</v>
       </c>
-      <c r="M183">
+      <c r="M183" s="13">
         <v>41.86345166666667</v>
       </c>
-      <c r="N183">
+      <c r="N183" s="13">
         <v>-82.850250000000003</v>
       </c>
     </row>
@@ -9107,10 +9091,10 @@
       <c r="L184" s="5">
         <v>0.73764145534447279</v>
       </c>
-      <c r="M184">
+      <c r="M184" s="13">
         <v>41.962758333333333</v>
       </c>
-      <c r="N184">
+      <c r="N184" s="13">
         <v>-82.850553333333337</v>
       </c>
     </row>
@@ -9153,10 +9137,10 @@
       <c r="L185" s="5">
         <v>0.85467536150295309</v>
       </c>
-      <c r="M185">
+      <c r="M185" s="13">
         <v>41.580773333333333</v>
       </c>
-      <c r="N185">
+      <c r="N185" s="13">
         <v>-82.747865000000004</v>
       </c>
     </row>
@@ -9199,10 +9183,10 @@
       <c r="L186" s="5">
         <v>0.74369312435553481</v>
       </c>
-      <c r="M186">
+      <c r="M186" s="13">
         <v>41.680284999999998</v>
       </c>
-      <c r="N186">
+      <c r="N186" s="13">
         <v>-82.750311666666661</v>
       </c>
     </row>
@@ -9245,10 +9229,10 @@
       <c r="L187" s="5">
         <v>0.6964496283610675</v>
       </c>
-      <c r="M187">
+      <c r="M187" s="13">
         <v>41.771756666666668</v>
       </c>
-      <c r="N187">
+      <c r="N187" s="13">
         <v>-82.751530000000002</v>
       </c>
     </row>
@@ -9291,10 +9275,10 @@
       <c r="L188" s="5">
         <v>0.75953084274452121</v>
       </c>
-      <c r="M188">
+      <c r="M188" s="13">
         <v>41.868448333333333</v>
       </c>
-      <c r="N188">
+      <c r="N188" s="13">
         <v>-82.750631666666663</v>
       </c>
     </row>
@@ -9337,10 +9321,10 @@
       <c r="L189" s="5">
         <v>0.7338326764618528</v>
       </c>
-      <c r="M189">
+      <c r="M189" s="13">
         <v>41.9636</v>
       </c>
-      <c r="N189">
+      <c r="N189" s="13">
         <v>-82.750093333333339</v>
       </c>
     </row>
@@ -9383,10 +9367,10 @@
       <c r="L190" s="5">
         <v>0.82989332791297588</v>
       </c>
-      <c r="M190">
+      <c r="M190" s="13">
         <v>41.580134999999999</v>
       </c>
-      <c r="N190">
+      <c r="N190" s="13">
         <v>-82.648619999999994</v>
       </c>
     </row>
@@ -9429,10 +9413,10 @@
       <c r="L191" s="5">
         <v>0.75803484923505349</v>
       </c>
-      <c r="M191">
+      <c r="M191" s="13">
         <v>41.662495</v>
       </c>
-      <c r="N191">
+      <c r="N191" s="13">
         <v>-82.647398333333328</v>
       </c>
     </row>
@@ -9475,10 +9459,10 @@
       <c r="L192" s="5">
         <v>0.64748603379052683</v>
       </c>
-      <c r="M192">
+      <c r="M192" s="13">
         <v>41.863681666666665</v>
       </c>
-      <c r="N192">
+      <c r="N192" s="13">
         <v>-82.650913333333335</v>
       </c>
     </row>
@@ -9521,10 +9505,10 @@
       <c r="L193" s="5">
         <v>0.68600725120260364</v>
       </c>
-      <c r="M193">
+      <c r="M193" s="13">
         <v>41.972034999999998</v>
       </c>
-      <c r="N193">
+      <c r="N193" s="13">
         <v>-82.65094666666667</v>
       </c>
     </row>
@@ -9567,10 +9551,10 @@
       <c r="L194" s="5">
         <v>0.88376532906890815</v>
       </c>
-      <c r="M194">
+      <c r="M194" s="13">
         <v>41.481563333333334</v>
       </c>
-      <c r="N194">
+      <c r="N194" s="13">
         <v>-82.549956666666674</v>
       </c>
     </row>
@@ -9613,10 +9597,10 @@
       <c r="L195" s="5">
         <v>0.87940347770151206</v>
       </c>
-      <c r="M195">
+      <c r="M195" s="13">
         <v>41.581296666666667</v>
       </c>
-      <c r="N195">
+      <c r="N195" s="13">
         <v>-82.550510000000003</v>
       </c>
     </row>
@@ -9659,10 +9643,10 @@
       <c r="L196" s="5">
         <v>0.71769479864435037</v>
       </c>
-      <c r="M196">
+      <c r="M196" s="13">
         <v>41.663183333333336</v>
       </c>
-      <c r="N196">
+      <c r="N196" s="13">
         <v>-82.548733333333331</v>
       </c>
     </row>
@@ -9705,10 +9689,10 @@
       <c r="L197" s="5">
         <v>0.68125984736593692</v>
       </c>
-      <c r="M197">
+      <c r="M197" s="13">
         <v>41.780160000000002</v>
       </c>
-      <c r="N197">
+      <c r="N197" s="13">
         <v>-82.550314999999998</v>
       </c>
     </row>
@@ -9751,10 +9735,10 @@
       <c r="L198" s="5">
         <v>0.69215502620444502</v>
       </c>
-      <c r="M198">
+      <c r="M198" s="13">
         <v>41.867066666666666</v>
       </c>
-      <c r="N198">
+      <c r="N198" s="13">
         <v>-82.533821666666668</v>
       </c>
     </row>
@@ -9797,10 +9781,10 @@
       <c r="L199" s="5">
         <v>0.68308052714420764</v>
       </c>
-      <c r="M199">
+      <c r="M199" s="13">
         <v>41.480358333333335</v>
       </c>
-      <c r="N199">
+      <c r="N199" s="13">
         <v>-82.449386666666669</v>
       </c>
     </row>
@@ -9843,10 +9827,10 @@
       <c r="L200" s="5">
         <v>0.81106341702955831</v>
       </c>
-      <c r="M200">
+      <c r="M200" s="13">
         <v>41.579990000000002</v>
       </c>
-      <c r="N200">
+      <c r="N200" s="13">
         <v>-82.449903333333339</v>
       </c>
     </row>
@@ -9889,10 +9873,10 @@
       <c r="L201" s="5">
         <v>0.76917723036944996</v>
       </c>
-      <c r="M201">
+      <c r="M201" s="13">
         <v>41.663306666666664</v>
       </c>
-      <c r="N201">
+      <c r="N201" s="13">
         <v>-82.450181666666666</v>
       </c>
     </row>
@@ -9935,10 +9919,10 @@
       <c r="L202" s="5">
         <v>0.7799078013088323</v>
       </c>
-      <c r="M202">
+      <c r="M202" s="13">
         <v>41.780259999999998</v>
       </c>
-      <c r="N202">
+      <c r="N202" s="13">
         <v>-82.449596666666665</v>
       </c>
     </row>
@@ -9981,10 +9965,10 @@
       <c r="L203" s="5">
         <v>0.76663410058512171</v>
       </c>
-      <c r="M203">
+      <c r="M203" s="13">
         <v>41.478568333333335</v>
       </c>
-      <c r="N203">
+      <c r="N203" s="13">
         <v>-82.349716666666666</v>
       </c>
     </row>
@@ -10027,10 +10011,10 @@
       <c r="L204" s="5">
         <v>0.80397368333118291</v>
       </c>
-      <c r="M204">
+      <c r="M204" s="13">
         <v>41.579943333333333</v>
       </c>
-      <c r="N204">
+      <c r="N204" s="13">
         <v>-82.349941666666666</v>
       </c>
     </row>
@@ -10073,10 +10057,10 @@
       <c r="L205" s="5">
         <v>0.7911390857880255</v>
       </c>
-      <c r="M205">
+      <c r="M205" s="13">
         <v>41.663148333333332</v>
       </c>
-      <c r="N205">
+      <c r="N205" s="13">
         <v>-82.348444999999998</v>
       </c>
     </row>
@@ -10119,10 +10103,10 @@
       <c r="L206" s="5">
         <v>0.72246178489116331</v>
       </c>
-      <c r="M206">
+      <c r="M206" s="13">
         <v>41.463318333333333</v>
       </c>
-      <c r="N206">
+      <c r="N206" s="13">
         <v>-82.249840000000006</v>
       </c>
     </row>
@@ -10165,10 +10149,10 @@
       <c r="L207" s="5">
         <v>0.54314763640551444</v>
       </c>
-      <c r="M207">
+      <c r="M207" s="13">
         <v>41.780496666666664</v>
       </c>
-      <c r="N207">
+      <c r="N207" s="13">
         <v>-83.349836666666661</v>
       </c>
     </row>
@@ -10211,10 +10195,10 @@
       <c r="L208" s="5">
         <v>0.70337501828027016</v>
       </c>
-      <c r="M208">
+      <c r="M208" s="13">
         <v>41.780200000000001</v>
       </c>
-      <c r="N208">
+      <c r="N208" s="13">
         <v>-83.250029999999995</v>
       </c>
     </row>
@@ -10257,10 +10241,10 @@
       <c r="L209" s="5">
         <v>0.67500286218232475</v>
       </c>
-      <c r="M209">
+      <c r="M209" s="13">
         <v>41.880015</v>
       </c>
-      <c r="N209">
+      <c r="N209" s="13">
         <v>-83.249663333333331</v>
       </c>
     </row>
@@ -10303,10 +10287,10 @@
       <c r="L210" s="5">
         <v>0.65295548071035225</v>
       </c>
-      <c r="M210">
+      <c r="M210" s="13">
         <v>41.680148333333335</v>
       </c>
-      <c r="N210">
+      <c r="N210" s="13">
         <v>-83.149141666666665</v>
       </c>
     </row>
@@ -10349,10 +10333,10 @@
       <c r="L211" s="5">
         <v>0.68992915808149025</v>
       </c>
-      <c r="M211">
+      <c r="M211" s="13">
         <v>41.780061666666668</v>
       </c>
-      <c r="N211">
+      <c r="N211" s="13">
         <v>-83.15041166666667</v>
       </c>
     </row>
@@ -10395,10 +10379,10 @@
       <c r="L212" s="5">
         <v>0.65173710867989243</v>
       </c>
-      <c r="M212">
+      <c r="M212" s="13">
         <v>41.880299999999998</v>
       </c>
-      <c r="N212">
+      <c r="N212" s="13">
         <v>-83.149749999999997</v>
       </c>
     </row>
@@ -10441,10 +10425,10 @@
       <c r="L213" s="5">
         <v>0.70699999999999996</v>
       </c>
-      <c r="M213">
+      <c r="M213" s="13">
         <v>41.967619999999997</v>
       </c>
-      <c r="N213">
+      <c r="N213" s="13">
         <v>-83.107991666666663</v>
       </c>
     </row>
@@ -10487,10 +10471,10 @@
       <c r="L214" s="5">
         <v>0.71369215979388334</v>
       </c>
-      <c r="M214">
+      <c r="M214" s="13">
         <v>41.681618333333333</v>
       </c>
-      <c r="N214">
+      <c r="N214" s="13">
         <v>-83.052401666666668</v>
       </c>
     </row>
@@ -10533,10 +10517,10 @@
       <c r="L215" s="5">
         <v>0.76135527292144567</v>
       </c>
-      <c r="M215">
+      <c r="M215" s="13">
         <v>41.779971666666668</v>
       </c>
-      <c r="N215">
+      <c r="N215" s="13">
         <v>-83.050718333333336</v>
       </c>
     </row>
@@ -10579,10 +10563,10 @@
       <c r="L216" s="5">
         <v>0.7287739311602669</v>
       </c>
-      <c r="M216">
+      <c r="M216" s="13">
         <v>41.879773333333333</v>
       </c>
-      <c r="N216">
+      <c r="N216" s="13">
         <v>-83.051929999999999</v>
       </c>
     </row>
@@ -10625,10 +10609,10 @@
       <c r="L217" s="5">
         <v>0.64635416748068431</v>
       </c>
-      <c r="M217">
+      <c r="M217" s="13">
         <v>41.979353333333336</v>
       </c>
-      <c r="N217">
+      <c r="N217" s="13">
         <v>-83.050420000000003</v>
       </c>
     </row>
@@ -10671,10 +10655,10 @@
       <c r="L218" s="5">
         <v>0.69749364894422783</v>
       </c>
-      <c r="M218">
+      <c r="M218" s="13">
         <v>41.580278333333332</v>
       </c>
-      <c r="N218">
+      <c r="N218" s="13">
         <v>-82.950406666666666</v>
       </c>
     </row>
@@ -10717,10 +10701,10 @@
       <c r="L219" s="5">
         <v>0.68319107793451894</v>
       </c>
-      <c r="M219">
+      <c r="M219" s="13">
         <v>41.681516666666667</v>
       </c>
-      <c r="N219">
+      <c r="N219" s="13">
         <v>-82.950073333333336</v>
       </c>
     </row>
@@ -10763,10 +10747,10 @@
       <c r="L220" s="5">
         <v>0.7653202063531187</v>
       </c>
-      <c r="M220">
+      <c r="M220" s="13">
         <v>41.764153333333333</v>
       </c>
-      <c r="N220">
+      <c r="N220" s="13">
         <v>-82.950996666666668</v>
       </c>
     </row>
@@ -10809,10 +10793,10 @@
       <c r="L221" s="5">
         <v>0.65835625266846132</v>
       </c>
-      <c r="M221">
+      <c r="M221" s="13">
         <v>41.879733333333334</v>
       </c>
-      <c r="N221">
+      <c r="N221" s="13">
         <v>-82.949584999999999</v>
       </c>
     </row>
@@ -10855,10 +10839,10 @@
       <c r="L222" s="5">
         <v>0.70643631536472928</v>
       </c>
-      <c r="M222">
+      <c r="M222" s="13">
         <v>41.673641666666668</v>
       </c>
-      <c r="N222">
+      <c r="N222" s="13">
         <v>-82.849578333333326</v>
       </c>
     </row>
@@ -10901,10 +10885,10 @@
       <c r="L223" s="5">
         <v>0.76072848553062478</v>
       </c>
-      <c r="M223">
+      <c r="M223" s="13">
         <v>41.763931666666664</v>
       </c>
-      <c r="N223">
+      <c r="N223" s="13">
         <v>-82.849721666666667</v>
       </c>
     </row>
@@ -10947,10 +10931,10 @@
       <c r="L224" s="5">
         <v>0.81100184058257496</v>
       </c>
-      <c r="M224">
+      <c r="M224" s="13">
         <v>41.864429999999999</v>
       </c>
-      <c r="N224">
+      <c r="N224" s="13">
         <v>-82.851031666666671</v>
       </c>
     </row>
@@ -10993,10 +10977,10 @@
       <c r="L225" s="5">
         <v>0.70074402478239584</v>
       </c>
-      <c r="M225">
+      <c r="M225" s="13">
         <v>41.963368333333335</v>
       </c>
-      <c r="N225">
+      <c r="N225" s="13">
         <v>-82.850043333333332</v>
       </c>
     </row>
@@ -11039,10 +11023,10 @@
       <c r="L226" s="5">
         <v>0.687285703837892</v>
       </c>
-      <c r="M226">
+      <c r="M226" s="13">
         <v>41.580604999999998</v>
       </c>
-      <c r="N226">
+      <c r="N226" s="13">
         <v>-82.748724999999993</v>
       </c>
     </row>
@@ -11085,10 +11069,10 @@
       <c r="L227" s="5">
         <v>0.70795147372792033</v>
       </c>
-      <c r="M227">
+      <c r="M227" s="13">
         <v>41.67868</v>
       </c>
-      <c r="N227">
+      <c r="N227" s="13">
         <v>-82.750368333333327</v>
       </c>
     </row>
@@ -11131,10 +11115,10 @@
       <c r="L228" s="5">
         <v>0.64111380390563422</v>
       </c>
-      <c r="M228">
+      <c r="M228" s="13">
         <v>41.779746666666668</v>
       </c>
-      <c r="N228">
+      <c r="N228" s="13">
         <v>-82.750056666666666</v>
       </c>
     </row>
@@ -11177,10 +11161,10 @@
       <c r="L229" s="5">
         <v>0.72128716716848384</v>
       </c>
-      <c r="M229">
+      <c r="M229" s="13">
         <v>41.866673333333331</v>
       </c>
-      <c r="N229">
+      <c r="N229" s="13">
         <v>-82.749285</v>
       </c>
     </row>
@@ -11223,10 +11207,10 @@
       <c r="L230" s="5">
         <v>0.72246039685039309</v>
       </c>
-      <c r="M230">
+      <c r="M230" s="13">
         <v>41.963426666666663</v>
       </c>
-      <c r="N230">
+      <c r="N230" s="13">
         <v>-82.748075</v>
       </c>
     </row>
@@ -11269,10 +11253,10 @@
       <c r="L231" s="5">
         <v>0.78329262291525759</v>
       </c>
-      <c r="M231">
+      <c r="M231" s="13">
         <v>41.580191666666664</v>
       </c>
-      <c r="N231">
+      <c r="N231" s="13">
         <v>-82.649150000000006</v>
       </c>
     </row>
@@ -11315,10 +11299,10 @@
       <c r="L232" s="5">
         <v>0.66338156698355244</v>
       </c>
-      <c r="M232">
+      <c r="M232" s="13">
         <v>41.679989999999997</v>
       </c>
-      <c r="N232">
+      <c r="N232" s="13">
         <v>-82.650606666666661</v>
       </c>
     </row>
@@ -11361,10 +11345,10 @@
       <c r="L233" s="5">
         <v>0.65243609420291038</v>
       </c>
-      <c r="M233">
+      <c r="M233" s="13">
         <v>41.86322333333333</v>
       </c>
-      <c r="N233">
+      <c r="N233" s="13">
         <v>-82.64994333333334</v>
       </c>
     </row>
@@ -11407,10 +11391,10 @@
       <c r="L234" s="5">
         <v>0.71539885569114103</v>
       </c>
-      <c r="M234">
+      <c r="M234" s="13">
         <v>41.979709999999997</v>
       </c>
-      <c r="N234">
+      <c r="N234" s="13">
         <v>-82.648321666666661</v>
       </c>
     </row>
@@ -11453,10 +11437,10 @@
       <c r="L235" s="5">
         <v>0.77952630699999126</v>
       </c>
-      <c r="M235">
+      <c r="M235" s="13">
         <v>41.479598333333335</v>
       </c>
-      <c r="N235">
+      <c r="N235" s="13">
         <v>-82.549705000000003</v>
       </c>
     </row>
@@ -11499,10 +11483,10 @@
       <c r="L236" s="5">
         <v>0.79039237547253893</v>
       </c>
-      <c r="M236">
+      <c r="M236" s="13">
         <v>41.580275</v>
       </c>
-      <c r="N236">
+      <c r="N236" s="13">
         <v>-82.549898333333331</v>
       </c>
     </row>
@@ -11545,10 +11529,10 @@
       <c r="L237" s="5">
         <v>0.76387525968160663</v>
       </c>
-      <c r="M237">
+      <c r="M237" s="13">
         <v>41.662996666666665</v>
       </c>
-      <c r="N237">
+      <c r="N237" s="13">
         <v>-82.548699999999997</v>
       </c>
     </row>
@@ -11591,10 +11575,10 @@
       <c r="L238" s="5">
         <v>0.67881606376855297</v>
       </c>
-      <c r="M238">
+      <c r="M238" s="13">
         <v>41.768798333333336</v>
       </c>
-      <c r="N238">
+      <c r="N238" s="13">
         <v>-82.560778333333332</v>
       </c>
     </row>
@@ -11637,10 +11621,10 @@
       <c r="L239" s="5">
         <v>0.66467098933697233</v>
       </c>
-      <c r="M239">
+      <c r="M239" s="13">
         <v>41.866776666666667</v>
       </c>
-      <c r="N239">
+      <c r="N239" s="13">
         <v>-82.533168333333336</v>
       </c>
     </row>
@@ -11683,10 +11667,10 @@
       <c r="L240" s="5">
         <v>0.69116001010806305</v>
       </c>
-      <c r="M240">
+      <c r="M240" s="13">
         <v>41.467066666666668</v>
       </c>
-      <c r="N240">
+      <c r="N240" s="13">
         <v>-82.449129999999997</v>
       </c>
     </row>
@@ -11729,10 +11713,10 @@
       <c r="L241" s="5">
         <v>0.68934783253085996</v>
       </c>
-      <c r="M241">
+      <c r="M241" s="13">
         <v>41.579605000000001</v>
       </c>
-      <c r="N241">
+      <c r="N241" s="13">
         <v>-82.449799999999996</v>
       </c>
     </row>
@@ -11775,10 +11759,10 @@
       <c r="L242" s="5">
         <v>0.74775541620038011</v>
       </c>
-      <c r="M242">
+      <c r="M242" s="13">
         <v>41.663441666666664</v>
       </c>
-      <c r="N242">
+      <c r="N242" s="13">
         <v>-82.451040000000006</v>
       </c>
     </row>
@@ -11821,10 +11805,10 @@
       <c r="L243" s="5">
         <v>0.76647693500472092</v>
       </c>
-      <c r="M243">
+      <c r="M243" s="13">
         <v>41.779924999999999</v>
       </c>
-      <c r="N243">
+      <c r="N243" s="13">
         <v>-82.449960000000004</v>
       </c>
     </row>
@@ -11867,10 +11851,10 @@
       <c r="L244" s="5">
         <v>0.67869628974442264</v>
       </c>
-      <c r="M244">
+      <c r="M244" s="13">
         <v>41.480318333333337</v>
       </c>
-      <c r="N244">
+      <c r="N244" s="13">
         <v>-82.351661666666672</v>
       </c>
     </row>
@@ -11913,10 +11897,10 @@
       <c r="L245" s="5">
         <v>0.74807136127038132</v>
       </c>
-      <c r="M245">
+      <c r="M245" s="13">
         <v>41.580271666666668</v>
       </c>
-      <c r="N245">
+      <c r="N245" s="13">
         <v>-82.350976666666668</v>
       </c>
     </row>
@@ -11959,10 +11943,10 @@
       <c r="L246" s="5">
         <v>0.74217960061917398</v>
       </c>
-      <c r="M246">
+      <c r="M246" s="13">
         <v>41.662689999999998</v>
       </c>
-      <c r="N246">
+      <c r="N246" s="13">
         <v>-82.347516666666664</v>
       </c>
     </row>
@@ -12005,10 +11989,10 @@
       <c r="L247" s="5">
         <v>0.72001272143480377</v>
       </c>
-      <c r="M247">
+      <c r="M247" s="13">
         <v>41.46508166666667</v>
       </c>
-      <c r="N247">
+      <c r="N247" s="13">
         <v>-82.251519999999999</v>
       </c>
     </row>
@@ -12033,7 +12017,7 @@
       <c r="F248" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G248" s="13" t="s">
+      <c r="G248" s="10" t="s">
         <v>62</v>
       </c>
       <c r="H248" s="4">
@@ -12051,10 +12035,10 @@
       <c r="L248" s="5">
         <v>0.45238801124254879</v>
       </c>
-      <c r="M248" s="10">
+      <c r="M248" s="14">
         <v>41.780617999999997</v>
       </c>
-      <c r="N248" s="10">
+      <c r="N248" s="14">
         <v>-83.357037000000005</v>
       </c>
     </row>
@@ -12079,7 +12063,7 @@
       <c r="F249" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G249" s="14" t="s">
+      <c r="G249" s="11" t="s">
         <v>63</v>
       </c>
       <c r="H249" s="4">
@@ -12097,10 +12081,10 @@
       <c r="L249" s="5">
         <v>0.53100171077520542</v>
       </c>
-      <c r="M249" s="11">
+      <c r="M249" s="15">
         <v>41.782623333333333</v>
       </c>
-      <c r="N249" s="11">
+      <c r="N249" s="15">
         <v>-83.257210000000001</v>
       </c>
     </row>
@@ -12125,7 +12109,7 @@
       <c r="F250" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G250" s="15">
+      <c r="G250" s="12">
         <v>1119</v>
       </c>
       <c r="H250" s="4">
@@ -12143,10 +12127,10 @@
       <c r="L250" s="5">
         <v>0.55051758220817859</v>
       </c>
-      <c r="M250" s="11">
+      <c r="M250" s="15">
         <v>41.882561666666668</v>
       </c>
-      <c r="N250" s="11">
+      <c r="N250" s="15">
         <v>-83.246515000000002</v>
       </c>
     </row>
@@ -12171,7 +12155,7 @@
       <c r="F251" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G251" s="15">
+      <c r="G251" s="12">
         <v>1410</v>
       </c>
       <c r="H251" s="4">
@@ -12189,10 +12173,10 @@
       <c r="L251" s="5">
         <v>0.61154901499628389</v>
       </c>
-      <c r="M251" s="11">
+      <c r="M251" s="15">
         <v>41.684106666666665</v>
       </c>
-      <c r="N251" s="11">
+      <c r="N251" s="15">
         <v>-83.152331666666669</v>
       </c>
     </row>
@@ -12217,7 +12201,7 @@
       <c r="F252" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G252" s="15">
+      <c r="G252" s="12">
         <v>1503</v>
       </c>
       <c r="H252" s="4">
@@ -12235,10 +12219,10 @@
       <c r="L252" s="5">
         <v>0.63553266238371908</v>
       </c>
-      <c r="M252" s="11">
+      <c r="M252" s="15">
         <v>41.780403333333332</v>
       </c>
-      <c r="N252" s="11">
+      <c r="N252" s="15">
         <v>-83.145273333333336</v>
       </c>
     </row>
@@ -12263,7 +12247,7 @@
       <c r="F253" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G253" s="15">
+      <c r="G253" s="12">
         <v>1211</v>
       </c>
       <c r="H253" s="4">
@@ -12281,10 +12265,10 @@
       <c r="L253" s="5">
         <v>0.52803516146815543</v>
       </c>
-      <c r="M253" s="11">
+      <c r="M253" s="15">
         <v>41.882696666666668</v>
       </c>
-      <c r="N253" s="11">
+      <c r="N253" s="15">
         <v>-83.156561666666661</v>
       </c>
     </row>
@@ -12309,7 +12293,7 @@
       <c r="F254" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G254" s="15">
+      <c r="G254" s="12">
         <v>1310</v>
       </c>
       <c r="H254" s="4">
@@ -12327,10 +12311,10 @@
       <c r="L254" s="5">
         <v>0.53515141076396611</v>
       </c>
-      <c r="M254" s="11">
+      <c r="M254" s="15">
         <v>41.981078333333336</v>
       </c>
-      <c r="N254" s="11">
+      <c r="N254" s="15">
         <v>-83.111045000000004</v>
       </c>
     </row>
@@ -12355,7 +12339,7 @@
       <c r="F255" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G255" s="15">
+      <c r="G255" s="12">
         <v>1316</v>
       </c>
       <c r="H255" s="4">
@@ -12373,10 +12357,10 @@
       <c r="L255" s="5">
         <v>0.60822456748496034</v>
       </c>
-      <c r="M255" s="11">
+      <c r="M255" s="15">
         <v>41.680958333333336</v>
       </c>
-      <c r="N255" s="11">
+      <c r="N255" s="15">
         <v>-83.047655000000006</v>
       </c>
     </row>
@@ -12401,7 +12385,7 @@
       <c r="F256" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G256" s="15">
+      <c r="G256" s="12">
         <v>1546</v>
       </c>
       <c r="H256" s="4">
@@ -12419,10 +12403,10 @@
       <c r="L256" s="5">
         <v>0.63752702728932775</v>
       </c>
-      <c r="M256" s="11">
+      <c r="M256" s="15">
         <v>41.777931666666667</v>
       </c>
-      <c r="N256" s="11">
+      <c r="N256" s="15">
         <v>-83.042265</v>
       </c>
     </row>
@@ -12447,7 +12431,7 @@
       <c r="F257" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G257" s="15">
+      <c r="G257" s="12">
         <v>1457</v>
       </c>
       <c r="H257" s="4">
@@ -12465,10 +12449,10 @@
       <c r="L257" s="5">
         <v>0.54907442667316364</v>
       </c>
-      <c r="M257" s="11">
+      <c r="M257" s="15">
         <v>41.878588333333333</v>
       </c>
-      <c r="N257" s="11">
+      <c r="N257" s="15">
         <v>-83.058131666666668</v>
       </c>
     </row>
@@ -12493,7 +12477,7 @@
       <c r="F258" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G258" s="15">
+      <c r="G258" s="12">
         <v>1357</v>
       </c>
       <c r="H258" s="4">
@@ -12511,10 +12495,10 @@
       <c r="L258" s="5">
         <v>0.6962758987596489</v>
       </c>
-      <c r="M258" s="11">
+      <c r="M258" s="15">
         <v>41.982321666666664</v>
       </c>
-      <c r="N258" s="11">
+      <c r="N258" s="15">
         <v>-83.055136666666669</v>
       </c>
     </row>
@@ -12539,7 +12523,7 @@
       <c r="F259" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G259" s="15">
+      <c r="G259" s="12">
         <v>1136</v>
       </c>
       <c r="H259" s="4">
@@ -12557,10 +12541,10 @@
       <c r="L259" s="5">
         <v>0.53229294460604593</v>
       </c>
-      <c r="M259" s="11">
+      <c r="M259" s="15">
         <v>41.568291666666667</v>
       </c>
-      <c r="N259" s="11">
+      <c r="N259" s="15">
         <v>-82.949968333333331</v>
       </c>
     </row>
@@ -12585,7 +12569,7 @@
       <c r="F260" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G260" s="15">
+      <c r="G260" s="12">
         <v>1228</v>
       </c>
       <c r="H260" s="4">
@@ -12603,10 +12587,10 @@
       <c r="L260" s="5">
         <v>0.63470061930631916</v>
       </c>
-      <c r="M260" s="11">
+      <c r="M260" s="15">
         <v>41.667029999999997</v>
       </c>
-      <c r="N260" s="11">
+      <c r="N260" s="15">
         <v>-82.957336666666663</v>
       </c>
     </row>
@@ -12631,7 +12615,7 @@
       <c r="F261" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G261" s="15">
+      <c r="G261" s="12">
         <v>1632</v>
       </c>
       <c r="H261" s="4">
@@ -12649,10 +12633,10 @@
       <c r="L261" s="5">
         <v>0.65856218008939083</v>
       </c>
-      <c r="M261" s="11">
+      <c r="M261" s="15">
         <v>41.759251666666664</v>
       </c>
-      <c r="N261" s="11">
+      <c r="N261" s="15">
         <v>-82.943691666666666</v>
       </c>
     </row>
@@ -12677,7 +12661,7 @@
       <c r="F262" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G262" s="15">
+      <c r="G262" s="12">
         <v>1553</v>
       </c>
       <c r="H262" s="4">
@@ -12695,10 +12679,10 @@
       <c r="L262" s="5">
         <v>0.62179239939909126</v>
       </c>
-      <c r="M262" s="12">
+      <c r="M262" s="15">
         <v>41.886748333333337</v>
       </c>
-      <c r="N262" s="12">
+      <c r="N262" s="15">
         <v>-82.975096666666673</v>
       </c>
     </row>
@@ -12723,7 +12707,7 @@
       <c r="F263" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G263" s="14" t="s">
+      <c r="G263" s="11" t="s">
         <v>64</v>
       </c>
       <c r="H263" s="4">
@@ -12741,10 +12725,10 @@
       <c r="L263" s="5">
         <v>0.47245629945413914</v>
       </c>
-      <c r="M263" s="11">
+      <c r="M263" s="15">
         <v>41.659418333333335</v>
       </c>
-      <c r="N263" s="11">
+      <c r="N263" s="15">
         <v>-82.864731666666671</v>
       </c>
     </row>
@@ -12769,7 +12753,7 @@
       <c r="F264" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G264" s="14">
+      <c r="G264" s="11">
         <v>1848</v>
       </c>
       <c r="H264" s="4">
@@ -12787,10 +12771,10 @@
       <c r="L264" s="5">
         <v>0.53739698166254224</v>
       </c>
-      <c r="M264" s="11">
+      <c r="M264" s="15">
         <v>41.764508333333332</v>
       </c>
-      <c r="N264" s="11">
+      <c r="N264" s="15">
         <v>-82.857323333333326</v>
       </c>
     </row>
@@ -12815,7 +12799,7 @@
       <c r="F265" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G265" s="15">
+      <c r="G265" s="12">
         <v>1002</v>
       </c>
       <c r="H265" s="4">
@@ -12833,10 +12817,10 @@
       <c r="L265" s="5">
         <v>0.60670685928041668</v>
       </c>
-      <c r="M265" s="11">
+      <c r="M265" s="15">
         <v>41.865475000000004</v>
       </c>
-      <c r="N265" s="11">
+      <c r="N265" s="15">
         <v>-82.857448333333338</v>
       </c>
     </row>
@@ -12861,7 +12845,7 @@
       <c r="F266" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G266" s="15">
+      <c r="G266" s="12">
         <v>1720</v>
       </c>
       <c r="H266" s="4">
@@ -12879,10 +12863,10 @@
       <c r="L266" s="5">
         <v>0.60156739967702966</v>
       </c>
-      <c r="M266" s="11">
+      <c r="M266" s="15">
         <v>41.960120000000003</v>
       </c>
-      <c r="N266" s="11">
+      <c r="N266" s="15">
         <v>-82.852365000000006</v>
       </c>
     </row>
@@ -12907,7 +12891,7 @@
       <c r="F267" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G267" s="15">
+      <c r="G267" s="12">
         <v>1025</v>
       </c>
       <c r="H267" s="4">
@@ -12925,10 +12909,10 @@
       <c r="L267" s="5">
         <v>0.6320147390890648</v>
       </c>
-      <c r="M267" s="11">
+      <c r="M267" s="15">
         <v>41.565370000000001</v>
       </c>
-      <c r="N267" s="11">
+      <c r="N267" s="15">
         <v>-82.756320000000002</v>
       </c>
     </row>
@@ -12953,7 +12937,7 @@
       <c r="F268" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G268" s="14" t="s">
+      <c r="G268" s="11" t="s">
         <v>65</v>
       </c>
       <c r="H268" s="4">
@@ -12971,10 +12955,10 @@
       <c r="L268" s="5">
         <v>0.60356586565014014</v>
       </c>
-      <c r="M268" s="11">
+      <c r="M268" s="15">
         <v>41.682253000000003</v>
       </c>
-      <c r="N268" s="11">
+      <c r="N268" s="15">
         <v>-82.757992999999999</v>
       </c>
     </row>
@@ -12999,7 +12983,7 @@
       <c r="F269" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G269" s="14" t="s">
+      <c r="G269" s="11" t="s">
         <v>66</v>
       </c>
       <c r="H269" s="4">
@@ -13017,10 +13001,10 @@
       <c r="L269" s="5">
         <v>0.55727284916328412</v>
       </c>
-      <c r="M269" s="11">
+      <c r="M269" s="15">
         <v>41.78208166666667</v>
       </c>
-      <c r="N269" s="11">
+      <c r="N269" s="15">
         <v>-82.75610833333333</v>
       </c>
     </row>
@@ -13045,7 +13029,7 @@
       <c r="F270" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G270" s="14" t="s">
+      <c r="G270" s="11" t="s">
         <v>67</v>
       </c>
       <c r="H270" s="4">
@@ -13063,10 +13047,10 @@
       <c r="L270" s="5">
         <v>0.62501302798094094</v>
       </c>
-      <c r="M270" s="11">
+      <c r="M270" s="15">
         <v>41.868568333333336</v>
       </c>
-      <c r="N270" s="11">
+      <c r="N270" s="15">
         <v>-82.756618333333336</v>
       </c>
     </row>
@@ -13091,7 +13075,7 @@
       <c r="F271" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G271" s="15">
+      <c r="G271" s="12">
         <v>1108</v>
       </c>
       <c r="H271" s="4">
@@ -13109,10 +13093,10 @@
       <c r="L271" s="5">
         <v>0.6466183059829822</v>
       </c>
-      <c r="M271" s="11">
+      <c r="M271" s="15">
         <v>41.966994999999997</v>
       </c>
-      <c r="N271" s="11">
+      <c r="N271" s="15">
         <v>-82.75908166666666</v>
       </c>
     </row>
@@ -13137,7 +13121,7 @@
       <c r="F272" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G272" s="14" t="s">
+      <c r="G272" s="11" t="s">
         <v>68</v>
       </c>
       <c r="H272" s="4">
@@ -13155,10 +13139,10 @@
       <c r="L272" s="5">
         <v>0.83484254000265412</v>
       </c>
-      <c r="M272" s="11">
+      <c r="M272" s="15">
         <v>41.561921666666663</v>
       </c>
-      <c r="N272" s="11">
+      <c r="N272" s="15">
         <v>-82.655696666666671</v>
       </c>
     </row>
@@ -13183,7 +13167,7 @@
       <c r="F273" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G273" s="15">
+      <c r="G273" s="12">
         <v>1723</v>
       </c>
       <c r="H273" s="4">
@@ -13201,10 +13185,10 @@
       <c r="L273" s="5">
         <v>0.62024117591913108</v>
       </c>
-      <c r="M273" s="11">
+      <c r="M273" s="15">
         <v>41.679755</v>
       </c>
-      <c r="N273" s="11">
+      <c r="N273" s="15">
         <v>-82.657749999999993</v>
       </c>
     </row>
@@ -13229,7 +13213,7 @@
       <c r="F274" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G274" s="15">
+      <c r="G274" s="12">
         <v>1317</v>
       </c>
       <c r="H274" s="4">
@@ -13247,10 +13231,10 @@
       <c r="L274" s="5">
         <v>0.56390263806937857</v>
       </c>
-      <c r="M274" s="11">
+      <c r="M274" s="15">
         <v>41.863208333333333</v>
       </c>
-      <c r="N274" s="11">
+      <c r="N274" s="15">
         <v>-82.643786666666671</v>
       </c>
     </row>
@@ -13275,7 +13259,7 @@
       <c r="F275" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G275" s="15">
+      <c r="G275" s="12">
         <v>1217</v>
       </c>
       <c r="H275" s="4">
@@ -13293,10 +13277,10 @@
       <c r="L275" s="5">
         <v>0.66134936727366744</v>
       </c>
-      <c r="M275" s="11">
+      <c r="M275" s="15">
         <v>41.975793333333336</v>
       </c>
-      <c r="N275" s="11">
+      <c r="N275" s="15">
         <v>-82.646136666666663</v>
       </c>
     </row>
@@ -13321,7 +13305,7 @@
       <c r="F276" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G276" s="14" t="s">
+      <c r="G276" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H276" s="4">
@@ -13339,10 +13323,10 @@
       <c r="L276" s="5">
         <v>0.61053044575004844</v>
       </c>
-      <c r="M276" s="11">
+      <c r="M276" s="15">
         <v>41.456028333333336</v>
       </c>
-      <c r="N276" s="11">
+      <c r="N276" s="15">
         <v>-82.564176666666668</v>
       </c>
     </row>
@@ -13367,7 +13351,7 @@
       <c r="F277" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G277" s="14" t="s">
+      <c r="G277" s="11" t="s">
         <v>70</v>
       </c>
       <c r="H277" s="4">
@@ -13385,10 +13369,10 @@
       <c r="L277" s="5">
         <v>0.66926522148606205</v>
       </c>
-      <c r="M277" s="11">
+      <c r="M277" s="15">
         <v>41.559903333333331</v>
       </c>
-      <c r="N277" s="11">
+      <c r="N277" s="15">
         <v>-82.554956666666669</v>
       </c>
     </row>
@@ -13413,7 +13397,7 @@
       <c r="F278" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G278" s="15">
+      <c r="G278" s="12">
         <v>1637</v>
       </c>
       <c r="H278" s="4">
@@ -13431,10 +13415,10 @@
       <c r="L278" s="5">
         <v>0.5780157123385935</v>
       </c>
-      <c r="M278" s="11">
+      <c r="M278" s="15">
         <v>41.663694999999997</v>
       </c>
-      <c r="N278" s="11">
+      <c r="N278" s="15">
         <v>-82.55978833333333</v>
       </c>
     </row>
@@ -13459,7 +13443,7 @@
       <c r="F279" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G279" s="15">
+      <c r="G279" s="12">
         <v>1540</v>
       </c>
       <c r="H279" s="4">
@@ -13477,10 +13461,10 @@
       <c r="L279" s="5">
         <v>0.57943883397356466</v>
       </c>
-      <c r="M279" s="11">
+      <c r="M279" s="15">
         <v>41.774635000000004</v>
       </c>
-      <c r="N279" s="11">
+      <c r="N279" s="15">
         <v>-82.55286666666666</v>
       </c>
     </row>
@@ -13505,7 +13489,7 @@
       <c r="F280" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G280" s="15">
+      <c r="G280" s="12">
         <v>1404</v>
       </c>
       <c r="H280" s="4">
@@ -13523,10 +13507,10 @@
       <c r="L280" s="5">
         <v>0.64243376002818542</v>
       </c>
-      <c r="M280" s="11">
+      <c r="M280" s="15">
         <v>41.862161666666665</v>
       </c>
-      <c r="N280" s="11">
+      <c r="N280" s="15">
         <v>-82.532025000000004</v>
       </c>
     </row>
@@ -13551,7 +13535,7 @@
       <c r="F281" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G281" s="15">
+      <c r="G281" s="12">
         <v>1534</v>
       </c>
       <c r="H281" s="4">
@@ -13569,10 +13553,10 @@
       <c r="L281" s="5">
         <v>0.6603960024276444</v>
       </c>
-      <c r="M281" s="11">
+      <c r="M281" s="15">
         <v>41.475636666666666</v>
       </c>
-      <c r="N281" s="11">
+      <c r="N281" s="15">
         <v>-82.441946666666666</v>
       </c>
     </row>
@@ -13597,7 +13581,7 @@
       <c r="F282" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G282" s="15">
+      <c r="G282" s="12">
         <v>1034</v>
       </c>
       <c r="H282" s="4">
@@ -13615,10 +13599,10 @@
       <c r="L282" s="5">
         <v>0.61322411701660473</v>
       </c>
-      <c r="M282" s="11">
+      <c r="M282" s="15">
         <v>41.579303333333336</v>
       </c>
-      <c r="N282" s="11">
+      <c r="N282" s="15">
         <v>-82.442565000000002</v>
       </c>
     </row>
@@ -13643,7 +13627,7 @@
       <c r="F283" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G283" s="14" t="s">
+      <c r="G283" s="11" t="s">
         <v>71</v>
       </c>
       <c r="H283" s="4">
@@ -13661,10 +13645,10 @@
       <c r="L283" s="5">
         <v>0.6114676560048935</v>
       </c>
-      <c r="M283" s="11">
+      <c r="M283" s="15">
         <v>41.671765000000001</v>
       </c>
-      <c r="N283" s="11">
+      <c r="N283" s="15">
         <v>-82.44804666666667</v>
       </c>
     </row>
@@ -13689,7 +13673,7 @@
       <c r="F284" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G284" s="15">
+      <c r="G284" s="12">
         <v>1457</v>
       </c>
       <c r="H284" s="4">
@@ -13707,10 +13691,10 @@
       <c r="L284" s="5">
         <v>0.63331817568793325</v>
       </c>
-      <c r="M284" s="11">
+      <c r="M284" s="15">
         <v>41.779963333333335</v>
       </c>
-      <c r="N284" s="11">
+      <c r="N284" s="15">
         <v>-82.457828333333339</v>
       </c>
     </row>
@@ -13735,7 +13719,7 @@
       <c r="F285" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G285" s="15">
+      <c r="G285" s="12">
         <v>1435</v>
       </c>
       <c r="H285" s="4">
@@ -13753,10 +13737,10 @@
       <c r="L285" s="5">
         <v>0.62162291674857484</v>
       </c>
-      <c r="M285" s="11">
+      <c r="M285" s="15">
         <v>41.479901666666663</v>
       </c>
-      <c r="N285" s="11">
+      <c r="N285" s="15">
         <v>-82.343586666666667</v>
       </c>
     </row>
@@ -13781,7 +13765,7 @@
       <c r="F286" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G286" s="15">
+      <c r="G286" s="12">
         <v>1119</v>
       </c>
       <c r="H286" s="4">
@@ -13799,10 +13783,10 @@
       <c r="L286" s="5">
         <v>0.61369627862665044</v>
       </c>
-      <c r="M286" s="11">
+      <c r="M286" s="15">
         <v>41.574436666666664</v>
       </c>
-      <c r="N286" s="11">
+      <c r="N286" s="15">
         <v>-82.343661666666662</v>
       </c>
     </row>
@@ -13827,7 +13811,7 @@
       <c r="F287" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G287" s="14" t="s">
+      <c r="G287" s="11" t="s">
         <v>72</v>
       </c>
       <c r="H287" s="4">
@@ -13845,10 +13829,10 @@
       <c r="L287" s="5">
         <v>0.6152698330510098</v>
       </c>
-      <c r="M287" s="11">
+      <c r="M287" s="15">
         <v>41.668039999999998</v>
       </c>
-      <c r="N287" s="11">
+      <c r="N287" s="15">
         <v>-82.347456666666673</v>
       </c>
     </row>
@@ -13873,7 +13857,7 @@
       <c r="F288" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G288" s="15">
+      <c r="G288" s="12">
         <v>1227</v>
       </c>
       <c r="H288" s="4">
@@ -13891,10 +13875,10 @@
       <c r="L288" s="5">
         <v>0.39173470292397777</v>
       </c>
-      <c r="M288" s="11">
+      <c r="M288" s="15">
         <v>41.460701666666665</v>
       </c>
-      <c r="N288" s="11">
+      <c r="N288" s="15">
         <v>-82.254831666666661</v>
       </c>
     </row>

</xml_diff>

<commit_message>
UPDATED with Autumn 2016 data
still needs some small revisions to fix MathJax and review the water
quality table for functionality
</commit_message>
<xml_diff>
--- a/data_prep/WB_Effort.xlsx
+++ b/data_prep/WB_Effort.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12720" windowHeight="12405"/>
+    <workbookView xWindow="12705" yWindow="-15" windowWidth="12510" windowHeight="11805"/>
   </bookViews>
   <sheets>
     <sheet name="Effort" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="80">
   <si>
     <t>serial</t>
   </si>
@@ -241,6 +241,27 @@
   </si>
   <si>
     <t>0927</t>
+  </si>
+  <si>
+    <t>0740</t>
+  </si>
+  <si>
+    <t>0729</t>
+  </si>
+  <si>
+    <t>0824</t>
+  </si>
+  <si>
+    <t>0913</t>
+  </si>
+  <si>
+    <t>1005</t>
+  </si>
+  <si>
+    <t>0943</t>
+  </si>
+  <si>
+    <t>0918</t>
   </si>
 </sst>
 </file>
@@ -611,11 +632,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N288"/>
+  <dimension ref="A1:N329"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A246" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U266" sqref="U266"/>
+      <pane ySplit="1" topLeftCell="A296" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G330" sqref="G330"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9566,11 +9587,11 @@
         <v>42170</v>
       </c>
       <c r="C195" s="4">
-        <f t="shared" ref="C195:C258" si="6">DAY(B195)</f>
+        <f t="shared" ref="C195:C247" si="6">DAY(B195)</f>
         <v>15</v>
       </c>
       <c r="D195" s="4">
-        <f t="shared" ref="D195:D258" si="7">MONTH(B195)</f>
+        <f t="shared" ref="D195:D247" si="7">MONTH(B195)</f>
         <v>6</v>
       </c>
       <c r="E195" s="2">
@@ -12004,11 +12025,9 @@
         <v>42535</v>
       </c>
       <c r="C248" s="4">
-        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="D248" s="4">
-        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="E248" s="2">
@@ -12021,7 +12040,7 @@
         <v>62</v>
       </c>
       <c r="H248" s="4">
-        <v>16.5</v>
+        <v>5.0292000000000003</v>
       </c>
       <c r="I248" s="7">
         <v>6.16</v>
@@ -12050,11 +12069,9 @@
         <v>42535</v>
       </c>
       <c r="C249" s="4">
-        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="D249" s="4">
-        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="E249" s="2">
@@ -12067,7 +12084,7 @@
         <v>63</v>
       </c>
       <c r="H249" s="4">
-        <v>23.3</v>
+        <v>7.1018400000000002</v>
       </c>
       <c r="I249" s="7">
         <v>6.96</v>
@@ -12096,11 +12113,9 @@
         <v>42535</v>
       </c>
       <c r="C250" s="4">
-        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="D250" s="4">
-        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="E250" s="2">
@@ -12113,7 +12128,7 @@
         <v>1119</v>
       </c>
       <c r="H250" s="4">
-        <v>24</v>
+        <v>7.3151999999999999</v>
       </c>
       <c r="I250" s="7">
         <v>7.0600000000000005</v>
@@ -12142,11 +12157,9 @@
         <v>42534</v>
       </c>
       <c r="C251" s="4">
-        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="D251" s="4">
-        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="E251" s="2">
@@ -12159,7 +12172,7 @@
         <v>1410</v>
       </c>
       <c r="H251" s="4">
-        <v>23</v>
+        <v>7.0103999999999997</v>
       </c>
       <c r="I251" s="7">
         <v>7.36</v>
@@ -12188,11 +12201,9 @@
         <v>42534</v>
       </c>
       <c r="C252" s="4">
-        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="D252" s="4">
-        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="E252" s="2">
@@ -12205,7 +12216,7 @@
         <v>1503</v>
       </c>
       <c r="H252" s="4">
-        <v>26</v>
+        <v>7.9248000000000003</v>
       </c>
       <c r="I252" s="7">
         <v>7.66</v>
@@ -12234,11 +12245,9 @@
         <v>42535</v>
       </c>
       <c r="C253" s="4">
-        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="D253" s="4">
-        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="E253" s="2">
@@ -12251,7 +12260,7 @@
         <v>1211</v>
       </c>
       <c r="H253" s="4">
-        <v>31</v>
+        <v>9.4488000000000003</v>
       </c>
       <c r="I253" s="7">
         <v>7.0600000000000005</v>
@@ -12280,11 +12289,9 @@
         <v>42535</v>
       </c>
       <c r="C254" s="4">
-        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="D254" s="4">
-        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="E254" s="2">
@@ -12297,7 +12304,7 @@
         <v>1310</v>
       </c>
       <c r="H254" s="4">
-        <v>25</v>
+        <v>7.62</v>
       </c>
       <c r="I254" s="7">
         <v>6.76</v>
@@ -12326,11 +12333,9 @@
         <v>42534</v>
       </c>
       <c r="C255" s="4">
-        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="D255" s="4">
-        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="E255" s="2">
@@ -12343,7 +12348,7 @@
         <v>1316</v>
       </c>
       <c r="H255" s="4">
-        <v>27</v>
+        <v>8.2295999999999996</v>
       </c>
       <c r="I255" s="7">
         <v>7.76</v>
@@ -12372,11 +12377,9 @@
         <v>42534</v>
       </c>
       <c r="C256" s="4">
-        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="D256" s="4">
-        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="E256" s="2">
@@ -12389,7 +12392,7 @@
         <v>1546</v>
       </c>
       <c r="H256" s="4">
-        <v>30</v>
+        <v>9.1440000000000001</v>
       </c>
       <c r="I256" s="7">
         <v>7.76</v>
@@ -12418,11 +12421,9 @@
         <v>42535</v>
       </c>
       <c r="C257" s="4">
-        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="D257" s="4">
-        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="E257" s="2">
@@ -12435,7 +12436,7 @@
         <v>1457</v>
       </c>
       <c r="H257" s="4">
-        <v>33</v>
+        <v>10.058400000000001</v>
       </c>
       <c r="I257" s="7">
         <v>7.0600000000000005</v>
@@ -12464,11 +12465,9 @@
         <v>42535</v>
       </c>
       <c r="C258" s="4">
-        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="D258" s="4">
-        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="E258" s="2">
@@ -12481,7 +12480,7 @@
         <v>1357</v>
       </c>
       <c r="H258" s="4">
-        <v>28</v>
+        <v>8.5343999999999998</v>
       </c>
       <c r="I258" s="7">
         <v>6.96</v>
@@ -12510,11 +12509,9 @@
         <v>42534</v>
       </c>
       <c r="C259" s="4">
-        <f t="shared" ref="C259:C288" si="8">DAY(B259)</f>
         <v>13</v>
       </c>
       <c r="D259" s="4">
-        <f t="shared" ref="D259:D288" si="9">MONTH(B259)</f>
         <v>6</v>
       </c>
       <c r="E259" s="2">
@@ -12527,7 +12524,7 @@
         <v>1136</v>
       </c>
       <c r="H259" s="4">
-        <v>18.5</v>
+        <v>5.6387999999999998</v>
       </c>
       <c r="I259" s="7">
         <v>6.86</v>
@@ -12556,11 +12553,9 @@
         <v>42534</v>
       </c>
       <c r="C260" s="4">
-        <f t="shared" si="8"/>
         <v>13</v>
       </c>
       <c r="D260" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E260" s="2">
@@ -12573,7 +12568,7 @@
         <v>1228</v>
       </c>
       <c r="H260" s="4">
-        <v>28.5</v>
+        <v>8.6867999999999999</v>
       </c>
       <c r="I260" s="7">
         <v>7.96</v>
@@ -12602,11 +12597,9 @@
         <v>42534</v>
       </c>
       <c r="C261" s="4">
-        <f t="shared" si="8"/>
         <v>13</v>
       </c>
       <c r="D261" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E261" s="2">
@@ -12619,7 +12612,7 @@
         <v>1632</v>
       </c>
       <c r="H261" s="4">
-        <v>31</v>
+        <v>9.4488000000000003</v>
       </c>
       <c r="I261" s="7">
         <v>8.36</v>
@@ -12648,11 +12641,9 @@
         <v>42535</v>
       </c>
       <c r="C262" s="4">
-        <f t="shared" si="8"/>
         <v>14</v>
       </c>
       <c r="D262" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E262" s="2">
@@ -12665,7 +12656,7 @@
         <v>1553</v>
       </c>
       <c r="H262" s="4">
-        <v>35.5</v>
+        <v>10.820399999999999</v>
       </c>
       <c r="I262" s="7">
         <v>7.5600000000000005</v>
@@ -12694,11 +12685,9 @@
         <v>42535</v>
       </c>
       <c r="C263" s="4">
-        <f t="shared" si="8"/>
         <v>14</v>
       </c>
       <c r="D263" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E263" s="2">
@@ -12711,7 +12700,7 @@
         <v>64</v>
       </c>
       <c r="H263" s="4">
-        <v>30</v>
+        <v>9.1440000000000001</v>
       </c>
       <c r="I263" s="7">
         <v>7.46</v>
@@ -12740,11 +12729,9 @@
         <v>42535</v>
       </c>
       <c r="C264" s="4">
-        <f t="shared" si="8"/>
         <v>14</v>
       </c>
       <c r="D264" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E264" s="2">
@@ -12757,7 +12744,7 @@
         <v>1848</v>
       </c>
       <c r="H264" s="4">
-        <v>36</v>
+        <v>10.972799999999999</v>
       </c>
       <c r="I264" s="7">
         <v>7.0600000000000005</v>
@@ -12786,11 +12773,9 @@
         <v>42536</v>
       </c>
       <c r="C265" s="4">
-        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="D265" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E265" s="2">
@@ -12803,7 +12788,7 @@
         <v>1002</v>
       </c>
       <c r="H265" s="4">
-        <v>38</v>
+        <v>11.5824</v>
       </c>
       <c r="I265" s="7">
         <v>7.5600000000000005</v>
@@ -12832,11 +12817,9 @@
         <v>42535</v>
       </c>
       <c r="C266" s="4">
-        <f t="shared" si="8"/>
         <v>14</v>
       </c>
       <c r="D266" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E266" s="2">
@@ -12849,7 +12832,7 @@
         <v>1720</v>
       </c>
       <c r="H266" s="4">
-        <v>35</v>
+        <v>10.667999999999999</v>
       </c>
       <c r="I266" s="7">
         <v>7.16</v>
@@ -12878,11 +12861,9 @@
         <v>42534</v>
       </c>
       <c r="C267" s="4">
-        <f t="shared" si="8"/>
         <v>13</v>
       </c>
       <c r="D267" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E267" s="2">
@@ -12895,7 +12876,7 @@
         <v>1025</v>
       </c>
       <c r="H267" s="4">
-        <v>25</v>
+        <v>7.62</v>
       </c>
       <c r="I267" s="7">
         <v>7.86</v>
@@ -12924,11 +12905,9 @@
         <v>42536</v>
       </c>
       <c r="C268" s="4">
-        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="D268" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E268" s="2">
@@ -12941,7 +12920,7 @@
         <v>65</v>
       </c>
       <c r="H268" s="4">
-        <v>35</v>
+        <v>10.667999999999999</v>
       </c>
       <c r="I268" s="7">
         <v>7.46</v>
@@ -12970,11 +12949,9 @@
         <v>42536</v>
       </c>
       <c r="C269" s="4">
-        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="D269" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E269" s="2">
@@ -12987,7 +12964,7 @@
         <v>66</v>
       </c>
       <c r="H269" s="4">
-        <v>33</v>
+        <v>10.058400000000001</v>
       </c>
       <c r="I269" s="7">
         <v>7.16</v>
@@ -13016,11 +12993,9 @@
         <v>42536</v>
       </c>
       <c r="C270" s="4">
-        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="D270" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E270" s="2">
@@ -13033,7 +13008,7 @@
         <v>67</v>
       </c>
       <c r="H270" s="4">
-        <v>40</v>
+        <v>12.192</v>
       </c>
       <c r="I270" s="7">
         <v>7.76</v>
@@ -13062,11 +13037,9 @@
         <v>42536</v>
       </c>
       <c r="C271" s="4">
-        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="D271" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E271" s="2">
@@ -13079,7 +13052,7 @@
         <v>1108</v>
       </c>
       <c r="H271" s="4">
-        <v>37</v>
+        <v>11.2776</v>
       </c>
       <c r="I271" s="7">
         <v>7.66</v>
@@ -13108,11 +13081,9 @@
         <v>42534</v>
       </c>
       <c r="C272" s="4">
-        <f t="shared" si="8"/>
         <v>13</v>
       </c>
       <c r="D272" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E272" s="2">
@@ -13125,7 +13096,7 @@
         <v>68</v>
       </c>
       <c r="H272" s="4">
-        <v>40</v>
+        <v>12.192</v>
       </c>
       <c r="I272" s="7">
         <v>9.66</v>
@@ -13154,11 +13125,9 @@
         <v>42536</v>
       </c>
       <c r="C273" s="4">
-        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="D273" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E273" s="2">
@@ -13171,7 +13140,7 @@
         <v>1723</v>
       </c>
       <c r="H273" s="4">
-        <v>36</v>
+        <v>10.972799999999999</v>
       </c>
       <c r="I273" s="7">
         <v>7.0600000000000005</v>
@@ -13200,11 +13169,9 @@
         <v>42536</v>
       </c>
       <c r="C274" s="4">
-        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="D274" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E274" s="2">
@@ -13217,7 +13184,7 @@
         <v>1317</v>
       </c>
       <c r="H274" s="4">
-        <v>38</v>
+        <v>11.5824</v>
       </c>
       <c r="I274" s="7">
         <v>7.16</v>
@@ -13246,11 +13213,9 @@
         <v>42536</v>
       </c>
       <c r="C275" s="4">
-        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="D275" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E275" s="2">
@@ -13263,7 +13228,7 @@
         <v>1217</v>
       </c>
       <c r="H275" s="4">
-        <v>36.5</v>
+        <v>11.1252</v>
       </c>
       <c r="I275" s="7">
         <v>7.66</v>
@@ -13292,11 +13257,9 @@
         <v>42534</v>
       </c>
       <c r="C276" s="4">
-        <f t="shared" si="8"/>
         <v>13</v>
       </c>
       <c r="D276" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E276" s="2">
@@ -13309,7 +13272,7 @@
         <v>69</v>
       </c>
       <c r="H276" s="4">
-        <v>39</v>
+        <v>11.8872</v>
       </c>
       <c r="I276" s="7">
         <v>8.56</v>
@@ -13338,11 +13301,9 @@
         <v>42534</v>
       </c>
       <c r="C277" s="4">
-        <f t="shared" si="8"/>
         <v>13</v>
       </c>
       <c r="D277" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E277" s="2">
@@ -13355,7 +13316,7 @@
         <v>70</v>
       </c>
       <c r="H277" s="4">
-        <v>42</v>
+        <v>12.801600000000001</v>
       </c>
       <c r="I277" s="7">
         <v>8.4599999999999991</v>
@@ -13384,11 +13345,9 @@
         <v>42536</v>
       </c>
       <c r="C278" s="4">
-        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="D278" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E278" s="2">
@@ -13401,7 +13360,7 @@
         <v>1637</v>
       </c>
       <c r="H278" s="4">
-        <v>45</v>
+        <v>13.715999999999999</v>
       </c>
       <c r="I278" s="7">
         <v>7.66</v>
@@ -13430,11 +13389,9 @@
         <v>42536</v>
       </c>
       <c r="C279" s="4">
-        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="D279" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E279" s="2">
@@ -13447,7 +13404,7 @@
         <v>1540</v>
       </c>
       <c r="H279" s="4">
-        <v>37.5</v>
+        <v>11.43</v>
       </c>
       <c r="I279" s="7">
         <v>7.46</v>
@@ -13476,11 +13433,9 @@
         <v>42536</v>
       </c>
       <c r="C280" s="4">
-        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="D280" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E280" s="2">
@@ -13493,7 +13448,7 @@
         <v>1404</v>
       </c>
       <c r="H280" s="4">
-        <v>40.5</v>
+        <v>12.3444</v>
       </c>
       <c r="I280" s="7">
         <v>7.96</v>
@@ -13522,11 +13477,9 @@
         <v>42537</v>
       </c>
       <c r="C281" s="4">
-        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="D281" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E281" s="2">
@@ -13539,7 +13492,7 @@
         <v>1534</v>
       </c>
       <c r="H281" s="4">
-        <v>48</v>
+        <v>14.6304</v>
       </c>
       <c r="I281" s="7">
         <v>7.96</v>
@@ -13568,11 +13521,9 @@
         <v>42537</v>
       </c>
       <c r="C282" s="4">
-        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="D282" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E282" s="2">
@@ -13585,7 +13536,7 @@
         <v>1034</v>
       </c>
       <c r="H282" s="4">
-        <v>48</v>
+        <v>14.6304</v>
       </c>
       <c r="I282" s="7">
         <v>7.76</v>
@@ -13614,11 +13565,9 @@
         <v>42537</v>
       </c>
       <c r="C283" s="4">
-        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="D283" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E283" s="2">
@@ -13631,7 +13580,7 @@
         <v>71</v>
       </c>
       <c r="H283" s="4">
-        <v>48</v>
+        <v>14.6304</v>
       </c>
       <c r="I283" s="7">
         <v>7.86</v>
@@ -13660,11 +13609,9 @@
         <v>42536</v>
       </c>
       <c r="C284" s="4">
-        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="D284" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E284" s="2">
@@ -13677,7 +13624,7 @@
         <v>1457</v>
       </c>
       <c r="H284" s="4">
-        <v>43.6</v>
+        <v>13.28928</v>
       </c>
       <c r="I284" s="7">
         <v>8.16</v>
@@ -13706,11 +13653,9 @@
         <v>42537</v>
       </c>
       <c r="C285" s="4">
-        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="D285" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E285" s="2">
@@ -13723,7 +13668,7 @@
         <v>1435</v>
       </c>
       <c r="H285" s="4">
-        <v>47</v>
+        <v>14.3256</v>
       </c>
       <c r="I285" s="7">
         <v>7.86</v>
@@ -13752,11 +13697,9 @@
         <v>42537</v>
       </c>
       <c r="C286" s="4">
-        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="D286" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E286" s="2">
@@ -13769,7 +13712,7 @@
         <v>1119</v>
       </c>
       <c r="H286" s="4">
-        <v>48</v>
+        <v>14.6304</v>
       </c>
       <c r="I286" s="7">
         <v>7.76</v>
@@ -13798,11 +13741,9 @@
         <v>42537</v>
       </c>
       <c r="C287" s="4">
-        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="D287" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E287" s="2">
@@ -13815,7 +13756,7 @@
         <v>72</v>
       </c>
       <c r="H287" s="4">
-        <v>48</v>
+        <v>14.6304</v>
       </c>
       <c r="I287" s="7">
         <v>7.96</v>
@@ -13844,11 +13785,9 @@
         <v>42537</v>
       </c>
       <c r="C288" s="4">
-        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="D288" s="4">
-        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="E288" s="2">
@@ -13861,7 +13800,7 @@
         <v>1227</v>
       </c>
       <c r="H288" s="4">
-        <v>38</v>
+        <v>11.5824</v>
       </c>
       <c r="I288" s="7">
         <v>7.66</v>
@@ -13880,6 +13819,1810 @@
       </c>
       <c r="N288" s="15">
         <v>-82.254831666666661</v>
+      </c>
+    </row>
+    <row r="289" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A289">
+        <v>501</v>
+      </c>
+      <c r="B289" s="3">
+        <v>42633</v>
+      </c>
+      <c r="C289" s="4">
+        <v>20</v>
+      </c>
+      <c r="D289" s="4">
+        <v>9</v>
+      </c>
+      <c r="E289" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F289" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G289" s="9">
+        <v>1032</v>
+      </c>
+      <c r="H289" s="5">
+        <v>5.1816000000000004</v>
+      </c>
+      <c r="I289" s="7">
+        <v>6.3</v>
+      </c>
+      <c r="J289" s="5">
+        <v>882.85702774841741</v>
+      </c>
+      <c r="K289" s="5">
+        <v>5561.9992748150298</v>
+      </c>
+      <c r="L289" s="5">
+        <v>0.55619992748150293</v>
+      </c>
+      <c r="M289" s="13">
+        <v>41.781185000000001</v>
+      </c>
+      <c r="N289" s="13">
+        <v>-83.354271999999995</v>
+      </c>
+    </row>
+    <row r="290" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A290">
+        <v>502</v>
+      </c>
+      <c r="B290" s="3">
+        <v>42633</v>
+      </c>
+      <c r="C290" s="4">
+        <v>20</v>
+      </c>
+      <c r="D290" s="4">
+        <v>9</v>
+      </c>
+      <c r="E290" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F290" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G290" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H290" s="5">
+        <v>7.62</v>
+      </c>
+      <c r="I290" s="7">
+        <v>6.8</v>
+      </c>
+      <c r="J290" s="5">
+        <v>851.27276485354287</v>
+      </c>
+      <c r="K290" s="5">
+        <v>5788.6548010040915</v>
+      </c>
+      <c r="L290" s="5">
+        <v>0.57886548010040917</v>
+      </c>
+      <c r="M290" s="13">
+        <v>41.781820000000003</v>
+      </c>
+      <c r="N290" s="13">
+        <v>-83.254251999999994</v>
+      </c>
+    </row>
+    <row r="291" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A291">
+        <v>503</v>
+      </c>
+      <c r="B291" s="3">
+        <v>42633</v>
+      </c>
+      <c r="C291" s="4">
+        <v>20</v>
+      </c>
+      <c r="D291" s="4">
+        <v>9</v>
+      </c>
+      <c r="E291" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F291" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G291" s="9">
+        <v>1144</v>
+      </c>
+      <c r="H291" s="5">
+        <v>7.62</v>
+      </c>
+      <c r="I291" s="7">
+        <v>6.5</v>
+      </c>
+      <c r="J291" s="5">
+        <v>890.7385915677088</v>
+      </c>
+      <c r="K291" s="5">
+        <v>5789.8008451901069</v>
+      </c>
+      <c r="L291" s="5">
+        <v>0.57898008451901073</v>
+      </c>
+      <c r="M291" s="13">
+        <v>41.885506999999997</v>
+      </c>
+      <c r="N291" s="13">
+        <v>-83.244820000000004</v>
+      </c>
+    </row>
+    <row r="292" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A292">
+        <v>504</v>
+      </c>
+      <c r="B292" s="3">
+        <v>42632</v>
+      </c>
+      <c r="C292" s="4">
+        <v>19</v>
+      </c>
+      <c r="D292" s="4">
+        <v>9</v>
+      </c>
+      <c r="E292" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F292" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G292" s="9">
+        <v>1449</v>
+      </c>
+      <c r="H292" s="5">
+        <v>7.7724000000000002</v>
+      </c>
+      <c r="I292" s="7">
+        <v>7.2</v>
+      </c>
+      <c r="J292" s="5">
+        <v>1131.5687210197505</v>
+      </c>
+      <c r="K292" s="5">
+        <v>8147.2947913422031</v>
+      </c>
+      <c r="L292" s="5">
+        <v>0.81472947913422034</v>
+      </c>
+      <c r="M292" s="13">
+        <v>41.683883000000002</v>
+      </c>
+      <c r="N292" s="13">
+        <v>-83.153064999999998</v>
+      </c>
+    </row>
+    <row r="293" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A293">
+        <v>505</v>
+      </c>
+      <c r="B293" s="3">
+        <v>42632</v>
+      </c>
+      <c r="C293" s="4">
+        <v>19</v>
+      </c>
+      <c r="D293" s="4">
+        <v>9</v>
+      </c>
+      <c r="E293" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F293" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G293" s="9">
+        <v>1541</v>
+      </c>
+      <c r="H293" s="5">
+        <v>8.2295999999999996</v>
+      </c>
+      <c r="I293" s="7">
+        <v>6.7</v>
+      </c>
+      <c r="J293" s="5">
+        <v>916.79532329564586</v>
+      </c>
+      <c r="K293" s="5">
+        <v>6142.5286660808279</v>
+      </c>
+      <c r="L293" s="5">
+        <v>0.61425286660808276</v>
+      </c>
+      <c r="M293" s="13">
+        <v>41.782767</v>
+      </c>
+      <c r="N293" s="13">
+        <v>-83.144486999999998</v>
+      </c>
+    </row>
+    <row r="294" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A294">
+        <v>506</v>
+      </c>
+      <c r="B294" s="3">
+        <v>42633</v>
+      </c>
+      <c r="C294" s="4">
+        <v>20</v>
+      </c>
+      <c r="D294" s="4">
+        <v>9</v>
+      </c>
+      <c r="E294" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F294" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G294" s="9">
+        <v>1229</v>
+      </c>
+      <c r="H294" s="5">
+        <v>9.1440000000000001</v>
+      </c>
+      <c r="I294" s="7">
+        <v>6.7</v>
+      </c>
+      <c r="J294" s="5">
+        <v>829.73843674608815</v>
+      </c>
+      <c r="K294" s="5">
+        <v>5559.2475261987911</v>
+      </c>
+      <c r="L294" s="5">
+        <v>0.55592475261987906</v>
+      </c>
+      <c r="M294" s="13">
+        <v>41.883198</v>
+      </c>
+      <c r="N294" s="13">
+        <v>-83.148747</v>
+      </c>
+    </row>
+    <row r="295" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A295">
+        <v>507</v>
+      </c>
+      <c r="B295" s="3">
+        <v>42633</v>
+      </c>
+      <c r="C295" s="4">
+        <v>20</v>
+      </c>
+      <c r="D295" s="4">
+        <v>9</v>
+      </c>
+      <c r="E295" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F295" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G295" s="9">
+        <v>1326</v>
+      </c>
+      <c r="H295" s="5">
+        <v>7.2237600000000004</v>
+      </c>
+      <c r="I295" s="7">
+        <v>6.6</v>
+      </c>
+      <c r="J295" s="5">
+        <v>910.17437634595603</v>
+      </c>
+      <c r="K295" s="5">
+        <v>6007.1508838833097</v>
+      </c>
+      <c r="L295" s="5">
+        <v>0.60071508838833099</v>
+      </c>
+      <c r="M295" s="13">
+        <v>41.980077000000001</v>
+      </c>
+      <c r="N295" s="13">
+        <v>-83.111172999999994</v>
+      </c>
+    </row>
+    <row r="296" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A296">
+        <v>508</v>
+      </c>
+      <c r="B296" s="3">
+        <v>42632</v>
+      </c>
+      <c r="C296" s="4">
+        <v>19</v>
+      </c>
+      <c r="D296" s="4">
+        <v>9</v>
+      </c>
+      <c r="E296" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F296" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G296" s="9">
+        <v>1351</v>
+      </c>
+      <c r="H296" s="5">
+        <v>8.5343999999999998</v>
+      </c>
+      <c r="I296" s="7">
+        <v>7.3</v>
+      </c>
+      <c r="J296" s="5">
+        <v>896.36565843881192</v>
+      </c>
+      <c r="K296" s="5">
+        <v>6543.4693066033269</v>
+      </c>
+      <c r="L296" s="5">
+        <v>0.65434693066033267</v>
+      </c>
+      <c r="M296" s="13">
+        <v>41.682792999999997</v>
+      </c>
+      <c r="N296" s="13">
+        <v>-83.044593000000006</v>
+      </c>
+    </row>
+    <row r="297" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A297">
+        <v>509</v>
+      </c>
+      <c r="B297" s="3">
+        <v>42632</v>
+      </c>
+      <c r="C297" s="4">
+        <v>19</v>
+      </c>
+      <c r="D297" s="4">
+        <v>9</v>
+      </c>
+      <c r="E297" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F297" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G297" s="9">
+        <v>1628</v>
+      </c>
+      <c r="H297" s="5">
+        <v>9.7536000000000005</v>
+      </c>
+      <c r="I297" s="7">
+        <v>7.2</v>
+      </c>
+      <c r="J297" s="5">
+        <v>937.1492883571691</v>
+      </c>
+      <c r="K297" s="5">
+        <v>6747.4748761716173</v>
+      </c>
+      <c r="L297" s="5">
+        <v>0.67474748761716175</v>
+      </c>
+      <c r="M297" s="13">
+        <v>41.780907999999997</v>
+      </c>
+      <c r="N297" s="13">
+        <v>-83.041152999999994</v>
+      </c>
+    </row>
+    <row r="298" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A298">
+        <v>510</v>
+      </c>
+      <c r="B298" s="3">
+        <v>42633</v>
+      </c>
+      <c r="C298" s="4">
+        <v>20</v>
+      </c>
+      <c r="D298" s="4">
+        <v>9</v>
+      </c>
+      <c r="E298" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F298" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G298" s="9">
+        <v>1501</v>
+      </c>
+      <c r="H298" s="5">
+        <v>9.7536000000000005</v>
+      </c>
+      <c r="I298" s="7">
+        <v>6.8</v>
+      </c>
+      <c r="J298" s="5">
+        <v>913.24751106830433</v>
+      </c>
+      <c r="K298" s="5">
+        <v>6210.0830752644697</v>
+      </c>
+      <c r="L298" s="5">
+        <v>0.62100830752644698</v>
+      </c>
+      <c r="M298" s="13">
+        <v>41.878704999999997</v>
+      </c>
+      <c r="N298" s="13">
+        <v>-83.043468000000004</v>
+      </c>
+    </row>
+    <row r="299" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A299">
+        <v>511</v>
+      </c>
+      <c r="B299" s="3">
+        <v>42633</v>
+      </c>
+      <c r="C299" s="4">
+        <v>20</v>
+      </c>
+      <c r="D299" s="4">
+        <v>9</v>
+      </c>
+      <c r="E299" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F299" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G299" s="9">
+        <v>1405</v>
+      </c>
+      <c r="H299" s="5">
+        <v>8.2295999999999996</v>
+      </c>
+      <c r="I299" s="7">
+        <v>6.9</v>
+      </c>
+      <c r="J299" s="5">
+        <v>936.77218888904997</v>
+      </c>
+      <c r="K299" s="5">
+        <v>6463.7281033344452</v>
+      </c>
+      <c r="L299" s="5">
+        <v>0.64637281033344451</v>
+      </c>
+      <c r="M299" s="13">
+        <v>41.980103</v>
+      </c>
+      <c r="N299" s="13">
+        <v>-83.041780000000003</v>
+      </c>
+    </row>
+    <row r="300" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A300">
+        <v>512</v>
+      </c>
+      <c r="B300" s="3">
+        <v>42632</v>
+      </c>
+      <c r="C300" s="4">
+        <v>19</v>
+      </c>
+      <c r="D300" s="4">
+        <v>9</v>
+      </c>
+      <c r="E300" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F300" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G300" s="9">
+        <v>1155</v>
+      </c>
+      <c r="H300" s="5">
+        <v>7.3151999999999999</v>
+      </c>
+      <c r="I300" s="7">
+        <v>7.3</v>
+      </c>
+      <c r="J300" s="5">
+        <v>887.82882160585825</v>
+      </c>
+      <c r="K300" s="5">
+        <v>6481.1503977227649</v>
+      </c>
+      <c r="L300" s="5">
+        <v>0.64811503977227647</v>
+      </c>
+      <c r="M300" s="13">
+        <v>41.568227999999998</v>
+      </c>
+      <c r="N300" s="13">
+        <v>-82.950687000000002</v>
+      </c>
+    </row>
+    <row r="301" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A301">
+        <v>513</v>
+      </c>
+      <c r="B301" s="3">
+        <v>42632</v>
+      </c>
+      <c r="C301" s="4">
+        <v>19</v>
+      </c>
+      <c r="D301" s="4">
+        <v>9</v>
+      </c>
+      <c r="E301" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F301" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G301" s="9">
+        <v>1259</v>
+      </c>
+      <c r="H301" s="5">
+        <v>9.7536000000000005</v>
+      </c>
+      <c r="I301" s="7">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="J301" s="5">
+        <v>1009.8199990061299</v>
+      </c>
+      <c r="K301" s="5">
+        <v>8381.5059917508788</v>
+      </c>
+      <c r="L301" s="5">
+        <v>0.83815059917508783</v>
+      </c>
+      <c r="M301" s="13">
+        <v>41.684263000000001</v>
+      </c>
+      <c r="N301" s="13">
+        <v>-82.946577000000005</v>
+      </c>
+    </row>
+    <row r="302" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A302">
+        <v>514</v>
+      </c>
+      <c r="B302" s="3">
+        <v>42632</v>
+      </c>
+      <c r="C302" s="4">
+        <v>19</v>
+      </c>
+      <c r="D302" s="4">
+        <v>9</v>
+      </c>
+      <c r="E302" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F302" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G302" s="9">
+        <v>1713</v>
+      </c>
+      <c r="H302" s="5">
+        <v>10.363200000000001</v>
+      </c>
+      <c r="I302" s="7">
+        <v>7.2</v>
+      </c>
+      <c r="J302" s="5">
+        <v>902.74350477362282</v>
+      </c>
+      <c r="K302" s="5">
+        <v>6499.7532343700841</v>
+      </c>
+      <c r="L302" s="5">
+        <v>0.64997532343700837</v>
+      </c>
+      <c r="M302" s="13">
+        <v>41.763328000000001</v>
+      </c>
+      <c r="N302" s="13">
+        <v>-82.943852000000007</v>
+      </c>
+    </row>
+    <row r="303" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A303">
+        <v>515</v>
+      </c>
+      <c r="B303" s="3">
+        <v>42633</v>
+      </c>
+      <c r="C303" s="4">
+        <v>20</v>
+      </c>
+      <c r="D303" s="4">
+        <v>9</v>
+      </c>
+      <c r="E303" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F303" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G303" s="9">
+        <v>1544</v>
+      </c>
+      <c r="H303" s="5">
+        <v>10.667999999999999</v>
+      </c>
+      <c r="I303" s="7">
+        <v>7.5</v>
+      </c>
+      <c r="J303" s="5">
+        <v>796.74828493340237</v>
+      </c>
+      <c r="K303" s="5">
+        <v>5975.6121370005176</v>
+      </c>
+      <c r="L303" s="5">
+        <v>0.59756121370005177</v>
+      </c>
+      <c r="M303" s="13">
+        <v>41.882772000000003</v>
+      </c>
+      <c r="N303" s="13">
+        <v>-82.944986999999998</v>
+      </c>
+    </row>
+    <row r="304" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A304">
+        <v>516</v>
+      </c>
+      <c r="B304" s="3">
+        <v>42633</v>
+      </c>
+      <c r="C304" s="4">
+        <v>20</v>
+      </c>
+      <c r="D304" s="4">
+        <v>9</v>
+      </c>
+      <c r="E304" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F304" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G304" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H304" s="5">
+        <v>9.7536000000000005</v>
+      </c>
+      <c r="I304" s="7">
+        <v>7.4</v>
+      </c>
+      <c r="J304" s="5">
+        <v>817.26711328048441</v>
+      </c>
+      <c r="K304" s="5">
+        <v>6047.7766382755854</v>
+      </c>
+      <c r="L304" s="5">
+        <v>0.60477766382755849</v>
+      </c>
+      <c r="M304" s="13">
+        <v>41.662196666666667</v>
+      </c>
+      <c r="N304" s="13">
+        <v>-82.856520000000003</v>
+      </c>
+    </row>
+    <row r="305" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A305">
+        <v>517</v>
+      </c>
+      <c r="B305" s="3">
+        <v>42632</v>
+      </c>
+      <c r="C305" s="4">
+        <v>19</v>
+      </c>
+      <c r="D305" s="4">
+        <v>9</v>
+      </c>
+      <c r="E305" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F305" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G305" s="9">
+        <v>1758</v>
+      </c>
+      <c r="H305" s="5">
+        <v>10.363200000000001</v>
+      </c>
+      <c r="I305" s="7">
+        <v>7.3</v>
+      </c>
+      <c r="J305" s="5">
+        <v>908.75595731995463</v>
+      </c>
+      <c r="K305" s="5">
+        <v>6633.9184884356682</v>
+      </c>
+      <c r="L305" s="5">
+        <v>0.66339184884356683</v>
+      </c>
+      <c r="M305" s="13">
+        <v>41.757691999999999</v>
+      </c>
+      <c r="N305" s="13">
+        <v>-82.851652000000001</v>
+      </c>
+    </row>
+    <row r="306" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A306">
+        <v>518</v>
+      </c>
+      <c r="B306" s="3">
+        <v>42633</v>
+      </c>
+      <c r="C306" s="4">
+        <v>20</v>
+      </c>
+      <c r="D306" s="4">
+        <v>9</v>
+      </c>
+      <c r="E306" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F306" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G306" s="9">
+        <v>1737</v>
+      </c>
+      <c r="H306" s="5">
+        <v>11.30808</v>
+      </c>
+      <c r="I306" s="7">
+        <v>7.3</v>
+      </c>
+      <c r="J306" s="5">
+        <v>930.7345353113152</v>
+      </c>
+      <c r="K306" s="5">
+        <v>6794.3621077726011</v>
+      </c>
+      <c r="L306" s="5">
+        <v>0.67943621077726013</v>
+      </c>
+      <c r="M306" s="13">
+        <v>41.859223</v>
+      </c>
+      <c r="N306" s="13">
+        <v>-82.853821999999994</v>
+      </c>
+    </row>
+    <row r="307" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A307">
+        <v>519</v>
+      </c>
+      <c r="B307" s="3">
+        <v>42633</v>
+      </c>
+      <c r="C307" s="4">
+        <v>20</v>
+      </c>
+      <c r="D307" s="4">
+        <v>9</v>
+      </c>
+      <c r="E307" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F307" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G307" s="9">
+        <v>1642</v>
+      </c>
+      <c r="H307" s="5">
+        <v>10.454639999999998</v>
+      </c>
+      <c r="I307" s="7">
+        <v>6.8</v>
+      </c>
+      <c r="J307" s="5">
+        <v>834.54858804347259</v>
+      </c>
+      <c r="K307" s="5">
+        <v>5674.9303986956138</v>
+      </c>
+      <c r="L307" s="5">
+        <v>0.56749303986956134</v>
+      </c>
+      <c r="M307" s="13">
+        <v>41.958599999999997</v>
+      </c>
+      <c r="N307" s="13">
+        <v>-82.848212000000004</v>
+      </c>
+    </row>
+    <row r="308" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A308">
+        <v>520</v>
+      </c>
+      <c r="B308" s="3">
+        <v>42632</v>
+      </c>
+      <c r="C308" s="4">
+        <v>19</v>
+      </c>
+      <c r="D308" s="4">
+        <v>9</v>
+      </c>
+      <c r="E308" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F308" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G308" s="9">
+        <v>1041</v>
+      </c>
+      <c r="H308" s="5">
+        <v>8.2295999999999996</v>
+      </c>
+      <c r="I308" s="7">
+        <v>7.8</v>
+      </c>
+      <c r="J308" s="5">
+        <v>945.83152385005803</v>
+      </c>
+      <c r="K308" s="5">
+        <v>7377.4858860304521</v>
+      </c>
+      <c r="L308" s="5">
+        <v>0.73774858860304526</v>
+      </c>
+      <c r="M308" s="13">
+        <v>41.565303</v>
+      </c>
+      <c r="N308" s="13">
+        <v>-82.753962999999999</v>
+      </c>
+    </row>
+    <row r="309" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A309">
+        <v>521</v>
+      </c>
+      <c r="B309" s="3">
+        <v>42634</v>
+      </c>
+      <c r="C309" s="4">
+        <v>21</v>
+      </c>
+      <c r="D309" s="4">
+        <v>9</v>
+      </c>
+      <c r="E309" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F309" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G309" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H309" s="5">
+        <v>10.149839999999999</v>
+      </c>
+      <c r="I309" s="7">
+        <v>7</v>
+      </c>
+      <c r="J309" s="5">
+        <v>872.02877875039906</v>
+      </c>
+      <c r="K309" s="5">
+        <v>6104.201451252793</v>
+      </c>
+      <c r="L309" s="5">
+        <v>0.61042014512527931</v>
+      </c>
+      <c r="M309" s="13">
+        <v>41.682879999999997</v>
+      </c>
+      <c r="N309" s="13">
+        <v>-82.755172000000002</v>
+      </c>
+    </row>
+    <row r="310" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A310">
+        <v>522</v>
+      </c>
+      <c r="B310" s="3">
+        <v>42634</v>
+      </c>
+      <c r="C310" s="4">
+        <v>21</v>
+      </c>
+      <c r="D310" s="4">
+        <v>9</v>
+      </c>
+      <c r="E310" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F310" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G310" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="H310" s="5">
+        <v>9.7536000000000005</v>
+      </c>
+      <c r="I310" s="7">
+        <v>7.3</v>
+      </c>
+      <c r="J310" s="5">
+        <v>939.41988894278302</v>
+      </c>
+      <c r="K310" s="5">
+        <v>6857.765189282316</v>
+      </c>
+      <c r="L310" s="5">
+        <v>0.68577651892823155</v>
+      </c>
+      <c r="M310" s="13">
+        <v>41.785870000000003</v>
+      </c>
+      <c r="N310" s="13">
+        <v>-82.752619999999993</v>
+      </c>
+    </row>
+    <row r="311" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A311">
+        <v>523</v>
+      </c>
+      <c r="B311" s="3">
+        <v>42634</v>
+      </c>
+      <c r="C311" s="4">
+        <v>21</v>
+      </c>
+      <c r="D311" s="4">
+        <v>9</v>
+      </c>
+      <c r="E311" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F311" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G311" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="H311" s="5">
+        <v>11.643360000000001</v>
+      </c>
+      <c r="I311" s="7">
+        <v>6.9</v>
+      </c>
+      <c r="J311" s="5">
+        <v>866.35450978300003</v>
+      </c>
+      <c r="K311" s="5">
+        <v>5977.8461175027005</v>
+      </c>
+      <c r="L311" s="5">
+        <v>0.59778461175027009</v>
+      </c>
+      <c r="M311" s="13">
+        <v>41.87171</v>
+      </c>
+      <c r="N311" s="13">
+        <v>-82.753226999999995</v>
+      </c>
+    </row>
+    <row r="312" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A312">
+        <v>524</v>
+      </c>
+      <c r="B312" s="3">
+        <v>42634</v>
+      </c>
+      <c r="C312" s="4">
+        <v>21</v>
+      </c>
+      <c r="D312" s="4">
+        <v>9</v>
+      </c>
+      <c r="E312" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F312" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G312" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="H312" s="5">
+        <v>10.881360000000001</v>
+      </c>
+      <c r="I312" s="7">
+        <v>7.3</v>
+      </c>
+      <c r="J312" s="5">
+        <v>891.94977226670687</v>
+      </c>
+      <c r="K312" s="5">
+        <v>6511.2333375469598</v>
+      </c>
+      <c r="L312" s="5">
+        <v>0.651123333754696</v>
+      </c>
+      <c r="M312" s="13">
+        <v>41.964632000000002</v>
+      </c>
+      <c r="N312" s="13">
+        <v>-82.744770000000003</v>
+      </c>
+    </row>
+    <row r="313" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A313">
+        <v>525</v>
+      </c>
+      <c r="B313" s="3">
+        <v>42632</v>
+      </c>
+      <c r="C313" s="4">
+        <v>19</v>
+      </c>
+      <c r="D313" s="4">
+        <v>9</v>
+      </c>
+      <c r="E313" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F313" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G313" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="H313" s="5">
+        <v>12.801600000000001</v>
+      </c>
+      <c r="I313" s="7">
+        <v>7.8</v>
+      </c>
+      <c r="J313" s="5">
+        <v>884.35392866840368</v>
+      </c>
+      <c r="K313" s="5">
+        <v>6897.9606436135482</v>
+      </c>
+      <c r="L313" s="5">
+        <v>0.68979606436135477</v>
+      </c>
+      <c r="M313" s="13">
+        <v>41.561546999999997</v>
+      </c>
+      <c r="N313" s="13">
+        <v>-82.644532999999996</v>
+      </c>
+    </row>
+    <row r="314" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A314">
+        <v>526</v>
+      </c>
+      <c r="B314" s="3">
+        <v>42635</v>
+      </c>
+      <c r="C314" s="4">
+        <v>22</v>
+      </c>
+      <c r="D314" s="4">
+        <v>9</v>
+      </c>
+      <c r="E314" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F314" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G314" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H314" s="5">
+        <v>11.064239999999998</v>
+      </c>
+      <c r="I314" s="7">
+        <v>7.4</v>
+      </c>
+      <c r="J314" s="5">
+        <v>893.41509550638727</v>
+      </c>
+      <c r="K314" s="5">
+        <v>6611.2717067472659</v>
+      </c>
+      <c r="L314" s="5">
+        <v>0.66112717067472659</v>
+      </c>
+      <c r="M314" s="13">
+        <v>41.678739999999998</v>
+      </c>
+      <c r="N314" s="13">
+        <v>-82.646027000000004</v>
+      </c>
+    </row>
+    <row r="315" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A315">
+        <v>527</v>
+      </c>
+      <c r="B315" s="3">
+        <v>42634</v>
+      </c>
+      <c r="C315" s="4">
+        <v>21</v>
+      </c>
+      <c r="D315" s="4">
+        <v>9</v>
+      </c>
+      <c r="E315" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F315" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G315" s="9">
+        <v>1208</v>
+      </c>
+      <c r="H315" s="5">
+        <v>11.00328</v>
+      </c>
+      <c r="I315" s="7">
+        <v>7</v>
+      </c>
+      <c r="J315" s="5">
+        <v>932.51802380938227</v>
+      </c>
+      <c r="K315" s="5">
+        <v>6527.6261666656756</v>
+      </c>
+      <c r="L315" s="5">
+        <v>0.65276261666656754</v>
+      </c>
+      <c r="M315" s="13">
+        <v>41.862907</v>
+      </c>
+      <c r="N315" s="13">
+        <v>-82.643167000000005</v>
+      </c>
+    </row>
+    <row r="316" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A316">
+        <v>528</v>
+      </c>
+      <c r="B316" s="3">
+        <v>42634</v>
+      </c>
+      <c r="C316" s="4">
+        <v>21</v>
+      </c>
+      <c r="D316" s="4">
+        <v>9</v>
+      </c>
+      <c r="E316" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F316" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G316" s="9">
+        <v>1112</v>
+      </c>
+      <c r="H316" s="5">
+        <v>10.667999999999999</v>
+      </c>
+      <c r="I316" s="7">
+        <v>7.2</v>
+      </c>
+      <c r="J316" s="5">
+        <v>867.02901707366482</v>
+      </c>
+      <c r="K316" s="5">
+        <v>6242.6089229303871</v>
+      </c>
+      <c r="L316" s="5">
+        <v>0.62426089229303872</v>
+      </c>
+      <c r="M316" s="13">
+        <v>41.975673</v>
+      </c>
+      <c r="N316" s="13">
+        <v>-82.650503</v>
+      </c>
+    </row>
+    <row r="317" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A317">
+        <v>529</v>
+      </c>
+      <c r="B317" s="3">
+        <v>42632</v>
+      </c>
+      <c r="C317" s="4">
+        <v>19</v>
+      </c>
+      <c r="D317" s="4">
+        <v>9</v>
+      </c>
+      <c r="E317" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F317" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G317" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H317" s="5">
+        <v>12.801600000000001</v>
+      </c>
+      <c r="I317" s="7">
+        <v>7.3</v>
+      </c>
+      <c r="J317" s="5">
+        <v>897.66698374323823</v>
+      </c>
+      <c r="K317" s="5">
+        <v>6552.9689813256391</v>
+      </c>
+      <c r="L317" s="5">
+        <v>0.65529689813256387</v>
+      </c>
+      <c r="M317" s="13">
+        <v>41.462743000000003</v>
+      </c>
+      <c r="N317" s="13">
+        <v>-82.541228000000004</v>
+      </c>
+    </row>
+    <row r="318" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A318">
+        <v>530</v>
+      </c>
+      <c r="B318" s="3">
+        <v>42632</v>
+      </c>
+      <c r="C318" s="4">
+        <v>19</v>
+      </c>
+      <c r="D318" s="4">
+        <v>9</v>
+      </c>
+      <c r="E318" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F318" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G318" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H318" s="5">
+        <v>13.411199999999999</v>
+      </c>
+      <c r="I318" s="7">
+        <v>8</v>
+      </c>
+      <c r="J318" s="5">
+        <v>913.68827528118209</v>
+      </c>
+      <c r="K318" s="5">
+        <v>7309.5062022494567</v>
+      </c>
+      <c r="L318" s="5">
+        <v>0.73095062022494572</v>
+      </c>
+      <c r="M318" s="13">
+        <v>41.563442000000002</v>
+      </c>
+      <c r="N318" s="13">
+        <v>-82.542862999999997</v>
+      </c>
+    </row>
+    <row r="319" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A319">
+        <v>531</v>
+      </c>
+      <c r="B319" s="3">
+        <v>42634</v>
+      </c>
+      <c r="C319" s="4">
+        <v>21</v>
+      </c>
+      <c r="D319" s="4">
+        <v>9</v>
+      </c>
+      <c r="E319" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F319" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G319" s="9">
+        <v>1728</v>
+      </c>
+      <c r="H319" s="5">
+        <v>12.801600000000001</v>
+      </c>
+      <c r="I319" s="7">
+        <v>7.4</v>
+      </c>
+      <c r="J319" s="5">
+        <v>870.329222667718</v>
+      </c>
+      <c r="K319" s="5">
+        <v>6440.4362477411132</v>
+      </c>
+      <c r="L319" s="5">
+        <v>0.64404362477411137</v>
+      </c>
+      <c r="M319" s="13">
+        <v>41.664152000000001</v>
+      </c>
+      <c r="N319" s="13">
+        <v>-82.560578000000007</v>
+      </c>
+    </row>
+    <row r="320" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A320">
+        <v>532</v>
+      </c>
+      <c r="B320" s="3">
+        <v>42634</v>
+      </c>
+      <c r="C320" s="4">
+        <v>21</v>
+      </c>
+      <c r="D320" s="4">
+        <v>9</v>
+      </c>
+      <c r="E320" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F320" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G320" s="9">
+        <v>1359</v>
+      </c>
+      <c r="H320" s="5">
+        <v>11.00328</v>
+      </c>
+      <c r="I320" s="7">
+        <v>7.5</v>
+      </c>
+      <c r="J320" s="5">
+        <v>889.47901870632154</v>
+      </c>
+      <c r="K320" s="5">
+        <v>6671.0926402974119</v>
+      </c>
+      <c r="L320" s="5">
+        <v>0.66710926402974113</v>
+      </c>
+      <c r="M320" s="13">
+        <v>41.779085000000002</v>
+      </c>
+      <c r="N320" s="13">
+        <v>-82.545946999999998</v>
+      </c>
+    </row>
+    <row r="321" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A321">
+        <v>533</v>
+      </c>
+      <c r="B321" s="3">
+        <v>42634</v>
+      </c>
+      <c r="C321" s="4">
+        <v>21</v>
+      </c>
+      <c r="D321" s="4">
+        <v>9</v>
+      </c>
+      <c r="E321" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F321" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G321" s="9">
+        <v>1257</v>
+      </c>
+      <c r="H321" s="5">
+        <v>12.192</v>
+      </c>
+      <c r="I321" s="7">
+        <v>7.3</v>
+      </c>
+      <c r="J321" s="5">
+        <v>901.67368965522189</v>
+      </c>
+      <c r="K321" s="5">
+        <v>6582.2179344831193</v>
+      </c>
+      <c r="L321" s="5">
+        <v>0.65822179344831189</v>
+      </c>
+      <c r="M321" s="13">
+        <v>41.861781999999998</v>
+      </c>
+      <c r="N321" s="13">
+        <v>-82.530923000000001</v>
+      </c>
+    </row>
+    <row r="322" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A322">
+        <v>534</v>
+      </c>
+      <c r="B322" s="3">
+        <v>42635</v>
+      </c>
+      <c r="C322" s="4">
+        <v>22</v>
+      </c>
+      <c r="D322" s="4">
+        <v>9</v>
+      </c>
+      <c r="E322" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F322" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G322" s="9">
+        <v>1510</v>
+      </c>
+      <c r="H322" s="5">
+        <v>13.014960000000002</v>
+      </c>
+      <c r="I322" s="7">
+        <v>7.7</v>
+      </c>
+      <c r="J322" s="5">
+        <v>899.19575155744849</v>
+      </c>
+      <c r="K322" s="5">
+        <v>6923.8072869923535</v>
+      </c>
+      <c r="L322" s="5">
+        <v>0.69238072869923539</v>
+      </c>
+      <c r="M322" s="13">
+        <v>41.456299999999999</v>
+      </c>
+      <c r="N322" s="13">
+        <v>-82.456393000000006</v>
+      </c>
+    </row>
+    <row r="323" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A323">
+        <v>535</v>
+      </c>
+      <c r="B323" s="3">
+        <v>42635</v>
+      </c>
+      <c r="C323" s="4">
+        <v>22</v>
+      </c>
+      <c r="D323" s="4">
+        <v>9</v>
+      </c>
+      <c r="E323" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F323" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G323" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="H323" s="5">
+        <v>14.6304</v>
+      </c>
+      <c r="I323" s="7">
+        <v>7.7</v>
+      </c>
+      <c r="J323" s="5">
+        <v>824.63635010184362</v>
+      </c>
+      <c r="K323" s="5">
+        <v>6349.6998957841961</v>
+      </c>
+      <c r="L323" s="5">
+        <v>0.63496998957841966</v>
+      </c>
+      <c r="M323" s="13">
+        <v>41.579970000000003</v>
+      </c>
+      <c r="N323" s="13">
+        <v>-82.443700000000007</v>
+      </c>
+    </row>
+    <row r="324" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A324">
+        <v>536</v>
+      </c>
+      <c r="B324" s="3">
+        <v>42634</v>
+      </c>
+      <c r="C324" s="4">
+        <v>21</v>
+      </c>
+      <c r="D324" s="4">
+        <v>9</v>
+      </c>
+      <c r="E324" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F324" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G324" s="9">
+        <v>1635</v>
+      </c>
+      <c r="H324" s="5">
+        <v>14.081759999999999</v>
+      </c>
+      <c r="I324" s="7">
+        <v>7.8</v>
+      </c>
+      <c r="J324" s="5">
+        <v>984.14603245850287</v>
+      </c>
+      <c r="K324" s="5">
+        <v>7676.3390531763225</v>
+      </c>
+      <c r="L324" s="5">
+        <v>0.7676339053176322</v>
+      </c>
+      <c r="M324" s="13">
+        <v>41.662909999999997</v>
+      </c>
+      <c r="N324" s="13">
+        <v>-82.459447999999995</v>
+      </c>
+    </row>
+    <row r="325" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A325">
+        <v>537</v>
+      </c>
+      <c r="B325" s="3">
+        <v>42634</v>
+      </c>
+      <c r="C325" s="4">
+        <v>21</v>
+      </c>
+      <c r="D325" s="4">
+        <v>9</v>
+      </c>
+      <c r="E325" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F325" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G325" s="9">
+        <v>1446</v>
+      </c>
+      <c r="H325" s="5">
+        <v>13.045439999999999</v>
+      </c>
+      <c r="I325" s="7">
+        <v>7.1</v>
+      </c>
+      <c r="J325" s="5">
+        <v>845.13776566515389</v>
+      </c>
+      <c r="K325" s="5">
+        <v>6000.4781362225922</v>
+      </c>
+      <c r="L325" s="5">
+        <v>0.60004781362225923</v>
+      </c>
+      <c r="M325" s="13">
+        <v>41.775379999999998</v>
+      </c>
+      <c r="N325" s="13">
+        <v>-82.446560000000005</v>
+      </c>
+    </row>
+    <row r="326" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A326">
+        <v>538</v>
+      </c>
+      <c r="B326" s="3">
+        <v>42635</v>
+      </c>
+      <c r="C326" s="4">
+        <v>22</v>
+      </c>
+      <c r="D326" s="4">
+        <v>9</v>
+      </c>
+      <c r="E326" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F326" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G326" s="9">
+        <v>1314</v>
+      </c>
+      <c r="H326" s="5">
+        <v>13.929360000000001</v>
+      </c>
+      <c r="I326" s="7">
+        <v>8</v>
+      </c>
+      <c r="J326" s="5">
+        <v>911.98672725862036</v>
+      </c>
+      <c r="K326" s="5">
+        <v>7295.8938180689629</v>
+      </c>
+      <c r="L326" s="5">
+        <v>0.72958938180689625</v>
+      </c>
+      <c r="M326" s="13">
+        <v>41.480530000000002</v>
+      </c>
+      <c r="N326" s="13">
+        <v>-82.356482999999997</v>
+      </c>
+    </row>
+    <row r="327" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A327">
+        <v>539</v>
+      </c>
+      <c r="B327" s="3">
+        <v>42635</v>
+      </c>
+      <c r="C327" s="4">
+        <v>22</v>
+      </c>
+      <c r="D327" s="4">
+        <v>9</v>
+      </c>
+      <c r="E327" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F327" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G327" s="9">
+        <v>1003</v>
+      </c>
+      <c r="H327" s="5">
+        <v>14.3256</v>
+      </c>
+      <c r="I327" s="7">
+        <v>8.4</v>
+      </c>
+      <c r="J327" s="5">
+        <v>876.28230990896122</v>
+      </c>
+      <c r="K327" s="5">
+        <v>7360.7714032352742</v>
+      </c>
+      <c r="L327" s="5">
+        <v>0.73607714032352745</v>
+      </c>
+      <c r="M327" s="13">
+        <v>41.577888000000002</v>
+      </c>
+      <c r="N327" s="13">
+        <v>-82.347243000000006</v>
+      </c>
+    </row>
+    <row r="328" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A328">
+        <v>540</v>
+      </c>
+      <c r="B328" s="3">
+        <v>42634</v>
+      </c>
+      <c r="C328" s="4">
+        <v>21</v>
+      </c>
+      <c r="D328" s="4">
+        <v>9</v>
+      </c>
+      <c r="E328" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F328" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G328" s="9">
+        <v>1550</v>
+      </c>
+      <c r="H328" s="5">
+        <v>14.05128</v>
+      </c>
+      <c r="I328" s="7">
+        <v>8</v>
+      </c>
+      <c r="J328" s="5">
+        <v>864.36959478181609</v>
+      </c>
+      <c r="K328" s="5">
+        <v>6914.9567582545287</v>
+      </c>
+      <c r="L328" s="5">
+        <v>0.6914956758254529</v>
+      </c>
+      <c r="M328" s="13">
+        <v>41.662734999999998</v>
+      </c>
+      <c r="N328" s="13">
+        <v>-82.357595000000003</v>
+      </c>
+    </row>
+    <row r="329" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A329">
+        <v>541</v>
+      </c>
+      <c r="B329" s="3">
+        <v>42635</v>
+      </c>
+      <c r="C329" s="4">
+        <v>22</v>
+      </c>
+      <c r="D329" s="4">
+        <v>9</v>
+      </c>
+      <c r="E329" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F329" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G329" s="9">
+        <v>1103</v>
+      </c>
+      <c r="H329" s="5">
+        <v>13.38072</v>
+      </c>
+      <c r="I329" s="7">
+        <v>7.7</v>
+      </c>
+      <c r="J329" s="5">
+        <v>972.43971440225289</v>
+      </c>
+      <c r="K329" s="5">
+        <v>7487.7858008973471</v>
+      </c>
+      <c r="L329" s="5">
+        <v>0.74877858008973475</v>
+      </c>
+      <c r="M329" s="13">
+        <v>41.479632000000002</v>
+      </c>
+      <c r="N329" s="13">
+        <v>-82.255072999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2017 trawl data update
Finally got GitHub Desktop back on my new machine... this updates 2017 data and some script edits for the shiny app.
</commit_message>
<xml_diff>
--- a/data_prep/WB_Effort.xlsx
+++ b/data_prep/WB_Effort.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Western Basin Forage\lebs-western-basin-app\data_prep\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="12705" yWindow="-15" windowWidth="12510" windowHeight="11805"/>
   </bookViews>
   <sheets>
     <sheet name="Effort" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="146">
   <si>
     <t>serial</t>
   </si>
@@ -263,14 +268,213 @@
   <si>
     <t>0918</t>
   </si>
+  <si>
+    <t>0743</t>
+  </si>
+  <si>
+    <t>0853</t>
+  </si>
+  <si>
+    <t>0955</t>
+  </si>
+  <si>
+    <t>1101</t>
+  </si>
+  <si>
+    <t>1230</t>
+  </si>
+  <si>
+    <t>1400</t>
+  </si>
+  <si>
+    <t>1506</t>
+  </si>
+  <si>
+    <t>1632</t>
+  </si>
+  <si>
+    <t>1748</t>
+  </si>
+  <si>
+    <t>1833</t>
+  </si>
+  <si>
+    <t>1923</t>
+  </si>
+  <si>
+    <t>0721</t>
+  </si>
+  <si>
+    <t>0828</t>
+  </si>
+  <si>
+    <t>1026</t>
+  </si>
+  <si>
+    <t>1125</t>
+  </si>
+  <si>
+    <t>1227</t>
+  </si>
+  <si>
+    <t>1318</t>
+  </si>
+  <si>
+    <t>1423</t>
+  </si>
+  <si>
+    <t>1524</t>
+  </si>
+  <si>
+    <t>1648</t>
+  </si>
+  <si>
+    <t>1759</t>
+  </si>
+  <si>
+    <t>0726</t>
+  </si>
+  <si>
+    <t>1052</t>
+  </si>
+  <si>
+    <t>1146</t>
+  </si>
+  <si>
+    <t>1238</t>
+  </si>
+  <si>
+    <t>1415</t>
+  </si>
+  <si>
+    <t>1530</t>
+  </si>
+  <si>
+    <t>1627</t>
+  </si>
+  <si>
+    <t>1722</t>
+  </si>
+  <si>
+    <t>1835</t>
+  </si>
+  <si>
+    <t>1927</t>
+  </si>
+  <si>
+    <t>0907</t>
+  </si>
+  <si>
+    <t>0957</t>
+  </si>
+  <si>
+    <t>1106</t>
+  </si>
+  <si>
+    <t>0754</t>
+  </si>
+  <si>
+    <t>1014</t>
+  </si>
+  <si>
+    <t>1114</t>
+  </si>
+  <si>
+    <t>1314</t>
+  </si>
+  <si>
+    <t>1458</t>
+  </si>
+  <si>
+    <t>1544</t>
+  </si>
+  <si>
+    <t>1725</t>
+  </si>
+  <si>
+    <t>1818</t>
+  </si>
+  <si>
+    <t>0739</t>
+  </si>
+  <si>
+    <t>0923</t>
+  </si>
+  <si>
+    <t>1029</t>
+  </si>
+  <si>
+    <t>1225</t>
+  </si>
+  <si>
+    <t>1310</t>
+  </si>
+  <si>
+    <t>1412</t>
+  </si>
+  <si>
+    <t>1459</t>
+  </si>
+  <si>
+    <t>1614</t>
+  </si>
+  <si>
+    <t>1708</t>
+  </si>
+  <si>
+    <t>0838</t>
+  </si>
+  <si>
+    <t>1028</t>
+  </si>
+  <si>
+    <t>1134</t>
+  </si>
+  <si>
+    <t>1222</t>
+  </si>
+  <si>
+    <t>1407</t>
+  </si>
+  <si>
+    <t>1457</t>
+  </si>
+  <si>
+    <t>1552</t>
+  </si>
+  <si>
+    <t>1639</t>
+  </si>
+  <si>
+    <t>1746</t>
+  </si>
+  <si>
+    <t>0909</t>
+  </si>
+  <si>
+    <t>0959</t>
+  </si>
+  <si>
+    <t>1127</t>
+  </si>
+  <si>
+    <t>1224</t>
+  </si>
+  <si>
+    <t>1328</t>
+  </si>
+  <si>
+    <t>1617</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="hhmm"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -314,7 +518,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -350,6 +554,16 @@
     </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -624,7 +838,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -632,18 +846,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N329"/>
+  <dimension ref="A1:N407"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A296" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G330" sqref="G330"/>
+      <pane ySplit="1" topLeftCell="A371" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A408" sqref="A408"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.140625" style="1" bestFit="1" customWidth="1"/>
@@ -15625,6 +15839,3438 @@
         <v>-82.255072999999996</v>
       </c>
     </row>
+    <row r="330" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A330">
+        <v>129</v>
+      </c>
+      <c r="B330" s="3">
+        <v>42905</v>
+      </c>
+      <c r="C330" s="4">
+        <v>19</v>
+      </c>
+      <c r="D330" s="4">
+        <v>6</v>
+      </c>
+      <c r="E330" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F330" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G330" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="H330" s="17">
+        <v>12.801600000000001</v>
+      </c>
+      <c r="I330" s="7">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="J330" s="5">
+        <v>1465.941726565879</v>
+      </c>
+      <c r="K330" s="5">
+        <v>12167.316330496797</v>
+      </c>
+      <c r="L330" s="5">
+        <v>1.2167316330496796</v>
+      </c>
+      <c r="M330" s="13">
+        <v>41.461081666666665</v>
+      </c>
+      <c r="N330" s="13">
+        <v>-82.547441666666671</v>
+      </c>
+    </row>
+    <row r="331" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A331">
+        <v>130</v>
+      </c>
+      <c r="B331" s="3">
+        <v>42905</v>
+      </c>
+      <c r="C331" s="4">
+        <v>19</v>
+      </c>
+      <c r="D331" s="4">
+        <v>6</v>
+      </c>
+      <c r="E331" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F331" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G331" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="H331" s="18">
+        <v>13.715999999999999</v>
+      </c>
+      <c r="I331" s="7">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="J331" s="5">
+        <v>911.22395174571682</v>
+      </c>
+      <c r="K331" s="5">
+        <v>7563.1587994894498</v>
+      </c>
+      <c r="L331" s="5">
+        <v>0.756315879948945</v>
+      </c>
+      <c r="M331" s="13">
+        <v>41.472296666666665</v>
+      </c>
+      <c r="N331" s="13">
+        <v>-82.531805000000006</v>
+      </c>
+    </row>
+    <row r="332" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A332">
+        <v>125</v>
+      </c>
+      <c r="B332" s="3">
+        <v>42905</v>
+      </c>
+      <c r="C332" s="4">
+        <v>19</v>
+      </c>
+      <c r="D332" s="4">
+        <v>6</v>
+      </c>
+      <c r="E332" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F332" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G332" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="H332" s="17">
+        <v>12.801600000000001</v>
+      </c>
+      <c r="I332" s="7">
+        <v>8.4</v>
+      </c>
+      <c r="J332" s="5">
+        <v>965.86429621801403</v>
+      </c>
+      <c r="K332" s="5">
+        <v>8113.2600882313182</v>
+      </c>
+      <c r="L332" s="5">
+        <v>0.81132600882313177</v>
+      </c>
+      <c r="M332" s="13">
+        <v>41.564115000000001</v>
+      </c>
+      <c r="N332" s="13">
+        <v>-82.649666666666661</v>
+      </c>
+    </row>
+    <row r="333" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A333">
+        <v>120</v>
+      </c>
+      <c r="B333" s="3">
+        <v>42905</v>
+      </c>
+      <c r="C333" s="4">
+        <v>19</v>
+      </c>
+      <c r="D333" s="4">
+        <v>6</v>
+      </c>
+      <c r="E333" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F333" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G333" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="H333" s="18">
+        <v>8.5343999999999998</v>
+      </c>
+      <c r="I333" s="7">
+        <v>7.3</v>
+      </c>
+      <c r="J333" s="5">
+        <v>935.96981244021526</v>
+      </c>
+      <c r="K333" s="5">
+        <v>6832.5796308135714</v>
+      </c>
+      <c r="L333" s="5">
+        <v>0.68325796308135711</v>
+      </c>
+      <c r="M333" s="13">
+        <v>41.563968333333335</v>
+      </c>
+      <c r="N333" s="13">
+        <v>-82.749906666666661</v>
+      </c>
+    </row>
+    <row r="334" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A334">
+        <v>112</v>
+      </c>
+      <c r="B334" s="3">
+        <v>42905</v>
+      </c>
+      <c r="C334" s="4">
+        <v>19</v>
+      </c>
+      <c r="D334" s="4">
+        <v>6</v>
+      </c>
+      <c r="E334" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F334" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G334" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="H334" s="18">
+        <v>6.4008000000000003</v>
+      </c>
+      <c r="I334" s="7">
+        <v>7.5</v>
+      </c>
+      <c r="J334" s="5">
+        <v>904.72923870558043</v>
+      </c>
+      <c r="K334" s="5">
+        <v>6785.4692902918532</v>
+      </c>
+      <c r="L334" s="5">
+        <v>0.67854692902918534</v>
+      </c>
+      <c r="M334" s="13">
+        <v>41.56386333333333</v>
+      </c>
+      <c r="N334" s="13">
+        <v>-82.949744999999993</v>
+      </c>
+    </row>
+    <row r="335" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A335">
+        <v>113</v>
+      </c>
+      <c r="B335" s="3">
+        <v>42905</v>
+      </c>
+      <c r="C335" s="4">
+        <v>19</v>
+      </c>
+      <c r="D335" s="4">
+        <v>6</v>
+      </c>
+      <c r="E335" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F335" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G335" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="H335" s="17">
+        <v>9.7536000000000005</v>
+      </c>
+      <c r="I335" s="7">
+        <v>7.6</v>
+      </c>
+      <c r="J335" s="5">
+        <v>894.03149771914536</v>
+      </c>
+      <c r="K335" s="5">
+        <v>6794.6393826655049</v>
+      </c>
+      <c r="L335" s="5">
+        <v>0.67946393826655049</v>
+      </c>
+      <c r="M335" s="13">
+        <v>41.680346666666665</v>
+      </c>
+      <c r="N335" s="13">
+        <v>-82.949936666666673</v>
+      </c>
+    </row>
+    <row r="336" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A336">
+        <v>108</v>
+      </c>
+      <c r="B336" s="3">
+        <v>42905</v>
+      </c>
+      <c r="C336" s="4">
+        <v>19</v>
+      </c>
+      <c r="D336" s="4">
+        <v>6</v>
+      </c>
+      <c r="E336" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F336" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G336" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="H336" s="17">
+        <v>8.9916</v>
+      </c>
+      <c r="I336" s="7">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="J336" s="5">
+        <v>925.95687332103455</v>
+      </c>
+      <c r="K336" s="5">
+        <v>7685.4420485645878</v>
+      </c>
+      <c r="L336" s="5">
+        <v>0.7685442048564588</v>
+      </c>
+      <c r="M336" s="13">
+        <v>41.681375000000003</v>
+      </c>
+      <c r="N336" s="13">
+        <v>-83.049588333333332</v>
+      </c>
+    </row>
+    <row r="337" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A337">
+        <v>104</v>
+      </c>
+      <c r="B337" s="3">
+        <v>42905</v>
+      </c>
+      <c r="C337" s="4">
+        <v>19</v>
+      </c>
+      <c r="D337" s="4">
+        <v>6</v>
+      </c>
+      <c r="E337" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F337" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G337" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="H337" s="17">
+        <v>8.0771999999999995</v>
+      </c>
+      <c r="I337" s="7">
+        <v>7.6</v>
+      </c>
+      <c r="J337" s="5">
+        <v>917.249375926075</v>
+      </c>
+      <c r="K337" s="5">
+        <v>6971.0952570381696</v>
+      </c>
+      <c r="L337" s="5">
+        <v>0.69710952570381701</v>
+      </c>
+      <c r="M337" s="13">
+        <v>41.681293333333336</v>
+      </c>
+      <c r="N337" s="13">
+        <v>-83.151501666666661</v>
+      </c>
+    </row>
+    <row r="338" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A338">
+        <v>105</v>
+      </c>
+      <c r="B338" s="3">
+        <v>42905</v>
+      </c>
+      <c r="C338" s="4">
+        <v>19</v>
+      </c>
+      <c r="D338" s="4">
+        <v>6</v>
+      </c>
+      <c r="E338" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F338" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G338" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="H338" s="18">
+        <v>8.5343999999999998</v>
+      </c>
+      <c r="I338" s="7">
+        <v>7.8</v>
+      </c>
+      <c r="J338" s="5">
+        <v>926.00002891644999</v>
+      </c>
+      <c r="K338" s="5">
+        <v>7222.8002255483098</v>
+      </c>
+      <c r="L338" s="5">
+        <v>0.72228002255483092</v>
+      </c>
+      <c r="M338" s="13">
+        <v>41.780941666666664</v>
+      </c>
+      <c r="N338" s="13">
+        <v>-83.150553333333335</v>
+      </c>
+    </row>
+    <row r="339" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A339">
+        <v>109</v>
+      </c>
+      <c r="B339" s="3">
+        <v>42905</v>
+      </c>
+      <c r="C339" s="4">
+        <v>19</v>
+      </c>
+      <c r="D339" s="4">
+        <v>6</v>
+      </c>
+      <c r="E339" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F339" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G339" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="H339" s="17">
+        <v>10.08888</v>
+      </c>
+      <c r="I339" s="7">
+        <v>7.9</v>
+      </c>
+      <c r="J339" s="5">
+        <v>957.92222288483208</v>
+      </c>
+      <c r="K339" s="5">
+        <v>7567.585560790174</v>
+      </c>
+      <c r="L339" s="5">
+        <v>0.75675855607901743</v>
+      </c>
+      <c r="M339" s="13">
+        <v>41.780825</v>
+      </c>
+      <c r="N339" s="13">
+        <v>-83.049596666666673</v>
+      </c>
+    </row>
+    <row r="340" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A340">
+        <v>114</v>
+      </c>
+      <c r="B340" s="3">
+        <v>42905</v>
+      </c>
+      <c r="C340" s="4">
+        <v>19</v>
+      </c>
+      <c r="D340" s="4">
+        <v>6</v>
+      </c>
+      <c r="E340" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F340" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G340" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="H340" s="17">
+        <v>10.667999999999999</v>
+      </c>
+      <c r="I340" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="J340" s="5">
+        <v>903.04217311934087</v>
+      </c>
+      <c r="K340" s="5">
+        <v>7675.858471514397</v>
+      </c>
+      <c r="L340" s="5">
+        <v>0.76758584715143974</v>
+      </c>
+      <c r="M340" s="13">
+        <v>41.763444999999997</v>
+      </c>
+      <c r="N340" s="13">
+        <v>-82.950403333333327</v>
+      </c>
+    </row>
+    <row r="341" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A341">
+        <v>116</v>
+      </c>
+      <c r="B341" s="3">
+        <v>42906</v>
+      </c>
+      <c r="C341" s="4">
+        <v>20</v>
+      </c>
+      <c r="D341" s="4">
+        <v>6</v>
+      </c>
+      <c r="E341" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F341" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G341" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="H341" s="17">
+        <v>10.058400000000001</v>
+      </c>
+      <c r="I341" s="7">
+        <v>8</v>
+      </c>
+      <c r="J341" s="5">
+        <v>914.74439958784478</v>
+      </c>
+      <c r="K341" s="5">
+        <v>7317.9551967027583</v>
+      </c>
+      <c r="L341" s="5">
+        <v>0.73179551967027578</v>
+      </c>
+      <c r="M341" s="13">
+        <v>41.667369999999998</v>
+      </c>
+      <c r="N341" s="13">
+        <v>-82.850456666666673</v>
+      </c>
+    </row>
+    <row r="342" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A342">
+        <v>117</v>
+      </c>
+      <c r="B342" s="3">
+        <v>42906</v>
+      </c>
+      <c r="C342" s="4">
+        <v>20</v>
+      </c>
+      <c r="D342" s="4">
+        <v>6</v>
+      </c>
+      <c r="E342" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F342" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G342" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="H342" s="17">
+        <v>10.667999999999999</v>
+      </c>
+      <c r="I342" s="7">
+        <v>8</v>
+      </c>
+      <c r="J342" s="5">
+        <v>924.97759615966697</v>
+      </c>
+      <c r="K342" s="5">
+        <v>7399.8207692773358</v>
+      </c>
+      <c r="L342" s="5">
+        <v>0.73998207692773355</v>
+      </c>
+      <c r="M342" s="13">
+        <v>41.767276666666667</v>
+      </c>
+      <c r="N342" s="13">
+        <v>-82.875455000000002</v>
+      </c>
+    </row>
+    <row r="343" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A343">
+        <v>118</v>
+      </c>
+      <c r="B343" s="3">
+        <v>42906</v>
+      </c>
+      <c r="C343" s="4">
+        <v>20</v>
+      </c>
+      <c r="D343" s="4">
+        <v>6</v>
+      </c>
+      <c r="E343" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F343" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G343" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="H343" s="17">
+        <v>11.5824</v>
+      </c>
+      <c r="I343" s="7">
+        <v>8</v>
+      </c>
+      <c r="J343" s="5">
+        <v>923.5511918087326</v>
+      </c>
+      <c r="K343" s="5">
+        <v>7388.4095344698608</v>
+      </c>
+      <c r="L343" s="5">
+        <v>0.73884095344698608</v>
+      </c>
+      <c r="M343" s="13">
+        <v>41.867699999999999</v>
+      </c>
+      <c r="N343" s="13">
+        <v>-82.867194999999995</v>
+      </c>
+    </row>
+    <row r="344" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A344">
+        <v>115</v>
+      </c>
+      <c r="B344" s="3">
+        <v>42906</v>
+      </c>
+      <c r="C344" s="4">
+        <v>20</v>
+      </c>
+      <c r="D344" s="4">
+        <v>6</v>
+      </c>
+      <c r="E344" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F344" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G344" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="H344" s="17">
+        <v>10.667999999999999</v>
+      </c>
+      <c r="I344" s="7">
+        <v>8</v>
+      </c>
+      <c r="J344" s="5">
+        <v>943.87608633748494</v>
+      </c>
+      <c r="K344" s="5">
+        <v>7551.0086906998795</v>
+      </c>
+      <c r="L344" s="5">
+        <v>0.75510086906998797</v>
+      </c>
+      <c r="M344" s="13">
+        <v>41.87968166666667</v>
+      </c>
+      <c r="N344" s="13">
+        <v>-82.950220000000002</v>
+      </c>
+    </row>
+    <row r="345" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A345">
+        <v>110</v>
+      </c>
+      <c r="B345" s="3">
+        <v>42906</v>
+      </c>
+      <c r="C345" s="4">
+        <v>20</v>
+      </c>
+      <c r="D345" s="4">
+        <v>6</v>
+      </c>
+      <c r="E345" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F345" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G345" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="H345" s="17">
+        <v>9.7536000000000005</v>
+      </c>
+      <c r="I345" s="7">
+        <v>7.7</v>
+      </c>
+      <c r="J345" s="5">
+        <v>943.23419119424807</v>
+      </c>
+      <c r="K345" s="5">
+        <v>7262.9032721957101</v>
+      </c>
+      <c r="L345" s="5">
+        <v>0.72629032721957099</v>
+      </c>
+      <c r="M345" s="13">
+        <v>41.879481666666663</v>
+      </c>
+      <c r="N345" s="13">
+        <v>-83.050101666666663</v>
+      </c>
+    </row>
+    <row r="346" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A346">
+        <v>111</v>
+      </c>
+      <c r="B346" s="3">
+        <v>42906</v>
+      </c>
+      <c r="C346" s="4">
+        <v>20</v>
+      </c>
+      <c r="D346" s="4">
+        <v>6</v>
+      </c>
+      <c r="E346" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F346" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G346" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="H346" s="17">
+        <v>8.2295999999999996</v>
+      </c>
+      <c r="I346" s="7">
+        <v>7.7</v>
+      </c>
+      <c r="J346" s="5">
+        <v>942.47469050797031</v>
+      </c>
+      <c r="K346" s="5">
+        <v>7257.0551169113714</v>
+      </c>
+      <c r="L346" s="5">
+        <v>0.72570551169113717</v>
+      </c>
+      <c r="M346" s="13">
+        <v>41.979848333333337</v>
+      </c>
+      <c r="N346" s="13">
+        <v>-83.049788333333339</v>
+      </c>
+    </row>
+    <row r="347" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A347">
+        <v>107</v>
+      </c>
+      <c r="B347" s="3">
+        <v>42906</v>
+      </c>
+      <c r="C347" s="4">
+        <v>20</v>
+      </c>
+      <c r="D347" s="4">
+        <v>6</v>
+      </c>
+      <c r="E347" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F347" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G347" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="H347" s="17">
+        <v>7.3151999999999999</v>
+      </c>
+      <c r="I347" s="7">
+        <v>7.6</v>
+      </c>
+      <c r="J347" s="5">
+        <v>961.74539586241599</v>
+      </c>
+      <c r="K347" s="5">
+        <v>7309.265008554361</v>
+      </c>
+      <c r="L347" s="5">
+        <v>0.73092650085543609</v>
+      </c>
+      <c r="M347" s="13">
+        <v>41.98001</v>
+      </c>
+      <c r="N347" s="13">
+        <v>-83.117026666666661</v>
+      </c>
+    </row>
+    <row r="348" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A348">
+        <v>106</v>
+      </c>
+      <c r="B348" s="3">
+        <v>42906</v>
+      </c>
+      <c r="C348" s="4">
+        <v>20</v>
+      </c>
+      <c r="D348" s="4">
+        <v>6</v>
+      </c>
+      <c r="E348" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F348" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G348" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="H348" s="17">
+        <v>9.4488000000000003</v>
+      </c>
+      <c r="I348" s="7">
+        <v>7.3</v>
+      </c>
+      <c r="J348" s="5">
+        <v>883.06594744474546</v>
+      </c>
+      <c r="K348" s="5">
+        <v>6446.3814163466413</v>
+      </c>
+      <c r="L348" s="5">
+        <v>0.64463814163466415</v>
+      </c>
+      <c r="M348" s="13">
+        <v>41.879980000000003</v>
+      </c>
+      <c r="N348" s="13">
+        <v>-83.150251666666662</v>
+      </c>
+    </row>
+    <row r="349" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A349">
+        <v>103</v>
+      </c>
+      <c r="B349" s="3">
+        <v>42906</v>
+      </c>
+      <c r="C349" s="4">
+        <v>20</v>
+      </c>
+      <c r="D349" s="4">
+        <v>6</v>
+      </c>
+      <c r="E349" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F349" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G349" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="H349" s="17">
+        <v>8.2295999999999996</v>
+      </c>
+      <c r="I349" s="7">
+        <v>7.1</v>
+      </c>
+      <c r="J349" s="5">
+        <v>936.85674964987265</v>
+      </c>
+      <c r="K349" s="5">
+        <v>6651.6829225140955</v>
+      </c>
+      <c r="L349" s="5">
+        <v>0.6651682922514095</v>
+      </c>
+      <c r="M349" s="13">
+        <v>41.881568333333334</v>
+      </c>
+      <c r="N349" s="13">
+        <v>-83.249684999999999</v>
+      </c>
+    </row>
+    <row r="350" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A350">
+        <v>101</v>
+      </c>
+      <c r="B350" s="3">
+        <v>42906</v>
+      </c>
+      <c r="C350" s="4">
+        <v>20</v>
+      </c>
+      <c r="D350" s="4">
+        <v>6</v>
+      </c>
+      <c r="E350" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F350" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G350" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="H350" s="17">
+        <v>5.4863999999999997</v>
+      </c>
+      <c r="I350" s="7">
+        <v>7.3</v>
+      </c>
+      <c r="J350" s="5">
+        <v>935.42748104801819</v>
+      </c>
+      <c r="K350" s="5">
+        <v>6828.6206116505327</v>
+      </c>
+      <c r="L350" s="5">
+        <v>0.68286206116505332</v>
+      </c>
+      <c r="M350" s="13">
+        <v>41.780288333333331</v>
+      </c>
+      <c r="N350" s="13">
+        <v>-83.34992166666666</v>
+      </c>
+    </row>
+    <row r="351" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A351">
+        <v>102</v>
+      </c>
+      <c r="B351" s="3">
+        <v>42906</v>
+      </c>
+      <c r="C351" s="4">
+        <v>20</v>
+      </c>
+      <c r="D351" s="4">
+        <v>6</v>
+      </c>
+      <c r="E351" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F351" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G351" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="H351" s="17">
+        <v>8.2295999999999996</v>
+      </c>
+      <c r="I351" s="7">
+        <v>7.2</v>
+      </c>
+      <c r="J351" s="5">
+        <v>870.0555527046813</v>
+      </c>
+      <c r="K351" s="5">
+        <v>6264.3999794737056</v>
+      </c>
+      <c r="L351" s="5">
+        <v>0.6264399979473706</v>
+      </c>
+      <c r="M351" s="13">
+        <v>41.780313333333332</v>
+      </c>
+      <c r="N351" s="13">
+        <v>-83.250138333333339</v>
+      </c>
+    </row>
+    <row r="352" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A352">
+        <v>121</v>
+      </c>
+      <c r="B352" s="3">
+        <v>42907</v>
+      </c>
+      <c r="C352" s="4">
+        <v>21</v>
+      </c>
+      <c r="D352" s="4">
+        <v>6</v>
+      </c>
+      <c r="E352" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F352" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G352" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="H352" s="17">
+        <v>10.667999999999999</v>
+      </c>
+      <c r="I352" s="7">
+        <v>8.1</v>
+      </c>
+      <c r="J352" s="5">
+        <v>900.82570269656208</v>
+      </c>
+      <c r="K352" s="5">
+        <v>7296.6881918421523</v>
+      </c>
+      <c r="L352" s="5">
+        <v>0.72966881918421522</v>
+      </c>
+      <c r="M352" s="13">
+        <v>41.680566666666664</v>
+      </c>
+      <c r="N352" s="13">
+        <v>-82.751548333333332</v>
+      </c>
+    </row>
+    <row r="353" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A353">
+        <v>122</v>
+      </c>
+      <c r="B353" s="3">
+        <v>42907</v>
+      </c>
+      <c r="C353" s="4">
+        <v>21</v>
+      </c>
+      <c r="D353" s="4">
+        <v>6</v>
+      </c>
+      <c r="E353" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F353" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G353" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H353" s="17">
+        <v>10.667999999999999</v>
+      </c>
+      <c r="I353" s="7">
+        <v>7.9</v>
+      </c>
+      <c r="J353" s="5">
+        <v>909.17375832589448</v>
+      </c>
+      <c r="K353" s="5">
+        <v>7182.4726907745671</v>
+      </c>
+      <c r="L353" s="5">
+        <v>0.71824726907745673</v>
+      </c>
+      <c r="M353" s="13">
+        <v>41.779649999999997</v>
+      </c>
+      <c r="N353" s="13">
+        <v>-82.749224999999996</v>
+      </c>
+    </row>
+    <row r="354" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A354">
+        <v>123</v>
+      </c>
+      <c r="B354" s="3">
+        <v>42907</v>
+      </c>
+      <c r="C354" s="4">
+        <v>21</v>
+      </c>
+      <c r="D354" s="4">
+        <v>6</v>
+      </c>
+      <c r="E354" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F354" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G354" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="H354" s="17">
+        <v>12.192</v>
+      </c>
+      <c r="I354" s="7">
+        <v>8</v>
+      </c>
+      <c r="J354" s="5">
+        <v>919.38656305409961</v>
+      </c>
+      <c r="K354" s="5">
+        <v>7355.0925044327969</v>
+      </c>
+      <c r="L354" s="5">
+        <v>0.73550925044327964</v>
+      </c>
+      <c r="M354" s="13">
+        <v>41.866565000000001</v>
+      </c>
+      <c r="N354" s="13">
+        <v>-82.750586666666663</v>
+      </c>
+    </row>
+    <row r="355" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A355">
+        <v>119</v>
+      </c>
+      <c r="B355" s="3">
+        <v>42907</v>
+      </c>
+      <c r="C355" s="4">
+        <v>21</v>
+      </c>
+      <c r="D355" s="4">
+        <v>6</v>
+      </c>
+      <c r="E355" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F355" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G355" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="H355" s="17">
+        <v>10.667999999999999</v>
+      </c>
+      <c r="I355" s="7">
+        <v>7.7</v>
+      </c>
+      <c r="J355" s="5">
+        <v>874.12838698135397</v>
+      </c>
+      <c r="K355" s="5">
+        <v>6730.7885797564259</v>
+      </c>
+      <c r="L355" s="5">
+        <v>0.6730788579756426</v>
+      </c>
+      <c r="M355" s="13">
+        <v>41.963636666666666</v>
+      </c>
+      <c r="N355" s="13">
+        <v>-82.850018333333338</v>
+      </c>
+    </row>
+    <row r="356" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A356">
+        <v>124</v>
+      </c>
+      <c r="B356" s="3">
+        <v>42907</v>
+      </c>
+      <c r="C356" s="4">
+        <v>21</v>
+      </c>
+      <c r="D356" s="4">
+        <v>6</v>
+      </c>
+      <c r="E356" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F356" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G356" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="H356" s="17">
+        <v>11.5824</v>
+      </c>
+      <c r="I356" s="7">
+        <v>8</v>
+      </c>
+      <c r="J356" s="5">
+        <v>906.77135617637953</v>
+      </c>
+      <c r="K356" s="5">
+        <v>7254.1708494110362</v>
+      </c>
+      <c r="L356" s="5">
+        <v>0.72541708494110357</v>
+      </c>
+      <c r="M356" s="13">
+        <v>41.963673333333332</v>
+      </c>
+      <c r="N356" s="13">
+        <v>-82.749913333333339</v>
+      </c>
+    </row>
+    <row r="357" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A357">
+        <v>128</v>
+      </c>
+      <c r="B357" s="3">
+        <v>42907</v>
+      </c>
+      <c r="C357" s="4">
+        <v>21</v>
+      </c>
+      <c r="D357" s="4">
+        <v>6</v>
+      </c>
+      <c r="E357" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F357" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G357" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="H357" s="17">
+        <v>11.2776</v>
+      </c>
+      <c r="I357" s="7">
+        <v>7.8</v>
+      </c>
+      <c r="J357" s="5">
+        <v>907.23279527347756</v>
+      </c>
+      <c r="K357" s="5">
+        <v>7076.4158031331244</v>
+      </c>
+      <c r="L357" s="5">
+        <v>0.70764158031331248</v>
+      </c>
+      <c r="M357" s="13">
+        <v>41.980226666666667</v>
+      </c>
+      <c r="N357" s="13">
+        <v>-82.649953333333329</v>
+      </c>
+    </row>
+    <row r="358" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A358">
+        <v>127</v>
+      </c>
+      <c r="B358" s="3">
+        <v>42907</v>
+      </c>
+      <c r="C358" s="4">
+        <v>21</v>
+      </c>
+      <c r="D358" s="4">
+        <v>6</v>
+      </c>
+      <c r="E358" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F358" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G358" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="H358" s="17">
+        <v>11.5824</v>
+      </c>
+      <c r="I358" s="7">
+        <v>8.1</v>
+      </c>
+      <c r="J358" s="5">
+        <v>960.00197066016835</v>
+      </c>
+      <c r="K358" s="5">
+        <v>7776.0159623473637</v>
+      </c>
+      <c r="L358" s="5">
+        <v>0.77760159623473635</v>
+      </c>
+      <c r="M358" s="13">
+        <v>41.863646666666668</v>
+      </c>
+      <c r="N358" s="13">
+        <v>-82.650498333333331</v>
+      </c>
+    </row>
+    <row r="359" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A359">
+        <v>133</v>
+      </c>
+      <c r="B359" s="3">
+        <v>42907</v>
+      </c>
+      <c r="C359" s="4">
+        <v>21</v>
+      </c>
+      <c r="D359" s="4">
+        <v>6</v>
+      </c>
+      <c r="E359" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F359" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G359" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="H359" s="19">
+        <v>12.192</v>
+      </c>
+      <c r="I359" s="7">
+        <v>8.1</v>
+      </c>
+      <c r="J359" s="5">
+        <v>952.51962483964826</v>
+      </c>
+      <c r="K359" s="5">
+        <v>7715.4089612011503</v>
+      </c>
+      <c r="L359" s="5">
+        <v>0.77154089612011501</v>
+      </c>
+      <c r="M359" s="13">
+        <v>41.86740833333333</v>
+      </c>
+      <c r="N359" s="13">
+        <v>-82.532561666666666</v>
+      </c>
+    </row>
+    <row r="360" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A360">
+        <v>132</v>
+      </c>
+      <c r="B360" s="3">
+        <v>42907</v>
+      </c>
+      <c r="C360" s="4">
+        <v>21</v>
+      </c>
+      <c r="D360" s="4">
+        <v>6</v>
+      </c>
+      <c r="E360" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F360" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G360" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="H360" s="17">
+        <v>11.5824</v>
+      </c>
+      <c r="I360" s="7">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="J360" s="5">
+        <v>867.21819986280991</v>
+      </c>
+      <c r="K360" s="5">
+        <v>7111.1892388750402</v>
+      </c>
+      <c r="L360" s="5">
+        <v>0.71111892388750397</v>
+      </c>
+      <c r="M360" s="13">
+        <v>41.779211666666669</v>
+      </c>
+      <c r="N360" s="13">
+        <v>-82.551429999999996</v>
+      </c>
+    </row>
+    <row r="361" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A361">
+        <v>137</v>
+      </c>
+      <c r="B361" s="3">
+        <v>42907</v>
+      </c>
+      <c r="C361" s="4">
+        <v>21</v>
+      </c>
+      <c r="D361" s="4">
+        <v>6</v>
+      </c>
+      <c r="E361" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F361" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G361" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H361" s="17">
+        <v>13.411199999999999</v>
+      </c>
+      <c r="I361" s="7">
+        <v>8.6</v>
+      </c>
+      <c r="J361" s="5">
+        <v>855.67141092899055</v>
+      </c>
+      <c r="K361" s="5">
+        <v>7358.7741339893182</v>
+      </c>
+      <c r="L361" s="5">
+        <v>0.73587741339893187</v>
+      </c>
+      <c r="M361" s="13">
+        <v>41.780883333333335</v>
+      </c>
+      <c r="N361" s="13">
+        <v>-82.448693333333338</v>
+      </c>
+    </row>
+    <row r="362" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A362">
+        <v>131</v>
+      </c>
+      <c r="B362" s="3">
+        <v>42907</v>
+      </c>
+      <c r="C362" s="4">
+        <v>21</v>
+      </c>
+      <c r="D362" s="4">
+        <v>6</v>
+      </c>
+      <c r="E362" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F362" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G362" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="H362" s="17">
+        <v>13.715999999999999</v>
+      </c>
+      <c r="I362" s="7">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="J362" s="5">
+        <v>935.31867185816134</v>
+      </c>
+      <c r="K362" s="5">
+        <v>7669.6131092369224</v>
+      </c>
+      <c r="L362" s="5">
+        <v>0.76696131092369224</v>
+      </c>
+      <c r="M362" s="13">
+        <v>41.662471666666669</v>
+      </c>
+      <c r="N362" s="13">
+        <v>-82.551696666666672</v>
+      </c>
+    </row>
+    <row r="363" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A363">
+        <v>126</v>
+      </c>
+      <c r="B363" s="3">
+        <v>42907</v>
+      </c>
+      <c r="C363" s="4">
+        <v>21</v>
+      </c>
+      <c r="D363" s="4">
+        <v>6</v>
+      </c>
+      <c r="E363" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F363" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G363" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="H363" s="17">
+        <v>11.2776</v>
+      </c>
+      <c r="I363" s="7">
+        <v>7.6</v>
+      </c>
+      <c r="J363" s="5">
+        <v>891.40021110721739</v>
+      </c>
+      <c r="K363" s="5">
+        <v>6774.6416044148518</v>
+      </c>
+      <c r="L363" s="5">
+        <v>0.67746416044148516</v>
+      </c>
+      <c r="M363" s="13">
+        <v>41.680328333333335</v>
+      </c>
+      <c r="N363" s="13">
+        <v>-82.650471666666661</v>
+      </c>
+    </row>
+    <row r="364" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A364">
+        <v>136</v>
+      </c>
+      <c r="B364" s="3">
+        <v>42908</v>
+      </c>
+      <c r="C364" s="4">
+        <v>22</v>
+      </c>
+      <c r="D364" s="4">
+        <v>6</v>
+      </c>
+      <c r="E364" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F364" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G364" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="H364" s="17">
+        <v>14.6304</v>
+      </c>
+      <c r="I364" s="7">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="J364" s="5">
+        <v>910.5369119095426</v>
+      </c>
+      <c r="K364" s="5">
+        <v>7921.6711336130202</v>
+      </c>
+      <c r="L364" s="5">
+        <v>0.79216711336130197</v>
+      </c>
+      <c r="M364" s="13">
+        <v>41.664076666666666</v>
+      </c>
+      <c r="N364" s="13">
+        <v>-82.449348333333333</v>
+      </c>
+    </row>
+    <row r="365" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A365">
+        <v>140</v>
+      </c>
+      <c r="B365" s="3">
+        <v>42908</v>
+      </c>
+      <c r="C365" s="4">
+        <v>22</v>
+      </c>
+      <c r="D365" s="4">
+        <v>6</v>
+      </c>
+      <c r="E365" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F365" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G365" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="H365" s="17">
+        <v>14.6304</v>
+      </c>
+      <c r="I365" s="7">
+        <v>8.6</v>
+      </c>
+      <c r="J365" s="5">
+        <v>910.65985099257364</v>
+      </c>
+      <c r="K365" s="5">
+        <v>7831.6747185361328</v>
+      </c>
+      <c r="L365" s="5">
+        <v>0.78316747185361324</v>
+      </c>
+      <c r="M365" s="13">
+        <v>41.663373333333332</v>
+      </c>
+      <c r="N365" s="13">
+        <v>-82.36231166666667</v>
+      </c>
+    </row>
+    <row r="366" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A366">
+        <v>135</v>
+      </c>
+      <c r="B366" s="3">
+        <v>42908</v>
+      </c>
+      <c r="C366" s="4">
+        <v>22</v>
+      </c>
+      <c r="D366" s="4">
+        <v>6</v>
+      </c>
+      <c r="E366" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F366" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G366" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="H366" s="17">
+        <v>14.9352</v>
+      </c>
+      <c r="I366" s="7">
+        <v>8.6</v>
+      </c>
+      <c r="J366" s="5">
+        <v>889.05744373314826</v>
+      </c>
+      <c r="K366" s="5">
+        <v>7645.894016105075</v>
+      </c>
+      <c r="L366" s="5">
+        <v>0.76458940161050748</v>
+      </c>
+      <c r="M366" s="13">
+        <v>41.579054999999997</v>
+      </c>
+      <c r="N366" s="13">
+        <v>-82.45006166666667</v>
+      </c>
+    </row>
+    <row r="367" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A367">
+        <v>529</v>
+      </c>
+      <c r="B367" s="3">
+        <v>42996</v>
+      </c>
+      <c r="C367" s="4">
+        <v>18</v>
+      </c>
+      <c r="D367" s="4">
+        <v>9</v>
+      </c>
+      <c r="E367" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F367" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G367" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="H367" s="5">
+        <v>13</v>
+      </c>
+      <c r="I367" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="J367" s="5">
+        <v>850.09802811765451</v>
+      </c>
+      <c r="K367" s="5">
+        <v>7225.8332390000633</v>
+      </c>
+      <c r="L367" s="5">
+        <v>0.72258332390000635</v>
+      </c>
+      <c r="M367" s="13">
+        <v>41.464588333333303</v>
+      </c>
+      <c r="N367" s="13">
+        <v>-82.550264999999996</v>
+      </c>
+    </row>
+    <row r="368" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A368">
+        <v>530</v>
+      </c>
+      <c r="B368" s="3">
+        <v>42996</v>
+      </c>
+      <c r="C368" s="4">
+        <v>18</v>
+      </c>
+      <c r="D368" s="4">
+        <v>9</v>
+      </c>
+      <c r="E368" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F368" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G368" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H368" s="5">
+        <v>13.7</v>
+      </c>
+      <c r="I368" s="7">
+        <v>8.4</v>
+      </c>
+      <c r="J368" s="5">
+        <v>828.38546867996865</v>
+      </c>
+      <c r="K368" s="5">
+        <v>6958.4379369117369</v>
+      </c>
+      <c r="L368" s="5">
+        <v>0.69584379369117366</v>
+      </c>
+      <c r="M368" s="13">
+        <v>41.568666666666701</v>
+      </c>
+      <c r="N368" s="13">
+        <v>-82.547870000000003</v>
+      </c>
+    </row>
+    <row r="369" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A369">
+        <v>525</v>
+      </c>
+      <c r="B369" s="3">
+        <v>42996</v>
+      </c>
+      <c r="C369" s="4">
+        <v>18</v>
+      </c>
+      <c r="D369" s="4">
+        <v>9</v>
+      </c>
+      <c r="E369" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F369" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G369" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="H369" s="5">
+        <v>13</v>
+      </c>
+      <c r="I369" s="7">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="J369" s="5">
+        <v>848.78363347116544</v>
+      </c>
+      <c r="K369" s="5">
+        <v>7384.4176111991392</v>
+      </c>
+      <c r="L369" s="5">
+        <v>0.73844176111991389</v>
+      </c>
+      <c r="M369" s="13">
+        <v>41.564056666666701</v>
+      </c>
+      <c r="N369" s="13">
+        <v>-82.646486666666704</v>
+      </c>
+    </row>
+    <row r="370" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A370">
+        <v>520</v>
+      </c>
+      <c r="B370" s="3">
+        <v>42996</v>
+      </c>
+      <c r="C370" s="4">
+        <v>18</v>
+      </c>
+      <c r="D370" s="4">
+        <v>9</v>
+      </c>
+      <c r="E370" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F370" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G370" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="H370" s="5">
+        <v>9</v>
+      </c>
+      <c r="I370" s="7">
+        <v>7.9249999999999998</v>
+      </c>
+      <c r="J370" s="5">
+        <v>600.56655999999998</v>
+      </c>
+      <c r="K370" s="5">
+        <v>4759.4899879999994</v>
+      </c>
+      <c r="L370" s="5">
+        <v>0.47594899879999991</v>
+      </c>
+      <c r="M370" s="13">
+        <v>41.563783333333298</v>
+      </c>
+      <c r="N370" s="13">
+        <v>-82.743520000000004</v>
+      </c>
+    </row>
+    <row r="371" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A371">
+        <v>512</v>
+      </c>
+      <c r="B371" s="3">
+        <v>42996</v>
+      </c>
+      <c r="C371" s="4">
+        <v>18</v>
+      </c>
+      <c r="D371" s="4">
+        <v>9</v>
+      </c>
+      <c r="E371" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F371" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G371" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="H371" s="5">
+        <v>6.8</v>
+      </c>
+      <c r="I371" s="7">
+        <v>7.2</v>
+      </c>
+      <c r="J371" s="5">
+        <v>927.8683843881787</v>
+      </c>
+      <c r="K371" s="5">
+        <v>6680.6523675948865</v>
+      </c>
+      <c r="L371" s="5">
+        <v>0.6680652367594887</v>
+      </c>
+      <c r="M371" s="13">
+        <v>41.567264999999999</v>
+      </c>
+      <c r="N371" s="13">
+        <v>-82.9412466666667</v>
+      </c>
+    </row>
+    <row r="372" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A372">
+        <v>513</v>
+      </c>
+      <c r="B372" s="3">
+        <v>42996</v>
+      </c>
+      <c r="C372" s="4">
+        <v>18</v>
+      </c>
+      <c r="D372" s="4">
+        <v>9</v>
+      </c>
+      <c r="E372" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F372" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G372" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="H372" s="5">
+        <v>9.5</v>
+      </c>
+      <c r="I372" s="7">
+        <v>8.1</v>
+      </c>
+      <c r="J372" s="5">
+        <v>1075.1904342584521</v>
+      </c>
+      <c r="K372" s="5">
+        <v>8709.0425174934626</v>
+      </c>
+      <c r="L372" s="5">
+        <v>0.87090425174934627</v>
+      </c>
+      <c r="M372" s="13">
+        <v>41.678658333333303</v>
+      </c>
+      <c r="N372" s="13">
+        <v>-82.949376666666694</v>
+      </c>
+    </row>
+    <row r="373" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A373">
+        <v>508</v>
+      </c>
+      <c r="B373" s="3">
+        <v>42996</v>
+      </c>
+      <c r="C373" s="4">
+        <v>18</v>
+      </c>
+      <c r="D373" s="4">
+        <v>9</v>
+      </c>
+      <c r="E373" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F373" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G373" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="H373" s="5">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="I373" s="7">
+        <v>8</v>
+      </c>
+      <c r="J373" s="5">
+        <v>790.2221487964996</v>
+      </c>
+      <c r="K373" s="5">
+        <v>6321.7771903719968</v>
+      </c>
+      <c r="L373" s="5">
+        <v>0.63217771903719966</v>
+      </c>
+      <c r="M373" s="13">
+        <v>41.681808333333301</v>
+      </c>
+      <c r="N373" s="13">
+        <v>-83.047626666666702</v>
+      </c>
+    </row>
+    <row r="374" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A374">
+        <v>504</v>
+      </c>
+      <c r="B374" s="3">
+        <v>42996</v>
+      </c>
+      <c r="C374" s="4">
+        <v>18</v>
+      </c>
+      <c r="D374" s="4">
+        <v>9</v>
+      </c>
+      <c r="E374" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F374" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G374" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="H374" s="5">
+        <v>7.8</v>
+      </c>
+      <c r="I374" s="7">
+        <v>7.6</v>
+      </c>
+      <c r="J374" s="5">
+        <v>850.00485766463146</v>
+      </c>
+      <c r="K374" s="5">
+        <v>6460.0369182511986</v>
+      </c>
+      <c r="L374" s="5">
+        <v>0.64600369182511985</v>
+      </c>
+      <c r="M374" s="13">
+        <v>41.6800766666667</v>
+      </c>
+      <c r="N374" s="13">
+        <v>-83.147675000000007</v>
+      </c>
+    </row>
+    <row r="375" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A375">
+        <v>505</v>
+      </c>
+      <c r="B375" s="3">
+        <v>42996</v>
+      </c>
+      <c r="C375" s="4">
+        <v>18</v>
+      </c>
+      <c r="D375" s="4">
+        <v>9</v>
+      </c>
+      <c r="E375" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F375" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G375" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="H375" s="5">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="I375" s="7">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="J375" s="5">
+        <v>825.03173824923363</v>
+      </c>
+      <c r="K375" s="5">
+        <v>7177.7761227683322</v>
+      </c>
+      <c r="L375" s="5">
+        <v>0.71777761227683323</v>
+      </c>
+      <c r="M375" s="13">
+        <v>41.778438333333298</v>
+      </c>
+      <c r="N375" s="13">
+        <v>-83.149748333333307</v>
+      </c>
+    </row>
+    <row r="376" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A376">
+        <v>509</v>
+      </c>
+      <c r="B376" s="3">
+        <v>42996</v>
+      </c>
+      <c r="C376" s="4">
+        <v>18</v>
+      </c>
+      <c r="D376" s="4">
+        <v>9</v>
+      </c>
+      <c r="E376" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F376" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G376" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="H376" s="5">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="I376" s="7">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="J376" s="5">
+        <v>850.94296048931255</v>
+      </c>
+      <c r="K376" s="5">
+        <v>6977.7322760123625</v>
+      </c>
+      <c r="L376" s="5">
+        <v>0.69777322760123628</v>
+      </c>
+      <c r="M376" s="13">
+        <v>41.779118333333301</v>
+      </c>
+      <c r="N376" s="13">
+        <v>-83.052046666666698</v>
+      </c>
+    </row>
+    <row r="377" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A377">
+        <v>516</v>
+      </c>
+      <c r="B377" s="3">
+        <v>42997</v>
+      </c>
+      <c r="C377" s="4">
+        <v>19</v>
+      </c>
+      <c r="D377" s="4">
+        <v>9</v>
+      </c>
+      <c r="E377" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F377" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G377" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="H377" s="5">
+        <v>10</v>
+      </c>
+      <c r="I377" s="7">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="J377" s="5">
+        <v>1036.541203186217</v>
+      </c>
+      <c r="K377" s="5">
+        <v>8499.6378661269791</v>
+      </c>
+      <c r="L377" s="5">
+        <v>0.84996378661269789</v>
+      </c>
+      <c r="M377" s="13">
+        <v>41.671473333333303</v>
+      </c>
+      <c r="N377" s="13">
+        <v>-82.851434999999995</v>
+      </c>
+    </row>
+    <row r="378" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A378">
+        <v>517</v>
+      </c>
+      <c r="B378" s="3">
+        <v>42997</v>
+      </c>
+      <c r="C378" s="4">
+        <v>19</v>
+      </c>
+      <c r="D378" s="4">
+        <v>9</v>
+      </c>
+      <c r="E378" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F378" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G378" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="H378" s="5">
+        <v>10.6</v>
+      </c>
+      <c r="I378" s="7">
+        <v>7.7</v>
+      </c>
+      <c r="J378" s="5">
+        <v>861.63903602476614</v>
+      </c>
+      <c r="K378" s="5">
+        <v>6634.6205773906995</v>
+      </c>
+      <c r="L378" s="5">
+        <v>0.66346205773906997</v>
+      </c>
+      <c r="M378" s="13">
+        <v>41.754638333333297</v>
+      </c>
+      <c r="N378" s="13">
+        <v>-82.854403333333295</v>
+      </c>
+    </row>
+    <row r="379" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A379">
+        <v>514</v>
+      </c>
+      <c r="B379" s="3">
+        <v>42997</v>
+      </c>
+      <c r="C379" s="4">
+        <v>19</v>
+      </c>
+      <c r="D379" s="4">
+        <v>9</v>
+      </c>
+      <c r="E379" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F379" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G379" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="H379" s="5">
+        <v>10.5</v>
+      </c>
+      <c r="I379" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="J379" s="5">
+        <v>857.83424912292037</v>
+      </c>
+      <c r="K379" s="5">
+        <v>7291.5911175448227</v>
+      </c>
+      <c r="L379" s="5">
+        <v>0.72915911175448223</v>
+      </c>
+      <c r="M379" s="13">
+        <v>41.760015000000003</v>
+      </c>
+      <c r="N379" s="13">
+        <v>-82.936655000000002</v>
+      </c>
+    </row>
+    <row r="380" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A380">
+        <v>515</v>
+      </c>
+      <c r="B380" s="3">
+        <v>42997</v>
+      </c>
+      <c r="C380" s="4">
+        <v>19</v>
+      </c>
+      <c r="D380" s="4">
+        <v>9</v>
+      </c>
+      <c r="E380" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F380" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G380" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="H380" s="5">
+        <v>10.5</v>
+      </c>
+      <c r="I380" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="J380" s="5">
+        <v>883.15632554847457</v>
+      </c>
+      <c r="K380" s="5">
+        <v>7506.8287671620337</v>
+      </c>
+      <c r="L380" s="5">
+        <v>0.75068287671620337</v>
+      </c>
+      <c r="M380" s="13">
+        <v>41.877733333333303</v>
+      </c>
+      <c r="N380" s="13">
+        <v>-82.950993333333301</v>
+      </c>
+    </row>
+    <row r="381" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A381">
+        <v>510</v>
+      </c>
+      <c r="B381" s="3">
+        <v>42997</v>
+      </c>
+      <c r="C381" s="4">
+        <v>19</v>
+      </c>
+      <c r="D381" s="4">
+        <v>9</v>
+      </c>
+      <c r="E381" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F381" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G381" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="H381" s="5">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="I381" s="7">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="J381" s="5">
+        <v>866.9028757525025</v>
+      </c>
+      <c r="K381" s="5">
+        <v>7195.2938687457718</v>
+      </c>
+      <c r="L381" s="5">
+        <v>0.71952938687457713</v>
+      </c>
+      <c r="M381" s="13">
+        <v>41.8791333333333</v>
+      </c>
+      <c r="N381" s="13">
+        <v>-83.048793333333293</v>
+      </c>
+    </row>
+    <row r="382" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A382">
+        <v>511</v>
+      </c>
+      <c r="B382" s="3">
+        <v>42997</v>
+      </c>
+      <c r="C382" s="4">
+        <v>19</v>
+      </c>
+      <c r="D382" s="4">
+        <v>9</v>
+      </c>
+      <c r="E382" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F382" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G382" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="H382" s="5">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="I382" s="7">
+        <v>8</v>
+      </c>
+      <c r="J382" s="5">
+        <v>857.96516875999998</v>
+      </c>
+      <c r="K382" s="5">
+        <v>6863.7213500799999</v>
+      </c>
+      <c r="L382" s="5">
+        <v>0.68637213500799998</v>
+      </c>
+      <c r="M382" s="13">
+        <v>41.9743383333333</v>
+      </c>
+      <c r="N382" s="13">
+        <v>-83.028630000000007</v>
+      </c>
+    </row>
+    <row r="383" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A383">
+        <v>507</v>
+      </c>
+      <c r="B383" s="3">
+        <v>42997</v>
+      </c>
+      <c r="C383" s="4">
+        <v>19</v>
+      </c>
+      <c r="D383" s="4">
+        <v>9</v>
+      </c>
+      <c r="E383" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F383" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G383" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="H383" s="5">
+        <v>7.4</v>
+      </c>
+      <c r="I383" s="7">
+        <v>7.8</v>
+      </c>
+      <c r="J383" s="5">
+        <v>867.79994839214055</v>
+      </c>
+      <c r="K383" s="5">
+        <v>6768.8395974586965</v>
+      </c>
+      <c r="L383" s="5">
+        <v>0.67688395974586968</v>
+      </c>
+      <c r="M383" s="13">
+        <v>41.979891666666703</v>
+      </c>
+      <c r="N383" s="13">
+        <v>-83.115476666666694</v>
+      </c>
+    </row>
+    <row r="384" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A384">
+        <v>506</v>
+      </c>
+      <c r="B384" s="3">
+        <v>42997</v>
+      </c>
+      <c r="C384" s="4">
+        <v>19</v>
+      </c>
+      <c r="D384" s="4">
+        <v>9</v>
+      </c>
+      <c r="E384" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F384" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G384" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="H384" s="5">
+        <v>9.4</v>
+      </c>
+      <c r="I384" s="7">
+        <v>8.1</v>
+      </c>
+      <c r="J384" s="5">
+        <v>873.23458301768642</v>
+      </c>
+      <c r="K384" s="5">
+        <v>7073.2001224432597</v>
+      </c>
+      <c r="L384" s="5">
+        <v>0.70732001224432595</v>
+      </c>
+      <c r="M384" s="13">
+        <v>41.879958333333299</v>
+      </c>
+      <c r="N384" s="13">
+        <v>-83.149836666666701</v>
+      </c>
+    </row>
+    <row r="385" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A385">
+        <v>503</v>
+      </c>
+      <c r="B385" s="3">
+        <v>42997</v>
+      </c>
+      <c r="C385" s="4">
+        <v>19</v>
+      </c>
+      <c r="D385" s="4">
+        <v>9</v>
+      </c>
+      <c r="E385" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F385" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G385" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="H385" s="5">
+        <v>8</v>
+      </c>
+      <c r="I385" s="7">
+        <v>7.8</v>
+      </c>
+      <c r="J385" s="5">
+        <v>807.89262280481614</v>
+      </c>
+      <c r="K385" s="5">
+        <v>6301.562457877566</v>
+      </c>
+      <c r="L385" s="5">
+        <v>0.63015624578775664</v>
+      </c>
+      <c r="M385" s="13">
+        <v>41.880625000000002</v>
+      </c>
+      <c r="N385" s="13">
+        <v>-83.239526666666706</v>
+      </c>
+    </row>
+    <row r="386" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A386">
+        <v>501</v>
+      </c>
+      <c r="B386" s="3">
+        <v>42997</v>
+      </c>
+      <c r="C386" s="4">
+        <v>19</v>
+      </c>
+      <c r="D386" s="4">
+        <v>9</v>
+      </c>
+      <c r="E386" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F386" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G386" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="H386" s="5">
+        <v>5.9</v>
+      </c>
+      <c r="I386" s="7">
+        <v>7.4</v>
+      </c>
+      <c r="J386" s="5">
+        <v>926.42642373306876</v>
+      </c>
+      <c r="K386" s="5">
+        <v>6855.5555356247096</v>
+      </c>
+      <c r="L386" s="5">
+        <v>0.685555553562471</v>
+      </c>
+      <c r="M386" s="13">
+        <v>41.784680000000002</v>
+      </c>
+      <c r="N386" s="13">
+        <v>-83.366325000000003</v>
+      </c>
+    </row>
+    <row r="387" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A387">
+        <v>502</v>
+      </c>
+      <c r="B387" s="3">
+        <v>42997</v>
+      </c>
+      <c r="C387" s="4">
+        <v>19</v>
+      </c>
+      <c r="D387" s="4">
+        <v>9</v>
+      </c>
+      <c r="E387" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F387" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G387" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="H387" s="5">
+        <v>7.9</v>
+      </c>
+      <c r="I387" s="7">
+        <v>7.4</v>
+      </c>
+      <c r="J387" s="5">
+        <v>835.24761812232919</v>
+      </c>
+      <c r="K387" s="5">
+        <v>6180.8323741052363</v>
+      </c>
+      <c r="L387" s="5">
+        <v>0.61808323741052362</v>
+      </c>
+      <c r="M387" s="13">
+        <v>41.779580000000003</v>
+      </c>
+      <c r="N387" s="13">
+        <v>-83.253249999999994</v>
+      </c>
+    </row>
+    <row r="388" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A388">
+        <v>521</v>
+      </c>
+      <c r="B388" s="3">
+        <v>42998</v>
+      </c>
+      <c r="C388" s="4">
+        <v>20</v>
+      </c>
+      <c r="D388" s="4">
+        <v>9</v>
+      </c>
+      <c r="E388" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F388" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G388" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H388" s="5">
+        <v>10.6</v>
+      </c>
+      <c r="I388" s="7">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="J388" s="5">
+        <v>761.75646805433882</v>
+      </c>
+      <c r="K388" s="5">
+        <v>6246.4030380455779</v>
+      </c>
+      <c r="L388" s="5">
+        <v>0.62464030380455782</v>
+      </c>
+      <c r="M388" s="13">
+        <v>41.6808433333333</v>
+      </c>
+      <c r="N388" s="13">
+        <v>-82.749958333333296</v>
+      </c>
+    </row>
+    <row r="389" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A389">
+        <v>522</v>
+      </c>
+      <c r="B389" s="3">
+        <v>42998</v>
+      </c>
+      <c r="C389" s="4">
+        <v>20</v>
+      </c>
+      <c r="D389" s="4">
+        <v>9</v>
+      </c>
+      <c r="E389" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F389" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G389" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="H389" s="5">
+        <v>9.9</v>
+      </c>
+      <c r="I389" s="7">
+        <v>7.9</v>
+      </c>
+      <c r="J389" s="5">
+        <v>794.86027548424306</v>
+      </c>
+      <c r="K389" s="5">
+        <v>6279.3961763255202</v>
+      </c>
+      <c r="L389" s="5">
+        <v>0.62793961763255202</v>
+      </c>
+      <c r="M389" s="13">
+        <v>41.778643333333299</v>
+      </c>
+      <c r="N389" s="13">
+        <v>-82.749228333333306</v>
+      </c>
+    </row>
+    <row r="390" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A390">
+        <v>523</v>
+      </c>
+      <c r="B390" s="3">
+        <v>42998</v>
+      </c>
+      <c r="C390" s="4">
+        <v>20</v>
+      </c>
+      <c r="D390" s="4">
+        <v>9</v>
+      </c>
+      <c r="E390" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F390" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G390" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="H390" s="5">
+        <v>12</v>
+      </c>
+      <c r="I390" s="7">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="J390" s="5">
+        <v>941.73645129685588</v>
+      </c>
+      <c r="K390" s="5">
+        <v>8193.1071262826463</v>
+      </c>
+      <c r="L390" s="5">
+        <v>0.8193107126282646</v>
+      </c>
+      <c r="M390" s="13">
+        <v>41.866196666666703</v>
+      </c>
+      <c r="N390" s="13">
+        <v>-82.749684999999999</v>
+      </c>
+    </row>
+    <row r="391" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A391">
+        <v>518</v>
+      </c>
+      <c r="B391" s="3">
+        <v>42998</v>
+      </c>
+      <c r="C391" s="4">
+        <v>20</v>
+      </c>
+      <c r="D391" s="4">
+        <v>9</v>
+      </c>
+      <c r="E391" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F391" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G391" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="H391" s="5">
+        <v>11.5</v>
+      </c>
+      <c r="I391" s="7">
+        <v>9.25</v>
+      </c>
+      <c r="J391" s="5">
+        <v>1019.3776729009339</v>
+      </c>
+      <c r="K391" s="5">
+        <v>9429.243474333638</v>
+      </c>
+      <c r="L391" s="5">
+        <v>0.94292434743336384</v>
+      </c>
+      <c r="M391" s="13">
+        <v>41.863261666666702</v>
+      </c>
+      <c r="N391" s="13">
+        <v>-82.849338333333293</v>
+      </c>
+    </row>
+    <row r="392" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A392">
+        <v>519</v>
+      </c>
+      <c r="B392" s="3">
+        <v>42998</v>
+      </c>
+      <c r="C392" s="4">
+        <v>20</v>
+      </c>
+      <c r="D392" s="4">
+        <v>9</v>
+      </c>
+      <c r="E392" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F392" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G392" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="H392" s="5">
+        <v>10.3</v>
+      </c>
+      <c r="I392" s="7">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="J392" s="5">
+        <v>822.82796704438101</v>
+      </c>
+      <c r="K392" s="5">
+        <v>7158.6033132861139</v>
+      </c>
+      <c r="L392" s="5">
+        <v>0.71586033132861138</v>
+      </c>
+      <c r="M392" s="13">
+        <v>41.96114</v>
+      </c>
+      <c r="N392" s="13">
+        <v>-82.850041666666698</v>
+      </c>
+    </row>
+    <row r="393" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A393">
+        <v>524</v>
+      </c>
+      <c r="B393" s="3">
+        <v>42998</v>
+      </c>
+      <c r="C393" s="4">
+        <v>20</v>
+      </c>
+      <c r="D393" s="4">
+        <v>9</v>
+      </c>
+      <c r="E393" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F393" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G393" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="H393" s="5">
+        <v>11.2</v>
+      </c>
+      <c r="I393" s="7">
+        <v>8.9</v>
+      </c>
+      <c r="J393" s="5">
+        <v>900.19615206553101</v>
+      </c>
+      <c r="K393" s="5">
+        <v>8011.7457533832267</v>
+      </c>
+      <c r="L393" s="5">
+        <v>0.8011745753383227</v>
+      </c>
+      <c r="M393" s="13">
+        <v>41.963214999999998</v>
+      </c>
+      <c r="N393" s="13">
+        <v>-82.750571666666701</v>
+      </c>
+    </row>
+    <row r="394" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A394">
+        <v>528</v>
+      </c>
+      <c r="B394" s="3">
+        <v>42998</v>
+      </c>
+      <c r="C394" s="4">
+        <v>20</v>
+      </c>
+      <c r="D394" s="4">
+        <v>9</v>
+      </c>
+      <c r="E394" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F394" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G394" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="H394" s="5">
+        <v>10.9</v>
+      </c>
+      <c r="I394" s="7">
+        <v>8.9</v>
+      </c>
+      <c r="J394" s="5">
+        <v>825.62610105570172</v>
+      </c>
+      <c r="K394" s="5">
+        <v>7348.0722993957461</v>
+      </c>
+      <c r="L394" s="5">
+        <v>0.73480722993957459</v>
+      </c>
+      <c r="M394" s="13">
+        <v>41.979804999999999</v>
+      </c>
+      <c r="N394" s="13">
+        <v>-82.651521666666696</v>
+      </c>
+    </row>
+    <row r="395" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A395">
+        <v>527</v>
+      </c>
+      <c r="B395" s="3">
+        <v>42998</v>
+      </c>
+      <c r="C395" s="4">
+        <v>20</v>
+      </c>
+      <c r="D395" s="4">
+        <v>9</v>
+      </c>
+      <c r="E395" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F395" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G395" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="H395" s="5">
+        <v>11.3</v>
+      </c>
+      <c r="I395" s="7">
+        <v>9.1</v>
+      </c>
+      <c r="J395" s="5">
+        <v>958.99374865721052</v>
+      </c>
+      <c r="K395" s="5">
+        <v>8726.8431127806161</v>
+      </c>
+      <c r="L395" s="5">
+        <v>0.87268431127806156</v>
+      </c>
+      <c r="M395" s="13">
+        <v>41.863399999999999</v>
+      </c>
+      <c r="N395" s="13">
+        <v>-82.649844999999999</v>
+      </c>
+    </row>
+    <row r="396" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A396">
+        <v>533</v>
+      </c>
+      <c r="B396" s="3">
+        <v>42998</v>
+      </c>
+      <c r="C396" s="4">
+        <v>20</v>
+      </c>
+      <c r="D396" s="4">
+        <v>9</v>
+      </c>
+      <c r="E396" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F396" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G396" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="H396" s="5">
+        <v>12.4</v>
+      </c>
+      <c r="I396" s="7">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="J396" s="5">
+        <v>878.58459007635258</v>
+      </c>
+      <c r="K396" s="5">
+        <v>8082.9782287024427</v>
+      </c>
+      <c r="L396" s="5">
+        <v>0.80829782287024432</v>
+      </c>
+      <c r="M396" s="13">
+        <v>41.865718333333298</v>
+      </c>
+      <c r="N396" s="13">
+        <v>-82.536191666666696</v>
+      </c>
+    </row>
+    <row r="397" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A397">
+        <v>537</v>
+      </c>
+      <c r="B397" s="3">
+        <v>42998</v>
+      </c>
+      <c r="C397" s="4">
+        <v>20</v>
+      </c>
+      <c r="D397" s="4">
+        <v>9</v>
+      </c>
+      <c r="E397" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F397" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G397" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="H397" s="5">
+        <v>13.1</v>
+      </c>
+      <c r="I397" s="7">
+        <v>9.6</v>
+      </c>
+      <c r="J397" s="5">
+        <v>828.94253614547517</v>
+      </c>
+      <c r="K397" s="5">
+        <v>7957.8483469965613</v>
+      </c>
+      <c r="L397" s="5">
+        <v>0.79578483469965611</v>
+      </c>
+      <c r="M397" s="13">
+        <v>41.781878333333303</v>
+      </c>
+      <c r="N397" s="13">
+        <v>-82.451288333333295</v>
+      </c>
+    </row>
+    <row r="398" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A398">
+        <v>532</v>
+      </c>
+      <c r="B398" s="3">
+        <v>42998</v>
+      </c>
+      <c r="C398" s="4">
+        <v>20</v>
+      </c>
+      <c r="D398" s="4">
+        <v>9</v>
+      </c>
+      <c r="E398" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F398" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G398" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="H398" s="5">
+        <v>11.2</v>
+      </c>
+      <c r="I398" s="7">
+        <v>10.7</v>
+      </c>
+      <c r="J398" s="5">
+        <v>820.06704941960663</v>
+      </c>
+      <c r="K398" s="5">
+        <v>8774.7174287897906</v>
+      </c>
+      <c r="L398" s="5">
+        <v>0.87747174287897911</v>
+      </c>
+      <c r="M398" s="13">
+        <v>41.780198333333303</v>
+      </c>
+      <c r="N398" s="13">
+        <v>-82.548043333333297</v>
+      </c>
+    </row>
+    <row r="399" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A399">
+        <v>531</v>
+      </c>
+      <c r="B399" s="3">
+        <v>42998</v>
+      </c>
+      <c r="C399" s="4">
+        <v>20</v>
+      </c>
+      <c r="D399" s="4">
+        <v>9</v>
+      </c>
+      <c r="E399" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F399" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G399" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="H399" s="5">
+        <v>13.4</v>
+      </c>
+      <c r="I399" s="7">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="J399" s="5">
+        <v>846.37543521075486</v>
+      </c>
+      <c r="K399" s="5">
+        <v>8294.4792650653981</v>
+      </c>
+      <c r="L399" s="5">
+        <v>0.82944792650653976</v>
+      </c>
+      <c r="M399" s="13">
+        <v>41.664900000000003</v>
+      </c>
+      <c r="N399" s="13">
+        <v>-82.551523333333293</v>
+      </c>
+    </row>
+    <row r="400" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A400">
+        <v>526</v>
+      </c>
+      <c r="B400" s="3">
+        <v>42999</v>
+      </c>
+      <c r="C400" s="4">
+        <v>21</v>
+      </c>
+      <c r="D400" s="4">
+        <v>9</v>
+      </c>
+      <c r="E400" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F400" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G400" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="H400" s="5">
+        <v>10.8</v>
+      </c>
+      <c r="I400" s="7">
+        <v>9.1</v>
+      </c>
+      <c r="J400" s="5">
+        <v>813.09613142023454</v>
+      </c>
+      <c r="K400" s="5">
+        <v>7399.1747959241338</v>
+      </c>
+      <c r="L400" s="5">
+        <v>0.73991747959241339</v>
+      </c>
+      <c r="M400" s="13">
+        <v>41.6801866666667</v>
+      </c>
+      <c r="N400" s="13">
+        <v>-82.649019999999993</v>
+      </c>
+    </row>
+    <row r="401" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A401">
+        <v>536</v>
+      </c>
+      <c r="B401" s="3">
+        <v>42999</v>
+      </c>
+      <c r="C401" s="4">
+        <v>21</v>
+      </c>
+      <c r="D401" s="4">
+        <v>9</v>
+      </c>
+      <c r="E401" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F401" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G401" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="H401" s="5">
+        <v>14.6</v>
+      </c>
+      <c r="I401" s="7">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="J401" s="5">
+        <v>820.29877192432241</v>
+      </c>
+      <c r="K401" s="5">
+        <v>7956.8980876659271</v>
+      </c>
+      <c r="L401" s="5">
+        <v>0.79568980876659268</v>
+      </c>
+      <c r="M401" s="13">
+        <v>41.6636016666667</v>
+      </c>
+      <c r="N401" s="13">
+        <v>-82.450441666666705</v>
+      </c>
+    </row>
+    <row r="402" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A402">
+        <v>540</v>
+      </c>
+      <c r="B402" s="3">
+        <v>42999</v>
+      </c>
+      <c r="C402" s="4">
+        <v>21</v>
+      </c>
+      <c r="D402" s="4">
+        <v>9</v>
+      </c>
+      <c r="E402" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F402" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G402" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="H402" s="5">
+        <v>14.3</v>
+      </c>
+      <c r="I402" s="7">
+        <v>9.6</v>
+      </c>
+      <c r="J402" s="5">
+        <v>768.2931060306064</v>
+      </c>
+      <c r="K402" s="5">
+        <v>7375.6138178938209</v>
+      </c>
+      <c r="L402" s="5">
+        <v>0.73756138178938213</v>
+      </c>
+      <c r="M402" s="13">
+        <v>41.663066666666701</v>
+      </c>
+      <c r="N402" s="13">
+        <v>-82.349751666666705</v>
+      </c>
+    </row>
+    <row r="403" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A403">
+        <v>535</v>
+      </c>
+      <c r="B403" s="3">
+        <v>42999</v>
+      </c>
+      <c r="C403" s="4">
+        <v>21</v>
+      </c>
+      <c r="D403" s="4">
+        <v>9</v>
+      </c>
+      <c r="E403" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F403" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G403" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="H403" s="5">
+        <v>14.7</v>
+      </c>
+      <c r="I403" s="7">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="J403" s="5">
+        <v>887.96988370126155</v>
+      </c>
+      <c r="K403" s="5">
+        <v>8613.307871902236</v>
+      </c>
+      <c r="L403" s="5">
+        <v>0.8613307871902236</v>
+      </c>
+      <c r="M403" s="13">
+        <v>41.583435000000001</v>
+      </c>
+      <c r="N403" s="13">
+        <v>-82.446430000000007</v>
+      </c>
+    </row>
+    <row r="404" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A404">
+        <v>539</v>
+      </c>
+      <c r="B404" s="3">
+        <v>42999</v>
+      </c>
+      <c r="C404" s="4">
+        <v>21</v>
+      </c>
+      <c r="D404" s="4">
+        <v>9</v>
+      </c>
+      <c r="E404" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F404" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G404" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="H404" s="5">
+        <v>14.3</v>
+      </c>
+      <c r="I404" s="7">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="J404" s="5">
+        <v>738.6901183029662</v>
+      </c>
+      <c r="K404" s="5">
+        <v>7165.2941475387715</v>
+      </c>
+      <c r="L404" s="5">
+        <v>0.7165294147538771</v>
+      </c>
+      <c r="M404" s="13">
+        <v>41.581046666666701</v>
+      </c>
+      <c r="N404" s="13">
+        <v>-82.349496666666695</v>
+      </c>
+    </row>
+    <row r="405" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A405">
+        <v>541</v>
+      </c>
+      <c r="B405" s="3">
+        <v>42999</v>
+      </c>
+      <c r="C405" s="4">
+        <v>21</v>
+      </c>
+      <c r="D405" s="4">
+        <v>9</v>
+      </c>
+      <c r="E405" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F405" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G405" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="H405" s="5">
+        <v>14</v>
+      </c>
+      <c r="I405" s="7">
+        <v>9.4</v>
+      </c>
+      <c r="J405" s="5">
+        <v>968.34476745100915</v>
+      </c>
+      <c r="K405" s="5">
+        <v>9102.4408140394862</v>
+      </c>
+      <c r="L405" s="5">
+        <v>0.91024408140394863</v>
+      </c>
+      <c r="M405" s="13">
+        <v>41.481446666666699</v>
+      </c>
+      <c r="N405" s="13">
+        <v>-82.265389999999996</v>
+      </c>
+    </row>
+    <row r="406" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A406">
+        <v>538</v>
+      </c>
+      <c r="B406" s="3">
+        <v>42999</v>
+      </c>
+      <c r="C406" s="4">
+        <v>21</v>
+      </c>
+      <c r="D406" s="4">
+        <v>9</v>
+      </c>
+      <c r="E406" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F406" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G406" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="H406" s="5">
+        <v>14.2</v>
+      </c>
+      <c r="I406" s="7">
+        <v>9.6</v>
+      </c>
+      <c r="J406" s="5">
+        <v>861.15159299713252</v>
+      </c>
+      <c r="K406" s="5">
+        <v>8267.0552927724711</v>
+      </c>
+      <c r="L406" s="5">
+        <v>0.82670552927724716</v>
+      </c>
+      <c r="M406" s="13">
+        <v>41.480781666666701</v>
+      </c>
+      <c r="N406" s="13">
+        <v>-82.350621666666697</v>
+      </c>
+    </row>
+    <row r="407" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A407">
+        <v>534</v>
+      </c>
+      <c r="B407" s="3">
+        <v>42999</v>
+      </c>
+      <c r="C407" s="4">
+        <v>21</v>
+      </c>
+      <c r="D407" s="4">
+        <v>9</v>
+      </c>
+      <c r="E407" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F407" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G407" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="H407" s="5">
+        <v>14</v>
+      </c>
+      <c r="I407" s="7">
+        <v>9.4</v>
+      </c>
+      <c r="J407" s="5">
+        <v>701.54189798932543</v>
+      </c>
+      <c r="K407" s="5">
+        <v>6594.4938410996592</v>
+      </c>
+      <c r="L407" s="5">
+        <v>0.6594493841099659</v>
+      </c>
+      <c r="M407" s="13">
+        <v>41.480085000000003</v>
+      </c>
+      <c r="N407" s="13">
+        <v>-82.450154999999995</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A85:E124">
     <sortCondition ref="A84"/>

</xml_diff>